<commit_message>
fix: fix 5.3 solutions
</commit_message>
<xml_diff>
--- a/5.3 - Funkciya SUMMPROIZV.xlsx
+++ b/5.3 - Funkciya SUMMPROIZV.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yakushev\Documents\1_Excel\Онлайн обучение на GetCourse\Материалы курсов\Массивы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Courses\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C634B7-49AA-4AA9-AEE9-EDFED65B5450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="769" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="БАЗА" sheetId="59" r:id="rId1"/>
@@ -89,7 +88,7 @@
     <definedName name="ы" localSheetId="1" hidden="1">[1]MASTER!#REF!</definedName>
     <definedName name="ы" hidden="1">[1]MASTER!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -239,7 +238,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="9">
     <numFmt numFmtId="164" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
@@ -2656,2180 +2655,2180 @@
     </xf>
   </cellXfs>
   <cellStyles count="2174">
-    <cellStyle name="_3ДМ" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="_3ДМ_БЕЛ" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="_3ДМ_РЕЧ" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="_PRICE" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="_Август" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="_Август_Дистанц." xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="_Август_Индив." xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="_АКАД" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="_АКАД_БЕЛ" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="_АКАД_РЕЧ" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="_Апрель" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="_Апрель_3ДМ" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="_Апрель_3ДМ_БЕЛ" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="_Апрель_3ДМ_РЕЧ" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="_Апрель_Август" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="_Апрель_Август_Дистанц." xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="_Апрель_Август_Индив." xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="_Апрель_АКАД" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="_Апрель_АКАД_БЕЛ" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="_Апрель_АКАД_РЕЧ" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="_Апрель_Б9560" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="_Апрель_Б9560_БЕЛ" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="_Апрель_Б9560_РЕЧ" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="_Апрель_БЕЛ" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="_Апрель_БИНТ" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="_Апрель_БИНТ_БЕЛ" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="_Апрель_БИНТ_РЕЧ" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="_Апрель_БУХ" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="_Апрель_БУХ_БЕЛ" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="_Апрель_БУХ_РЕЧ" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="_Апрель_ВЕБДИЗ" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="_Апрель_ВЕБДИЗ_БЕЛ" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="_Апрель_ВЕБДИЗ_РЕЧ" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="_Апрель_ВЕБМАСТ" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="_Апрель_ВЕБМАСТ_БЕЛ" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="_Апрель_ВЕБМАСТ_РЕЧ" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="_Апрель_ВУЕ" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="_Апрель_ВУЕ_БЕЛ" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="_Апрель_ВУЕ_РЕЧ" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="_Апрель_Дети" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="_Апрель_Дети_БЕЛ" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="_Апрель_Дети_РЕЧ" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="_Апрель_Дистанц." xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="_Апрель_Индив." xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="_Апрель_Индив._БЕЛ" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="_Апрель_Индив._РЕЧ" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="_Апрель_Июль" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="_Апрель_Июль_Август" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="_Апрель_Июль_Август_Дистанц." xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="_Апрель_Июль_Август_Индив." xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="_Апрель_Июль_БЕЛ" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="_Апрель_Июль_БИНТ" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="_Апрель_Июль_БИНТ_БЕЛ" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="_Апрель_Июль_БИНТ_РЕЧ" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="_Апрель_Июль_ВЕБДИЗ" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="_Апрель_Июль_ВЕБМАСТ" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="_Апрель_Июль_ВЕБМАСТ_БЕЛ" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="_Апрель_Июль_ВЕБМАСТ_РЕЧ" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="_Апрель_Июль_Дети" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="_Апрель_Июль_Дистанц." xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="_Апрель_Июль_Индив." xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="_Апрель_Июль_Индив._БЕЛ" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="_Апрель_Июль_Индив._РЕЧ" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь_Август" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь_Дистанц." xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь_Индив." xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь_КБУ" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="_Апрель_Июль_Июнь_Май" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="_Апрель_Июль_КБУ" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="_Апрель_Июль_КРН" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="_Апрель_Июль_Май" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="_Апрель_Июль_ОПШ" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="_Апрель_Июль_СР" xfId="74" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="_Апрель_Июнь" xfId="75" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="_Апрель_Июнь_1" xfId="76" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="_Апрель_Июнь_1_Август" xfId="77" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="_Апрель_Июнь_1_Дистанц." xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="_Апрель_Июнь_1_Индив." xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="_Апрель_Июнь_1_КБУ" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="_Апрель_Июнь_1_Май" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="_Апрель_Июнь_Август" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="_Апрель_Июнь_Август_Дистанц." xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="_Апрель_Июнь_Август_Индив." xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="_Апрель_Июнь_БЕЛ" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="_Апрель_Июнь_БИНТ" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="_Апрель_Июнь_БИНТ_БЕЛ" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="_Апрель_Июнь_БИНТ_РЕЧ" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="_Апрель_Июнь_БУХ" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="_Апрель_Июнь_БУХ_БЕЛ" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="_Апрель_Июнь_БУХ_РЕЧ" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="_Апрель_Июнь_ВЕБДИЗ" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ_БЕЛ" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ_РЕЧ" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="_Апрель_Июнь_Дети" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="_Апрель_Июнь_Дистанц." xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="_Апрель_Июнь_Индив." xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="_Апрель_Июнь_Индив._БЕЛ" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="_Апрель_Июнь_Индив._РЕЧ" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="_Апрель_Июнь_Июнь" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="_Апрель_Июнь_Июнь_Август" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="_Апрель_Июнь_Июнь_Дистанц." xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="_Апрель_Июнь_Июнь_Индив." xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="_Апрель_Июнь_Июнь_КБУ" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="_Апрель_Июнь_КБУ" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="_Апрель_Июнь_КРН" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="_Апрель_Июнь_Май" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="_Апрель_Июнь_ОПШ" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="_Апрель_Июнь_СР" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="_Апрель_КБУ" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="_Апрель_КБУ_БЕЛ" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="_Апрель_КБУ_РЕЧ" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="_Апрель_КРН" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="_Апрель_Май" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="_Апрель_Май_1" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="_Апрель_Май_1_Август" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="_Апрель_Май_1_Август_Дистанц." xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="_Апрель_Май_1_Август_Индив." xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="_Апрель_Май_1_БЕЛ" xfId="120" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="_Апрель_Май_1_БИНТ" xfId="121" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="_Апрель_Май_1_БИНТ_БЕЛ" xfId="122" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="_Апрель_Май_1_БИНТ_РЕЧ" xfId="123" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="_Апрель_Май_1_ВЕБДИЗ" xfId="124" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ" xfId="125" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ_БЕЛ" xfId="126" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ_РЕЧ" xfId="127" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="_Апрель_Май_1_Дети" xfId="128" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="_Апрель_Май_1_Дистанц." xfId="129" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="_Апрель_Май_1_Индив." xfId="130" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="_Апрель_Май_1_Индив._БЕЛ" xfId="131" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="_Апрель_Май_1_Индив._РЕЧ" xfId="132" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="_Апрель_Май_1_Июнь" xfId="133" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="_Апрель_Май_1_Июнь_Август" xfId="134" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="_Апрель_Май_1_Июнь_Дистанц." xfId="135" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="_Апрель_Май_1_Июнь_Индив." xfId="136" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="_Апрель_Май_1_Июнь_КБУ" xfId="137" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="_Апрель_Май_1_КБУ" xfId="138" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="_Апрель_Май_1_КРН" xfId="139" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="_Апрель_Май_1_ОПШ" xfId="140" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="_Апрель_Май_1_СР" xfId="141" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="_Апрель_Май_2" xfId="142" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="_Апрель_Май_Август" xfId="143" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="_Апрель_Май_Август_Дистанц." xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="_Апрель_Май_Август_Индив." xfId="145" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="_Апрель_Май_АКАД" xfId="146" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="_Апрель_Май_АКАД_БЕЛ" xfId="147" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="_Апрель_Май_АКАД_РЕЧ" xfId="148" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="_Апрель_Май_Б9560" xfId="149" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="_Апрель_Май_Б9560_БЕЛ" xfId="150" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="_Апрель_Май_Б9560_РЕЧ" xfId="151" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="_Апрель_Май_БЕЛ" xfId="152" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="_Апрель_Май_БИНТ" xfId="153" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="_Апрель_Май_БИНТ_БЕЛ" xfId="154" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="_Апрель_Май_БИНТ_РЕЧ" xfId="155" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="_Апрель_Май_БУХ" xfId="156" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="_Апрель_Май_БУХ_БЕЛ" xfId="157" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="_Апрель_Май_БУХ_РЕЧ" xfId="158" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="_Апрель_Май_ВЕБДИЗ" xfId="159" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="_Апрель_Май_ВЕБМАСТ" xfId="160" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="_Апрель_Май_ВЕБМАСТ_БЕЛ" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="_Апрель_Май_ВЕБМАСТ_РЕЧ" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="_Апрель_Май_Дети" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="_Апрель_Май_Дистанц." xfId="164" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="_Апрель_Май_Индив." xfId="165" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="_Апрель_Май_Индив._БЕЛ" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="_Апрель_Май_Индив._РЕЧ" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="_Апрель_Май_Июль" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Август" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Август_Дистанц." xfId="170" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Август_Индив." xfId="171" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_БЕЛ" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_БИНТ" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_БИНТ_БЕЛ" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_БИНТ_РЕЧ" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_ВЕБДИЗ" xfId="176" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Дети" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Дистанц." xfId="181" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Индив." xfId="182" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Индив._БЕЛ" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Индив._РЕЧ" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Июнь" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Июнь_Август" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Июнь_Дистанц." xfId="187" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Июнь_Индив." xfId="188" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_Июнь_КБУ" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_КБУ" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_КРН" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_ОПШ" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="_Апрель_Май_Июль_СР" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_1" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_1_Август" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_1_Дистанц." xfId="197" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_1_Индив." xfId="198" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_1_КБУ" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Август" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Август_Дистанц." xfId="201" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Август_Индив." xfId="202" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БЕЛ" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БИНТ" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БИНТ_БЕЛ" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БИНТ_РЕЧ" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БУХ" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БУХ_БЕЛ" xfId="208" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_БУХ_РЕЧ" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_ВЕБДИЗ" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Дети" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Дистанц." xfId="215" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Индив." xfId="216" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Индив._БЕЛ" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Индив._РЕЧ" xfId="218" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Июнь" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Июнь_Август" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Июнь_Дистанц." xfId="221" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Июнь_Индив." xfId="222" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_Июнь_КБУ" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_КБУ" xfId="224" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_КРН" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_ОПШ" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="_Апрель_Май_Июнь_СР" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="_Апрель_Май_КБУ" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="_Апрель_Май_КРН" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="_Апрель_Май_Май" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Август" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Август_Дистанц." xfId="232" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Август_Индив." xfId="233" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="_Апрель_Май_Май_БЕЛ" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="_Апрель_Май_Май_БИНТ" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="_Апрель_Май_Май_БИНТ_БЕЛ" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="_Апрель_Май_Май_БИНТ_РЕЧ" xfId="237" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="_Апрель_Май_Май_ВЕБДИЗ" xfId="238" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ_БЕЛ" xfId="240" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ_РЕЧ" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Дети" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Дистанц." xfId="243" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Индив." xfId="244" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Индив._БЕЛ" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Индив._РЕЧ" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Июнь" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Июнь_Август" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Июнь_Дистанц." xfId="249" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Июнь_Индив." xfId="250" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="_Апрель_Май_Май_Июнь_КБУ" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="_Апрель_Май_Май_КБУ" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="_Апрель_Май_Май_КРН" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="_Апрель_Май_Май_ОПШ" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="_Апрель_Май_Май_СР" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="_Апрель_Май_ОПШ" xfId="256" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="_Апрель_Май_РЕЧ" xfId="257" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="_Апрель_Май_РЕЧ_БЕЛ" xfId="258" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="_Апрель_Май_РЕЧ_РЕЧ" xfId="259" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="_Апрель_Май_СИ" xfId="260" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="_Апрель_Май_СИ_БЕЛ" xfId="261" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="_Апрель_Май_СИ_РЕЧ" xfId="262" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="_Апрель_Май_СР" xfId="263" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="_Апрель_Май_СУБД" xfId="264" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="_Апрель_Май_СУБД_БЕЛ" xfId="265" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="_Апрель_Май_СУБД_РЕЧ" xfId="266" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="_Апрель_НТ" xfId="267" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="_Апрель_НТ_БЕЛ" xfId="268" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="_Апрель_НТ_РЕЧ" xfId="269" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="_Апрель_ОПШ" xfId="270" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="_Апрель_Офис" xfId="271" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="_Апрель_Офис_БЕЛ" xfId="272" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="_Апрель_Офис_РЕЧ" xfId="273" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="_Апрель_РЕЧ" xfId="274" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="_Апрель_РЕЧ_БЕЛ" xfId="275" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="_Апрель_РЕЧ_РЕЧ" xfId="276" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="_Апрель_СИ" xfId="277" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="_Апрель_СИ_БЕЛ" xfId="278" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="_Апрель_СИ_РЕЧ" xfId="279" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="_Апрель_СИС" xfId="280" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="_Апрель_СИС_БЕЛ" xfId="281" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="_Апрель_СИС_РЕЧ" xfId="282" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="_Апрель_СР" xfId="283" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="_Апрель_СУБД" xfId="284" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="_Апрель_СУБД_БЕЛ" xfId="285" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="_Апрель_СУБД_РЕЧ" xfId="286" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="_Апрель_ТЕК" xfId="287" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="_Апрель_ТЕК_БЕЛ" xfId="288" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="_Апрель_ТЕК_РЕЧ" xfId="289" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="_Апрель_Февраль" xfId="290" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="_Апрель_Февраль_Август" xfId="291" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="_Апрель_Февраль_Август_Дистанц." xfId="292" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="_Апрель_Февраль_Август_Индив." xfId="293" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="_Апрель_Февраль_АКАД" xfId="294" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="_Апрель_Февраль_АКАД_БЕЛ" xfId="295" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="_Апрель_Февраль_АКАД_РЕЧ" xfId="296" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="_Апрель_Февраль_Б9560" xfId="297" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="_Апрель_Февраль_Б9560_БЕЛ" xfId="298" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="_Апрель_Февраль_Б9560_РЕЧ" xfId="299" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="_Апрель_Февраль_БЕЛ" xfId="300" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="_Апрель_Февраль_БИНТ" xfId="301" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="_Апрель_Февраль_БИНТ_БЕЛ" xfId="302" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="_Апрель_Февраль_БИНТ_РЕЧ" xfId="303" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="_Апрель_Февраль_БУХ" xfId="304" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="_Апрель_Февраль_БУХ_БЕЛ" xfId="305" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="_Апрель_Февраль_БУХ_РЕЧ" xfId="306" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="_Апрель_Февраль_ВЕБДИЗ" xfId="307" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ" xfId="308" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ_БЕЛ" xfId="309" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ_РЕЧ" xfId="310" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="_Апрель_Февраль_Дети" xfId="311" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="_Апрель_Февраль_Дистанц." xfId="312" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="_Апрель_Февраль_Индив." xfId="313" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="_Апрель_Февраль_Индив._БЕЛ" xfId="314" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="_Апрель_Февраль_Индив._РЕЧ" xfId="315" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль" xfId="316" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Август" xfId="317" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Август_Дистанц." xfId="318" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Август_Индив." xfId="319" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_БЕЛ" xfId="320" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_БИНТ" xfId="321" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_БИНТ_БЕЛ" xfId="322" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_БИНТ_РЕЧ" xfId="323" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_ВЕБДИЗ" xfId="324" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ" xfId="325" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="326" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="327" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Дети" xfId="328" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Дистанц." xfId="329" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Индив." xfId="330" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Индив._БЕЛ" xfId="331" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Индив._РЕЧ" xfId="332" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Июнь" xfId="333" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Август" xfId="334" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Дистанц." xfId="335" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Индив." xfId="336" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_Июнь_КБУ" xfId="337" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_КБУ" xfId="338" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_КРН" xfId="339" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_ОПШ" xfId="340" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июль_СР" xfId="341" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_1" xfId="343" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_1_Август" xfId="344" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_1_Дистанц." xfId="345" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_1_Индив." xfId="346" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_1_КБУ" xfId="347" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Август" xfId="348" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Август_Дистанц." xfId="349" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Август_Индив." xfId="350" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БЕЛ" xfId="351" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ" xfId="352" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ_БЕЛ" xfId="353" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ_РЕЧ" xfId="354" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БУХ" xfId="355" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БУХ_БЕЛ" xfId="356" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_БУХ_РЕЧ" xfId="357" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБДИЗ" xfId="358" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ" xfId="359" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="360" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="361" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Дети" xfId="362" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Дистанц." xfId="363" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Индив." xfId="364" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Индив._БЕЛ" xfId="365" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Индив._РЕЧ" xfId="366" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Июнь" xfId="367" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Август" xfId="368" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Дистанц." xfId="369" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Индив." xfId="370" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_КБУ" xfId="371" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_КБУ" xfId="372" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_КРН" xfId="373" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_ОПШ" xfId="374" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
-    <cellStyle name="_Апрель_Февраль_Июнь_СР" xfId="375" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="_Апрель_Февраль_КБУ" xfId="376" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="_Апрель_Февраль_КРН" xfId="377" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май" xfId="378" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Август" xfId="379" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Август_Дистанц." xfId="380" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Август_Индив." xfId="381" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_БЕЛ" xfId="382" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_БИНТ" xfId="383" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_БИНТ_БЕЛ" xfId="384" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_БИНТ_РЕЧ" xfId="385" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_ВЕБДИЗ" xfId="386" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ" xfId="387" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="388" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="389" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Дети" xfId="390" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Дистанц." xfId="391" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Индив." xfId="392" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Индив._БЕЛ" xfId="393" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Индив._РЕЧ" xfId="394" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Июнь" xfId="395" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Июнь_Август" xfId="396" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Июнь_Дистанц." xfId="397" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Июнь_Индив." xfId="398" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_Июнь_КБУ" xfId="399" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_КБУ" xfId="400" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_КРН" xfId="401" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_ОПШ" xfId="402" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="_Апрель_Февраль_Май_СР" xfId="403" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="_Апрель_Февраль_ОПШ" xfId="404" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="_Апрель_Февраль_РЕЧ" xfId="405" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="_Апрель_Февраль_РЕЧ_БЕЛ" xfId="406" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="_Апрель_Февраль_РЕЧ_РЕЧ" xfId="407" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="_Апрель_Февраль_СИ" xfId="408" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="_Апрель_Февраль_СИ_БЕЛ" xfId="409" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="_Апрель_Февраль_СИ_РЕЧ" xfId="410" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="_Апрель_Февраль_СР" xfId="411" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="_Апрель_Февраль_СУБД" xfId="412" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="_Апрель_Февраль_СУБД_БЕЛ" xfId="413" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="_Апрель_Февраль_СУБД_РЕЧ" xfId="414" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="_Апрель_ФШ" xfId="415" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="_Апрель_ФШ_БЕЛ" xfId="416" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="_Апрель_ФШ_РЕЧ" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
-    <cellStyle name="_Б9560" xfId="418" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
-    <cellStyle name="_Б9560_БЕЛ" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="_Б9560_РЕЧ" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="_БЕЛ" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="_БЕЛ_БЕЛ" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="_БЕЛ_РЕЧ" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="_БИНТ" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="_БИНТ_БЕЛ" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="_БИНТ_РЕЧ" xfId="426" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="_БУХ" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="_БУХ_БЕЛ" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="_БУХ_РЕЧ" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="_ВЕБДИЗ" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="_ВЕБДИЗ_БЕЛ" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="_ВЕБДИЗ_РЕЧ" xfId="432" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="_ВЕБМАСТ" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="_ВЕБМАСТ_БЕЛ" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="_ВЕБМАСТ_РЕЧ" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="_ВУЕ" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="_ВУЕ_БЕЛ" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="_ВУЕ_РЕЧ" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="_Дети" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="_Дети_БЕЛ" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="_Дети_РЕЧ" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="_Дистанц." xfId="442" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
-    <cellStyle name="_ДОГ НУДО частн" xfId="443" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
-    <cellStyle name="_ДОГ НУДО частн_БЕЛ" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="_ДОГ НУДО частн_РЕЧ" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="_Заявление" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="_Заявление_БЕЛ" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="_Заявление_РЕЧ" xfId="448" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="_Индив." xfId="449" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="_Индив._БЕЛ" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="_Индив._РЕЧ" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="_ИНТ" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="_ИНТ_БЕЛ" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="_ИНТ_РЕЧ" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="_Июль" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="_Июль_Август" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="_Июль_Август_Дистанц." xfId="457" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="_Июль_Август_Индив." xfId="458" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="_Июль_БЕЛ" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="_Июль_БИНТ" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="_Июль_БИНТ_БЕЛ" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="_Июль_БИНТ_РЕЧ" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
-    <cellStyle name="_Июль_ВЕБДИЗ" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
-    <cellStyle name="_Июль_ВЕБМАСТ" xfId="464" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="_Июль_ВЕБМАСТ_БЕЛ" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="_Июль_ВЕБМАСТ_РЕЧ" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="_Июль_Дети" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="_Июль_Дистанц." xfId="468" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="_Июль_Индив." xfId="469" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="_Июль_Индив._БЕЛ" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="_Июль_Индив._РЕЧ" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="_Июль_Июнь" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="_Июль_Июнь_Август" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="_Июль_Июнь_Дистанц." xfId="474" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="_Июль_Июнь_Индив." xfId="475" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="_Июль_Июнь_КБУ" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="_Июль_КБУ" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="_Июль_КРН" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="_Июль_ОПШ" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="_Июль_СР" xfId="480" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="_Июнь" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="_Июнь_1" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="_Июнь_1_Август" xfId="483" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
-    <cellStyle name="_Июнь_1_Дистанц." xfId="484" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
-    <cellStyle name="_Июнь_1_Индив." xfId="485" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="_Июнь_1_КБУ" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="_Июнь_Август" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="_Июнь_Август_Дистанц." xfId="488" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="_Июнь_Август_Индив." xfId="489" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="_Июнь_БЕЛ" xfId="490" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="_Июнь_БИНТ" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="_Июнь_БИНТ_БЕЛ" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="_Июнь_БИНТ_РЕЧ" xfId="493" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="_Июнь_БУХ" xfId="494" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="_Июнь_БУХ_БЕЛ" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="_Июнь_БУХ_РЕЧ" xfId="496" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="_Июнь_ВЕБДИЗ" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="_Июнь_ВЕБМАСТ" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="_Июнь_ВЕБМАСТ_БЕЛ" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="_Июнь_ВЕБМАСТ_РЕЧ" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="_Июнь_Дети" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="_Июнь_Дистанц." xfId="502" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="_Июнь_Индив." xfId="503" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
-    <cellStyle name="_Июнь_Индив._БЕЛ" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
-    <cellStyle name="_Июнь_Индив._РЕЧ" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="_Июнь_Июнь" xfId="506" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="_Июнь_Июнь_Август" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="_Июнь_Июнь_Дистанц." xfId="508" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="_Июнь_Июнь_Индив." xfId="509" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="_Июнь_Июнь_КБУ" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="_Июнь_КБУ" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="_Июнь_КРН" xfId="512" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="_Июнь_ОПШ" xfId="513" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="_Июнь_СР" xfId="514" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="_КБУ" xfId="515" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="_КБУ_БЕЛ" xfId="516" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="_КБУ_РЕЧ" xfId="517" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="_Консультация" xfId="518" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="_Консультация_БЕЛ" xfId="519" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="_Консультация_РЕЧ" xfId="520" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="_КРН" xfId="521" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="_КРН_БЕЛ" xfId="522" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="_КРН_РЕЧ" xfId="523" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
-    <cellStyle name="_Лист1" xfId="524" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
-    <cellStyle name="_ЛСХ" xfId="525" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="_ЛСХ_БЕЛ" xfId="526" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="_ЛСХ_РЕЧ" xfId="527" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="_Май" xfId="528" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="_Май_1" xfId="529" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="_Май_1_Август" xfId="530" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="_Май_1_Август_Дистанц." xfId="531" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="_Май_1_Август_Индив." xfId="532" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="_Май_1_БЕЛ" xfId="533" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="_Май_1_БИНТ" xfId="534" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="_Май_1_БИНТ_БЕЛ" xfId="535" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="_Май_1_БИНТ_РЕЧ" xfId="536" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="_Май_1_ВЕБДИЗ" xfId="537" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="_Май_1_ВЕБМАСТ" xfId="538" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="_Май_1_ВЕБМАСТ_БЕЛ" xfId="539" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="_Май_1_ВЕБМАСТ_РЕЧ" xfId="540" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="_Май_1_Дети" xfId="541" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="_Май_1_Дистанц." xfId="542" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="_Май_1_Индив." xfId="543" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
-    <cellStyle name="_Май_1_Индив._БЕЛ" xfId="544" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
-    <cellStyle name="_Май_1_Индив._РЕЧ" xfId="545" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="_Май_1_Июнь" xfId="546" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="_Май_1_Июнь_Август" xfId="547" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="_Май_1_Июнь_Дистанц." xfId="548" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="_Май_1_Июнь_Индив." xfId="549" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="_Май_1_Июнь_КБУ" xfId="550" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="_Май_1_КБУ" xfId="551" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="_Май_1_КРН" xfId="552" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="_Май_1_ОПШ" xfId="553" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="_Май_1_СР" xfId="554" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="_Май_Август" xfId="555" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="_Май_Август_Дистанц." xfId="556" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="_Май_Август_Индив." xfId="557" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="_Май_АКАД" xfId="558" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="_Май_АКАД_БЕЛ" xfId="559" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="_Май_АКАД_РЕЧ" xfId="560" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="_Май_Б9560" xfId="561" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="_Май_Б9560_БЕЛ" xfId="562" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="_Май_Б9560_РЕЧ" xfId="563" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
-    <cellStyle name="_Май_БЕЛ" xfId="564" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
-    <cellStyle name="_Май_БИНТ" xfId="565" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="_Май_БИНТ_БЕЛ" xfId="566" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="_Май_БИНТ_РЕЧ" xfId="567" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="_Май_БУХ" xfId="568" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="_Май_БУХ_БЕЛ" xfId="569" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="_Май_БУХ_РЕЧ" xfId="570" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="_Май_ВЕБДИЗ" xfId="571" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="_Май_ВЕБМАСТ" xfId="572" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="_Май_ВЕБМАСТ_БЕЛ" xfId="573" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="_Май_ВЕБМАСТ_РЕЧ" xfId="574" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="_Май_Дети" xfId="575" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="_Май_Дистанц." xfId="576" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="_Май_Индив." xfId="577" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="_Май_Индив._БЕЛ" xfId="578" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="_Май_Индив._РЕЧ" xfId="579" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="_Май_Июль" xfId="580" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="_Май_Июль_Август" xfId="581" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="_Май_Июль_Август_Дистанц." xfId="582" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="_Май_Июль_Август_Индив." xfId="583" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
-    <cellStyle name="_Май_Июль_БЕЛ" xfId="584" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
-    <cellStyle name="_Май_Июль_БИНТ" xfId="585" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="_Май_Июль_БИНТ_БЕЛ" xfId="586" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="_Май_Июль_БИНТ_РЕЧ" xfId="587" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="_Май_Июль_ВЕБДИЗ" xfId="588" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="_Май_Июль_ВЕБМАСТ" xfId="589" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="590" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="591" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="_Май_Июль_Дети" xfId="592" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="_Май_Июль_Дистанц." xfId="593" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="_Май_Июль_Индив." xfId="594" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="_Май_Июль_Индив._БЕЛ" xfId="595" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="_Май_Июль_Индив._РЕЧ" xfId="596" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="_Май_Июль_Июнь" xfId="597" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="_Май_Июль_Июнь_Август" xfId="598" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="_Май_Июль_Июнь_Дистанц." xfId="599" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="_Май_Июль_Июнь_Индив." xfId="600" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="_Май_Июль_Июнь_КБУ" xfId="601" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="_Май_Июль_КБУ" xfId="602" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="_Май_Июль_КРН" xfId="603" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
-    <cellStyle name="_Май_Июль_ОПШ" xfId="604" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
-    <cellStyle name="_Май_Июль_СР" xfId="605" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="_Май_Июнь" xfId="606" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="_Май_Июнь_1" xfId="607" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="_Май_Июнь_1_Август" xfId="608" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="_Май_Июнь_1_Дистанц." xfId="609" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="_Май_Июнь_1_Индив." xfId="610" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="_Май_Июнь_1_КБУ" xfId="611" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="_Май_Июнь_Август" xfId="612" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="_Май_Июнь_Август_Дистанц." xfId="613" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="_Май_Июнь_Август_Индив." xfId="614" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="_Май_Июнь_БЕЛ" xfId="615" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="_Май_Июнь_БИНТ" xfId="616" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="_Май_Июнь_БИНТ_БЕЛ" xfId="617" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="_Май_Июнь_БИНТ_РЕЧ" xfId="618" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="_Май_Июнь_БУХ" xfId="619" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="_Май_Июнь_БУХ_БЕЛ" xfId="620" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="_Май_Июнь_БУХ_РЕЧ" xfId="621" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="_Май_Июнь_ВЕБДИЗ" xfId="622" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="_Май_Июнь_ВЕБМАСТ" xfId="623" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="624" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="625" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="_Май_Июнь_Дети" xfId="626" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="_Май_Июнь_Дистанц." xfId="627" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="_Май_Июнь_Индив." xfId="628" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="_Май_Июнь_Индив._БЕЛ" xfId="629" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="_Май_Июнь_Индив._РЕЧ" xfId="630" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="_Май_Июнь_Июнь" xfId="631" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="_Май_Июнь_Июнь_Август" xfId="632" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="_Май_Июнь_Июнь_Дистанц." xfId="633" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="_Май_Июнь_Июнь_Индив." xfId="634" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="_Май_Июнь_Июнь_КБУ" xfId="635" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="_Май_Июнь_КБУ" xfId="636" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="_Май_Июнь_КРН" xfId="637" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="_Май_Июнь_ОПШ" xfId="638" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="_Май_Июнь_СР" xfId="639" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="_Май_КБУ" xfId="640" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="_Май_КРН" xfId="641" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="_Май_Май" xfId="642" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="_Май_Май_Август" xfId="643" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="_Май_Май_Август_Дистанц." xfId="644" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="_Май_Май_Август_Индив." xfId="645" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="_Май_Май_БЕЛ" xfId="646" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="_Май_Май_БИНТ" xfId="647" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="_Май_Май_БИНТ_БЕЛ" xfId="648" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="_Май_Май_БИНТ_РЕЧ" xfId="649" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="_Май_Май_ВЕБДИЗ" xfId="650" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="_Май_Май_ВЕБМАСТ" xfId="651" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="_Май_Май_ВЕБМАСТ_БЕЛ" xfId="652" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="_Май_Май_ВЕБМАСТ_РЕЧ" xfId="653" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="_Май_Май_Дети" xfId="654" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="_Май_Май_Дистанц." xfId="655" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="_Май_Май_Индив." xfId="656" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="_Май_Май_Индив._БЕЛ" xfId="657" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="_Май_Май_Индив._РЕЧ" xfId="658" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="_Май_Май_Июнь" xfId="659" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="_Май_Май_Июнь_Август" xfId="660" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="_Май_Май_Июнь_Дистанц." xfId="661" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="_Май_Май_Июнь_Индив." xfId="662" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="_Май_Май_Июнь_КБУ" xfId="663" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
-    <cellStyle name="_Май_Май_КБУ" xfId="664" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
-    <cellStyle name="_Май_Май_КРН" xfId="665" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
-    <cellStyle name="_Май_Май_ОПШ" xfId="666" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
-    <cellStyle name="_Май_Май_СР" xfId="667" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
-    <cellStyle name="_Май_ОПШ" xfId="668" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
-    <cellStyle name="_Май_РЕЧ" xfId="669" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
-    <cellStyle name="_Май_РЕЧ_БЕЛ" xfId="670" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
-    <cellStyle name="_Май_РЕЧ_РЕЧ" xfId="671" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
-    <cellStyle name="_Май_СИ" xfId="672" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
-    <cellStyle name="_Май_СИ_БЕЛ" xfId="673" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
-    <cellStyle name="_Май_СИ_РЕЧ" xfId="674" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
-    <cellStyle name="_Май_СР" xfId="675" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
-    <cellStyle name="_Май_СУБД" xfId="676" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
-    <cellStyle name="_Май_СУБД_БЕЛ" xfId="677" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
-    <cellStyle name="_Май_СУБД_РЕЧ" xfId="678" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
-    <cellStyle name="_МП" xfId="679" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
-    <cellStyle name="_МП_БЕЛ" xfId="680" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
-    <cellStyle name="_МП_РЕЧ" xfId="681" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
-    <cellStyle name="_НТ" xfId="682" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
-    <cellStyle name="_НТ_БЕЛ" xfId="683" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
-    <cellStyle name="_НТ_РЕЧ" xfId="684" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
-    <cellStyle name="_ОПШ" xfId="685" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
-    <cellStyle name="_ОПШ_Апрель" xfId="686" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
-    <cellStyle name="_ОПШ_Апрель_БЕЛ" xfId="687" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
-    <cellStyle name="_ОПШ_Апрель_РЕЧ" xfId="688" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
-    <cellStyle name="_ОПШ_БЕЛ" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
-    <cellStyle name="_ОПШ_Июль" xfId="690" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
-    <cellStyle name="_ОПШ_Июль_БЕЛ" xfId="691" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
-    <cellStyle name="_ОПШ_Июль_РЕЧ" xfId="692" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
-    <cellStyle name="_ОПШ_Июнь" xfId="693" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
-    <cellStyle name="_ОПШ_Июнь_БЕЛ" xfId="694" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
-    <cellStyle name="_ОПШ_Июнь_РЕЧ" xfId="695" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
-    <cellStyle name="_ОПШ_Май" xfId="696" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
-    <cellStyle name="_ОПШ_Май_БЕЛ" xfId="697" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
-    <cellStyle name="_ОПШ_Май_РЕЧ" xfId="698" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
-    <cellStyle name="_ОПШ_РЕЧ" xfId="699" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
-    <cellStyle name="_ОПШ_Февраль" xfId="700" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
-    <cellStyle name="_ОПШ_Февраль_БЕЛ" xfId="701" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
-    <cellStyle name="_ОПШ_Февраль_РЕЧ" xfId="702" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
-    <cellStyle name="_ОПШ_Январь" xfId="703" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
-    <cellStyle name="_ОПШ_Январь_БЕЛ" xfId="704" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
-    <cellStyle name="_ОПШ_Январь_РЕЧ" xfId="705" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
-    <cellStyle name="_Офис" xfId="706" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
-    <cellStyle name="_Офис_БЕЛ" xfId="707" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
-    <cellStyle name="_Офис_РЕЧ" xfId="708" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
-    <cellStyle name="_ПРШ" xfId="709" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
-    <cellStyle name="_ПРШ_Апрель" xfId="710" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
-    <cellStyle name="_ПРШ_Апрель_БЕЛ" xfId="711" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
-    <cellStyle name="_ПРШ_Апрель_РЕЧ" xfId="712" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
-    <cellStyle name="_ПРШ_БЕЛ" xfId="713" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
-    <cellStyle name="_ПРШ_Июль" xfId="714" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
-    <cellStyle name="_ПРШ_Июль_БЕЛ" xfId="715" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
-    <cellStyle name="_ПРШ_Июль_РЕЧ" xfId="716" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
-    <cellStyle name="_ПРШ_Июнь" xfId="717" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
-    <cellStyle name="_ПРШ_Июнь_БЕЛ" xfId="718" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
-    <cellStyle name="_ПРШ_Июнь_РЕЧ" xfId="719" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
-    <cellStyle name="_ПРШ_Май" xfId="720" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
-    <cellStyle name="_ПРШ_Май_БЕЛ" xfId="721" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
-    <cellStyle name="_ПРШ_Май_РЕЧ" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
-    <cellStyle name="_ПРШ_РЕЧ" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
-    <cellStyle name="_ПРШ_Февраль" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
-    <cellStyle name="_ПРШ_Февраль_БЕЛ" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="_ПРШ_Февраль_РЕЧ" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
-    <cellStyle name="_ПРШ_Январь" xfId="727" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
-    <cellStyle name="_ПРШ_Январь_БЕЛ" xfId="728" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
-    <cellStyle name="_ПРШ_Январь_РЕЧ" xfId="729" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
-    <cellStyle name="_РЕЧ" xfId="730" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
-    <cellStyle name="_РЕЧ_БЕЛ" xfId="731" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
-    <cellStyle name="_РЕЧ_РЕЧ" xfId="732" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
-    <cellStyle name="_СВБ" xfId="733" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
-    <cellStyle name="_СВБ_БЕЛ" xfId="734" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
-    <cellStyle name="_СВБ_РЕЧ" xfId="735" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
-    <cellStyle name="_СИ" xfId="736" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
-    <cellStyle name="_СИ_БЕЛ" xfId="737" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
-    <cellStyle name="_СИ_РЕЧ" xfId="738" xr:uid="{00000000-0005-0000-0000-0000E1020000}"/>
-    <cellStyle name="_СИС" xfId="739" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
-    <cellStyle name="_СИС_БЕЛ" xfId="740" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
-    <cellStyle name="_СИС_РЕЧ" xfId="741" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
-    <cellStyle name="_СР" xfId="742" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
-    <cellStyle name="_СУБД" xfId="743" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
-    <cellStyle name="_СУБД_БЕЛ" xfId="744" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
-    <cellStyle name="_СУБД_РЕЧ" xfId="745" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
-    <cellStyle name="_СЧ СПЕЦ" xfId="746" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
-    <cellStyle name="_СЧ ЦКО" xfId="747" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
-    <cellStyle name="_СЧ ЦКО_Лист1" xfId="748" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
-    <cellStyle name="_СЧ ЦКО_Лист1_БЕЛ" xfId="749" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
-    <cellStyle name="_СЧ ЦКО_Лист1_РЕЧ" xfId="750" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
-    <cellStyle name="_СЧ ЦКО_СЧ СПЕЦ" xfId="751" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
-    <cellStyle name="_СЧ ЦКО_СЧДОГ СПЕЦ" xfId="752" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
-    <cellStyle name="_СЧДОГ" xfId="753" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
-    <cellStyle name="_СЧДОГ СПЕЦ" xfId="754" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
-    <cellStyle name="_СЧДОГ_1" xfId="755" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
-    <cellStyle name="_СЧДОГ_3ДМ" xfId="756" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
-    <cellStyle name="_СЧДОГ_3ДМ_БЕЛ" xfId="757" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
-    <cellStyle name="_СЧДОГ_3ДМ_РЕЧ" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F5020000}"/>
-    <cellStyle name="_СЧДОГ_Август" xfId="759" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
-    <cellStyle name="_СЧДОГ_Август_Дистанц." xfId="760" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
-    <cellStyle name="_СЧДОГ_Август_Индив." xfId="761" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
-    <cellStyle name="_СЧДОГ_АКАД" xfId="762" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
-    <cellStyle name="_СЧДОГ_АКАД_БЕЛ" xfId="763" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
-    <cellStyle name="_СЧДОГ_АКАД_РЕЧ" xfId="764" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
-    <cellStyle name="_СЧДОГ_Б9560" xfId="765" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
-    <cellStyle name="_СЧДОГ_Б9560_БЕЛ" xfId="766" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
-    <cellStyle name="_СЧДОГ_Б9560_РЕЧ" xfId="767" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
-    <cellStyle name="_СЧДОГ_БЕЛ" xfId="768" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
-    <cellStyle name="_СЧДОГ_БИНТ" xfId="769" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
-    <cellStyle name="_СЧДОГ_БИНТ_БЕЛ" xfId="770" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
-    <cellStyle name="_СЧДОГ_БИНТ_РЕЧ" xfId="771" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
-    <cellStyle name="_СЧДОГ_БУХ" xfId="772" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
-    <cellStyle name="_СЧДОГ_БУХ_БЕЛ" xfId="773" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
-    <cellStyle name="_СЧДОГ_БУХ_РЕЧ" xfId="774" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБДИЗ" xfId="775" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБДИЗ_БЕЛ" xfId="776" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБДИЗ_РЕЧ" xfId="777" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБМАСТ" xfId="778" xr:uid="{00000000-0005-0000-0000-000009030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБМАСТ_БЕЛ" xfId="779" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
-    <cellStyle name="_СЧДОГ_ВЕБМАСТ_РЕЧ" xfId="780" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
-    <cellStyle name="_СЧДОГ_ВУЕ" xfId="781" xr:uid="{00000000-0005-0000-0000-00000C030000}"/>
-    <cellStyle name="_СЧДОГ_ВУЕ_БЕЛ" xfId="782" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
-    <cellStyle name="_СЧДОГ_ВУЕ_РЕЧ" xfId="783" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
-    <cellStyle name="_СЧДОГ_Дети" xfId="784" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
-    <cellStyle name="_СЧДОГ_Дети_БЕЛ" xfId="785" xr:uid="{00000000-0005-0000-0000-000010030000}"/>
-    <cellStyle name="_СЧДОГ_Дети_РЕЧ" xfId="786" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
-    <cellStyle name="_СЧДОГ_Дистанц." xfId="787" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
-    <cellStyle name="_СЧДОГ_Индив." xfId="788" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
-    <cellStyle name="_СЧДОГ_Индив._БЕЛ" xfId="789" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
-    <cellStyle name="_СЧДОГ_Индив._РЕЧ" xfId="790" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
-    <cellStyle name="_СЧДОГ_Июль" xfId="791" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Август" xfId="792" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Август_Дистанц." xfId="793" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Август_Индив." xfId="794" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_БЕЛ" xfId="795" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_БИНТ" xfId="796" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_БИНТ_БЕЛ" xfId="797" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_БИНТ_РЕЧ" xfId="798" xr:uid="{00000000-0005-0000-0000-00001D030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_ВЕБДИЗ" xfId="799" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ" xfId="800" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ_БЕЛ" xfId="801" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ_РЕЧ" xfId="802" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Дети" xfId="803" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Дистанц." xfId="804" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Индив." xfId="805" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Индив._БЕЛ" xfId="806" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Индив._РЕЧ" xfId="807" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Июнь" xfId="808" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Июнь_Август" xfId="809" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Июнь_Дистанц." xfId="810" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Июнь_Индив." xfId="811" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_Июнь_КБУ" xfId="812" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_КБУ" xfId="813" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_КРН" xfId="814" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_ОПШ" xfId="815" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
-    <cellStyle name="_СЧДОГ_Июль_СР" xfId="816" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь" xfId="817" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_1" xfId="818" xr:uid="{00000000-0005-0000-0000-000031030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_1_Август" xfId="819" xr:uid="{00000000-0005-0000-0000-000032030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_1_Дистанц." xfId="820" xr:uid="{00000000-0005-0000-0000-000033030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_1_Индив." xfId="821" xr:uid="{00000000-0005-0000-0000-000034030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_1_КБУ" xfId="822" xr:uid="{00000000-0005-0000-0000-000035030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Август" xfId="823" xr:uid="{00000000-0005-0000-0000-000036030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Август_Дистанц." xfId="824" xr:uid="{00000000-0005-0000-0000-000037030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Август_Индив." xfId="825" xr:uid="{00000000-0005-0000-0000-000038030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БЕЛ" xfId="826" xr:uid="{00000000-0005-0000-0000-000039030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БИНТ" xfId="827" xr:uid="{00000000-0005-0000-0000-00003A030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БИНТ_БЕЛ" xfId="828" xr:uid="{00000000-0005-0000-0000-00003B030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БИНТ_РЕЧ" xfId="829" xr:uid="{00000000-0005-0000-0000-00003C030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БУХ" xfId="830" xr:uid="{00000000-0005-0000-0000-00003D030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БУХ_БЕЛ" xfId="831" xr:uid="{00000000-0005-0000-0000-00003E030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_БУХ_РЕЧ" xfId="832" xr:uid="{00000000-0005-0000-0000-00003F030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_ВЕБДИЗ" xfId="833" xr:uid="{00000000-0005-0000-0000-000040030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ" xfId="834" xr:uid="{00000000-0005-0000-0000-000041030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ_БЕЛ" xfId="835" xr:uid="{00000000-0005-0000-0000-000042030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ_РЕЧ" xfId="836" xr:uid="{00000000-0005-0000-0000-000043030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Дети" xfId="837" xr:uid="{00000000-0005-0000-0000-000044030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Дистанц." xfId="838" xr:uid="{00000000-0005-0000-0000-000045030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Индив." xfId="839" xr:uid="{00000000-0005-0000-0000-000046030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Индив._БЕЛ" xfId="840" xr:uid="{00000000-0005-0000-0000-000047030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Индив._РЕЧ" xfId="841" xr:uid="{00000000-0005-0000-0000-000048030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Июнь" xfId="842" xr:uid="{00000000-0005-0000-0000-000049030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Июнь_Август" xfId="843" xr:uid="{00000000-0005-0000-0000-00004A030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Июнь_Дистанц." xfId="844" xr:uid="{00000000-0005-0000-0000-00004B030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Июнь_Индив." xfId="845" xr:uid="{00000000-0005-0000-0000-00004C030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_Июнь_КБУ" xfId="846" xr:uid="{00000000-0005-0000-0000-00004D030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_КБУ" xfId="847" xr:uid="{00000000-0005-0000-0000-00004E030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_КРН" xfId="848" xr:uid="{00000000-0005-0000-0000-00004F030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_ОПШ" xfId="849" xr:uid="{00000000-0005-0000-0000-000050030000}"/>
-    <cellStyle name="_СЧДОГ_Июнь_СР" xfId="850" xr:uid="{00000000-0005-0000-0000-000051030000}"/>
-    <cellStyle name="_СЧДОГ_КБУ" xfId="851" xr:uid="{00000000-0005-0000-0000-000052030000}"/>
-    <cellStyle name="_СЧДОГ_КБУ_БЕЛ" xfId="852" xr:uid="{00000000-0005-0000-0000-000053030000}"/>
-    <cellStyle name="_СЧДОГ_КБУ_РЕЧ" xfId="853" xr:uid="{00000000-0005-0000-0000-000054030000}"/>
-    <cellStyle name="_СЧДОГ_КРН" xfId="854" xr:uid="{00000000-0005-0000-0000-000055030000}"/>
-    <cellStyle name="_СЧДОГ_Май" xfId="855" xr:uid="{00000000-0005-0000-0000-000056030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1" xfId="856" xr:uid="{00000000-0005-0000-0000-000057030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Август" xfId="857" xr:uid="{00000000-0005-0000-0000-000058030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Август_Дистанц." xfId="858" xr:uid="{00000000-0005-0000-0000-000059030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Август_Индив." xfId="859" xr:uid="{00000000-0005-0000-0000-00005A030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_БЕЛ" xfId="860" xr:uid="{00000000-0005-0000-0000-00005B030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_БИНТ" xfId="861" xr:uid="{00000000-0005-0000-0000-00005C030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_БИНТ_БЕЛ" xfId="862" xr:uid="{00000000-0005-0000-0000-00005D030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_БИНТ_РЕЧ" xfId="863" xr:uid="{00000000-0005-0000-0000-00005E030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_ВЕБДИЗ" xfId="864" xr:uid="{00000000-0005-0000-0000-00005F030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ" xfId="865" xr:uid="{00000000-0005-0000-0000-000060030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ_БЕЛ" xfId="866" xr:uid="{00000000-0005-0000-0000-000061030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ_РЕЧ" xfId="867" xr:uid="{00000000-0005-0000-0000-000062030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Дети" xfId="868" xr:uid="{00000000-0005-0000-0000-000063030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Дистанц." xfId="869" xr:uid="{00000000-0005-0000-0000-000064030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Индив." xfId="870" xr:uid="{00000000-0005-0000-0000-000065030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Индив._БЕЛ" xfId="871" xr:uid="{00000000-0005-0000-0000-000066030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Индив._РЕЧ" xfId="872" xr:uid="{00000000-0005-0000-0000-000067030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Июнь" xfId="873" xr:uid="{00000000-0005-0000-0000-000068030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Июнь_Август" xfId="874" xr:uid="{00000000-0005-0000-0000-000069030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Июнь_Дистанц." xfId="875" xr:uid="{00000000-0005-0000-0000-00006A030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Июнь_Индив." xfId="876" xr:uid="{00000000-0005-0000-0000-00006B030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_Июнь_КБУ" xfId="877" xr:uid="{00000000-0005-0000-0000-00006C030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_КБУ" xfId="878" xr:uid="{00000000-0005-0000-0000-00006D030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_КРН" xfId="879" xr:uid="{00000000-0005-0000-0000-00006E030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_ОПШ" xfId="880" xr:uid="{00000000-0005-0000-0000-00006F030000}"/>
-    <cellStyle name="_СЧДОГ_Май_1_СР" xfId="881" xr:uid="{00000000-0005-0000-0000-000070030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Август" xfId="882" xr:uid="{00000000-0005-0000-0000-000071030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Август_Дистанц." xfId="883" xr:uid="{00000000-0005-0000-0000-000072030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Август_Индив." xfId="884" xr:uid="{00000000-0005-0000-0000-000073030000}"/>
-    <cellStyle name="_СЧДОГ_Май_АКАД" xfId="885" xr:uid="{00000000-0005-0000-0000-000074030000}"/>
-    <cellStyle name="_СЧДОГ_Май_АКАД_БЕЛ" xfId="886" xr:uid="{00000000-0005-0000-0000-000075030000}"/>
-    <cellStyle name="_СЧДОГ_Май_АКАД_РЕЧ" xfId="887" xr:uid="{00000000-0005-0000-0000-000076030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Б9560" xfId="888" xr:uid="{00000000-0005-0000-0000-000077030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Б9560_БЕЛ" xfId="889" xr:uid="{00000000-0005-0000-0000-000078030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Б9560_РЕЧ" xfId="890" xr:uid="{00000000-0005-0000-0000-000079030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БЕЛ" xfId="891" xr:uid="{00000000-0005-0000-0000-00007A030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БИНТ" xfId="892" xr:uid="{00000000-0005-0000-0000-00007B030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БИНТ_БЕЛ" xfId="893" xr:uid="{00000000-0005-0000-0000-00007C030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БИНТ_РЕЧ" xfId="894" xr:uid="{00000000-0005-0000-0000-00007D030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БУХ" xfId="895" xr:uid="{00000000-0005-0000-0000-00007E030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БУХ_БЕЛ" xfId="896" xr:uid="{00000000-0005-0000-0000-00007F030000}"/>
-    <cellStyle name="_СЧДОГ_Май_БУХ_РЕЧ" xfId="897" xr:uid="{00000000-0005-0000-0000-000080030000}"/>
-    <cellStyle name="_СЧДОГ_Май_ВЕБДИЗ" xfId="898" xr:uid="{00000000-0005-0000-0000-000081030000}"/>
-    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ" xfId="899" xr:uid="{00000000-0005-0000-0000-000082030000}"/>
-    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ_БЕЛ" xfId="900" xr:uid="{00000000-0005-0000-0000-000083030000}"/>
-    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ_РЕЧ" xfId="901" xr:uid="{00000000-0005-0000-0000-000084030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Дети" xfId="902" xr:uid="{00000000-0005-0000-0000-000085030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Дистанц." xfId="903" xr:uid="{00000000-0005-0000-0000-000086030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Индив." xfId="904" xr:uid="{00000000-0005-0000-0000-000087030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Индив._БЕЛ" xfId="905" xr:uid="{00000000-0005-0000-0000-000088030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Индив._РЕЧ" xfId="906" xr:uid="{00000000-0005-0000-0000-000089030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль" xfId="907" xr:uid="{00000000-0005-0000-0000-00008A030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Август" xfId="908" xr:uid="{00000000-0005-0000-0000-00008B030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Август_Дистанц." xfId="909" xr:uid="{00000000-0005-0000-0000-00008C030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Август_Индив." xfId="910" xr:uid="{00000000-0005-0000-0000-00008D030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_БЕЛ" xfId="911" xr:uid="{00000000-0005-0000-0000-00008E030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ" xfId="912" xr:uid="{00000000-0005-0000-0000-00008F030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ_БЕЛ" xfId="913" xr:uid="{00000000-0005-0000-0000-000090030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ_РЕЧ" xfId="914" xr:uid="{00000000-0005-0000-0000-000091030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБДИЗ" xfId="915" xr:uid="{00000000-0005-0000-0000-000092030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ" xfId="916" xr:uid="{00000000-0005-0000-0000-000093030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="917" xr:uid="{00000000-0005-0000-0000-000094030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="918" xr:uid="{00000000-0005-0000-0000-000095030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Дети" xfId="919" xr:uid="{00000000-0005-0000-0000-000096030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Дистанц." xfId="920" xr:uid="{00000000-0005-0000-0000-000097030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Индив." xfId="921" xr:uid="{00000000-0005-0000-0000-000098030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Индив._БЕЛ" xfId="922" xr:uid="{00000000-0005-0000-0000-000099030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Индив._РЕЧ" xfId="923" xr:uid="{00000000-0005-0000-0000-00009A030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Июнь" xfId="924" xr:uid="{00000000-0005-0000-0000-00009B030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Август" xfId="925" xr:uid="{00000000-0005-0000-0000-00009C030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Дистанц." xfId="926" xr:uid="{00000000-0005-0000-0000-00009D030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Индив." xfId="927" xr:uid="{00000000-0005-0000-0000-00009E030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_КБУ" xfId="928" xr:uid="{00000000-0005-0000-0000-00009F030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_КБУ" xfId="929" xr:uid="{00000000-0005-0000-0000-0000A0030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_КРН" xfId="930" xr:uid="{00000000-0005-0000-0000-0000A1030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_ОПШ" xfId="931" xr:uid="{00000000-0005-0000-0000-0000A2030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июль_СР" xfId="932" xr:uid="{00000000-0005-0000-0000-0000A3030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь" xfId="933" xr:uid="{00000000-0005-0000-0000-0000A4030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_1" xfId="934" xr:uid="{00000000-0005-0000-0000-0000A5030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_1_Август" xfId="935" xr:uid="{00000000-0005-0000-0000-0000A6030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_1_Дистанц." xfId="936" xr:uid="{00000000-0005-0000-0000-0000A7030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_1_Индив." xfId="937" xr:uid="{00000000-0005-0000-0000-0000A8030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_1_КБУ" xfId="938" xr:uid="{00000000-0005-0000-0000-0000A9030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Август" xfId="939" xr:uid="{00000000-0005-0000-0000-0000AA030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Август_Дистанц." xfId="940" xr:uid="{00000000-0005-0000-0000-0000AB030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Август_Индив." xfId="941" xr:uid="{00000000-0005-0000-0000-0000AC030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БЕЛ" xfId="942" xr:uid="{00000000-0005-0000-0000-0000AD030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ" xfId="943" xr:uid="{00000000-0005-0000-0000-0000AE030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ_БЕЛ" xfId="944" xr:uid="{00000000-0005-0000-0000-0000AF030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ_РЕЧ" xfId="945" xr:uid="{00000000-0005-0000-0000-0000B0030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ" xfId="946" xr:uid="{00000000-0005-0000-0000-0000B1030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ_БЕЛ" xfId="947" xr:uid="{00000000-0005-0000-0000-0000B2030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ_РЕЧ" xfId="948" xr:uid="{00000000-0005-0000-0000-0000B3030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБДИЗ" xfId="949" xr:uid="{00000000-0005-0000-0000-0000B4030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ" xfId="950" xr:uid="{00000000-0005-0000-0000-0000B5030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="951" xr:uid="{00000000-0005-0000-0000-0000B6030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="952" xr:uid="{00000000-0005-0000-0000-0000B7030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Дети" xfId="953" xr:uid="{00000000-0005-0000-0000-0000B8030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Дистанц." xfId="954" xr:uid="{00000000-0005-0000-0000-0000B9030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Индив." xfId="955" xr:uid="{00000000-0005-0000-0000-0000BA030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Индив._БЕЛ" xfId="956" xr:uid="{00000000-0005-0000-0000-0000BB030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Индив._РЕЧ" xfId="957" xr:uid="{00000000-0005-0000-0000-0000BC030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь" xfId="958" xr:uid="{00000000-0005-0000-0000-0000BD030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Август" xfId="959" xr:uid="{00000000-0005-0000-0000-0000BE030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Дистанц." xfId="960" xr:uid="{00000000-0005-0000-0000-0000BF030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Индив." xfId="961" xr:uid="{00000000-0005-0000-0000-0000C0030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_КБУ" xfId="962" xr:uid="{00000000-0005-0000-0000-0000C1030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_КБУ" xfId="963" xr:uid="{00000000-0005-0000-0000-0000C2030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_КРН" xfId="964" xr:uid="{00000000-0005-0000-0000-0000C3030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_ОПШ" xfId="965" xr:uid="{00000000-0005-0000-0000-0000C4030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Июнь_СР" xfId="966" xr:uid="{00000000-0005-0000-0000-0000C5030000}"/>
-    <cellStyle name="_СЧДОГ_Май_КБУ" xfId="967" xr:uid="{00000000-0005-0000-0000-0000C6030000}"/>
-    <cellStyle name="_СЧДОГ_Май_КРН" xfId="968" xr:uid="{00000000-0005-0000-0000-0000C7030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май" xfId="969" xr:uid="{00000000-0005-0000-0000-0000C8030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Август" xfId="970" xr:uid="{00000000-0005-0000-0000-0000C9030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Август_Дистанц." xfId="971" xr:uid="{00000000-0005-0000-0000-0000CA030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Август_Индив." xfId="972" xr:uid="{00000000-0005-0000-0000-0000CB030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_БЕЛ" xfId="973" xr:uid="{00000000-0005-0000-0000-0000CC030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_БИНТ" xfId="974" xr:uid="{00000000-0005-0000-0000-0000CD030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_БИНТ_БЕЛ" xfId="975" xr:uid="{00000000-0005-0000-0000-0000CE030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_БИНТ_РЕЧ" xfId="976" xr:uid="{00000000-0005-0000-0000-0000CF030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_ВЕБДИЗ" xfId="977" xr:uid="{00000000-0005-0000-0000-0000D0030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ" xfId="978" xr:uid="{00000000-0005-0000-0000-0000D1030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ_БЕЛ" xfId="979" xr:uid="{00000000-0005-0000-0000-0000D2030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ_РЕЧ" xfId="980" xr:uid="{00000000-0005-0000-0000-0000D3030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Дети" xfId="981" xr:uid="{00000000-0005-0000-0000-0000D4030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Дистанц." xfId="982" xr:uid="{00000000-0005-0000-0000-0000D5030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Индив." xfId="983" xr:uid="{00000000-0005-0000-0000-0000D6030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Индив._БЕЛ" xfId="984" xr:uid="{00000000-0005-0000-0000-0000D7030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Индив._РЕЧ" xfId="985" xr:uid="{00000000-0005-0000-0000-0000D8030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Июнь" xfId="986" xr:uid="{00000000-0005-0000-0000-0000D9030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Август" xfId="987" xr:uid="{00000000-0005-0000-0000-0000DA030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Дистанц." xfId="988" xr:uid="{00000000-0005-0000-0000-0000DB030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Индив." xfId="989" xr:uid="{00000000-0005-0000-0000-0000DC030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_Июнь_КБУ" xfId="990" xr:uid="{00000000-0005-0000-0000-0000DD030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_КБУ" xfId="991" xr:uid="{00000000-0005-0000-0000-0000DE030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_КРН" xfId="992" xr:uid="{00000000-0005-0000-0000-0000DF030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_ОПШ" xfId="993" xr:uid="{00000000-0005-0000-0000-0000E0030000}"/>
-    <cellStyle name="_СЧДОГ_Май_Май_СР" xfId="994" xr:uid="{00000000-0005-0000-0000-0000E1030000}"/>
-    <cellStyle name="_СЧДОГ_Май_ОПШ" xfId="995" xr:uid="{00000000-0005-0000-0000-0000E2030000}"/>
-    <cellStyle name="_СЧДОГ_Май_РЕЧ" xfId="996" xr:uid="{00000000-0005-0000-0000-0000E3030000}"/>
-    <cellStyle name="_СЧДОГ_Май_РЕЧ_БЕЛ" xfId="997" xr:uid="{00000000-0005-0000-0000-0000E4030000}"/>
-    <cellStyle name="_СЧДОГ_Май_РЕЧ_РЕЧ" xfId="998" xr:uid="{00000000-0005-0000-0000-0000E5030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СИ" xfId="999" xr:uid="{00000000-0005-0000-0000-0000E6030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СИ_БЕЛ" xfId="1000" xr:uid="{00000000-0005-0000-0000-0000E7030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СИ_РЕЧ" xfId="1001" xr:uid="{00000000-0005-0000-0000-0000E8030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СР" xfId="1002" xr:uid="{00000000-0005-0000-0000-0000E9030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СУБД" xfId="1003" xr:uid="{00000000-0005-0000-0000-0000EA030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СУБД_БЕЛ" xfId="1004" xr:uid="{00000000-0005-0000-0000-0000EB030000}"/>
-    <cellStyle name="_СЧДОГ_Май_СУБД_РЕЧ" xfId="1005" xr:uid="{00000000-0005-0000-0000-0000EC030000}"/>
-    <cellStyle name="_СЧДОГ_НТ" xfId="1006" xr:uid="{00000000-0005-0000-0000-0000ED030000}"/>
-    <cellStyle name="_СЧДОГ_НТ_БЕЛ" xfId="1007" xr:uid="{00000000-0005-0000-0000-0000EE030000}"/>
-    <cellStyle name="_СЧДОГ_НТ_РЕЧ" xfId="1008" xr:uid="{00000000-0005-0000-0000-0000EF030000}"/>
-    <cellStyle name="_СЧДОГ_ОПШ" xfId="1009" xr:uid="{00000000-0005-0000-0000-0000F0030000}"/>
-    <cellStyle name="_СЧДОГ_Офис" xfId="1010" xr:uid="{00000000-0005-0000-0000-0000F1030000}"/>
-    <cellStyle name="_СЧДОГ_Офис_БЕЛ" xfId="1011" xr:uid="{00000000-0005-0000-0000-0000F2030000}"/>
-    <cellStyle name="_СЧДОГ_Офис_РЕЧ" xfId="1012" xr:uid="{00000000-0005-0000-0000-0000F3030000}"/>
-    <cellStyle name="_СЧДОГ_РЕЧ" xfId="1013" xr:uid="{00000000-0005-0000-0000-0000F4030000}"/>
-    <cellStyle name="_СЧДОГ_РЕЧ_БЕЛ" xfId="1014" xr:uid="{00000000-0005-0000-0000-0000F5030000}"/>
-    <cellStyle name="_СЧДОГ_РЕЧ_РЕЧ" xfId="1015" xr:uid="{00000000-0005-0000-0000-0000F6030000}"/>
-    <cellStyle name="_СЧДОГ_СИ" xfId="1016" xr:uid="{00000000-0005-0000-0000-0000F7030000}"/>
-    <cellStyle name="_СЧДОГ_СИ_БЕЛ" xfId="1017" xr:uid="{00000000-0005-0000-0000-0000F8030000}"/>
-    <cellStyle name="_СЧДОГ_СИ_РЕЧ" xfId="1018" xr:uid="{00000000-0005-0000-0000-0000F9030000}"/>
-    <cellStyle name="_СЧДОГ_СИС" xfId="1019" xr:uid="{00000000-0005-0000-0000-0000FA030000}"/>
-    <cellStyle name="_СЧДОГ_СИС_БЕЛ" xfId="1020" xr:uid="{00000000-0005-0000-0000-0000FB030000}"/>
-    <cellStyle name="_СЧДОГ_СИС_РЕЧ" xfId="1021" xr:uid="{00000000-0005-0000-0000-0000FC030000}"/>
-    <cellStyle name="_СЧДОГ_СР" xfId="1022" xr:uid="{00000000-0005-0000-0000-0000FD030000}"/>
-    <cellStyle name="_СЧДОГ_СУБД" xfId="1023" xr:uid="{00000000-0005-0000-0000-0000FE030000}"/>
-    <cellStyle name="_СЧДОГ_СУБД_БЕЛ" xfId="1024" xr:uid="{00000000-0005-0000-0000-0000FF030000}"/>
-    <cellStyle name="_СЧДОГ_СУБД_РЕЧ" xfId="1025" xr:uid="{00000000-0005-0000-0000-000000040000}"/>
-    <cellStyle name="_СЧДОГ_ТЕК" xfId="1026" xr:uid="{00000000-0005-0000-0000-000001040000}"/>
-    <cellStyle name="_СЧДОГ_ТЕК_БЕЛ" xfId="1027" xr:uid="{00000000-0005-0000-0000-000002040000}"/>
-    <cellStyle name="_СЧДОГ_ТЕК_РЕЧ" xfId="1028" xr:uid="{00000000-0005-0000-0000-000003040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль" xfId="1029" xr:uid="{00000000-0005-0000-0000-000004040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Август" xfId="1030" xr:uid="{00000000-0005-0000-0000-000005040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Август_Дистанц." xfId="1031" xr:uid="{00000000-0005-0000-0000-000006040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Август_Индив." xfId="1032" xr:uid="{00000000-0005-0000-0000-000007040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_АКАД" xfId="1033" xr:uid="{00000000-0005-0000-0000-000008040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_АКАД_БЕЛ" xfId="1034" xr:uid="{00000000-0005-0000-0000-000009040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_АКАД_РЕЧ" xfId="1035" xr:uid="{00000000-0005-0000-0000-00000A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Б9560" xfId="1036" xr:uid="{00000000-0005-0000-0000-00000B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Б9560_БЕЛ" xfId="1037" xr:uid="{00000000-0005-0000-0000-00000C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Б9560_РЕЧ" xfId="1038" xr:uid="{00000000-0005-0000-0000-00000D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БЕЛ" xfId="1039" xr:uid="{00000000-0005-0000-0000-00000E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БИНТ" xfId="1040" xr:uid="{00000000-0005-0000-0000-00000F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БИНТ_БЕЛ" xfId="1041" xr:uid="{00000000-0005-0000-0000-000010040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БИНТ_РЕЧ" xfId="1042" xr:uid="{00000000-0005-0000-0000-000011040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БУХ" xfId="1043" xr:uid="{00000000-0005-0000-0000-000012040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БУХ_БЕЛ" xfId="1044" xr:uid="{00000000-0005-0000-0000-000013040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_БУХ_РЕЧ" xfId="1045" xr:uid="{00000000-0005-0000-0000-000014040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_ВЕБДИЗ" xfId="1046" xr:uid="{00000000-0005-0000-0000-000015040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ" xfId="1047" xr:uid="{00000000-0005-0000-0000-000016040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ_БЕЛ" xfId="1048" xr:uid="{00000000-0005-0000-0000-000017040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ_РЕЧ" xfId="1049" xr:uid="{00000000-0005-0000-0000-000018040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Дети" xfId="1050" xr:uid="{00000000-0005-0000-0000-000019040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Дистанц." xfId="1051" xr:uid="{00000000-0005-0000-0000-00001A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Индив." xfId="1052" xr:uid="{00000000-0005-0000-0000-00001B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Индив._БЕЛ" xfId="1053" xr:uid="{00000000-0005-0000-0000-00001C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Индив._РЕЧ" xfId="1054" xr:uid="{00000000-0005-0000-0000-00001D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль" xfId="1055" xr:uid="{00000000-0005-0000-0000-00001E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Август" xfId="1056" xr:uid="{00000000-0005-0000-0000-00001F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Август_Дистанц." xfId="1057" xr:uid="{00000000-0005-0000-0000-000020040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Август_Индив." xfId="1058" xr:uid="{00000000-0005-0000-0000-000021040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_БЕЛ" xfId="1059" xr:uid="{00000000-0005-0000-0000-000022040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ" xfId="1060" xr:uid="{00000000-0005-0000-0000-000023040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ_БЕЛ" xfId="1061" xr:uid="{00000000-0005-0000-0000-000024040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ_РЕЧ" xfId="1062" xr:uid="{00000000-0005-0000-0000-000025040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБДИЗ" xfId="1063" xr:uid="{00000000-0005-0000-0000-000026040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ" xfId="1064" xr:uid="{00000000-0005-0000-0000-000027040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1065" xr:uid="{00000000-0005-0000-0000-000028040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1066" xr:uid="{00000000-0005-0000-0000-000029040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Дети" xfId="1067" xr:uid="{00000000-0005-0000-0000-00002A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Дистанц." xfId="1068" xr:uid="{00000000-0005-0000-0000-00002B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив." xfId="1069" xr:uid="{00000000-0005-0000-0000-00002C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив._БЕЛ" xfId="1070" xr:uid="{00000000-0005-0000-0000-00002D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив._РЕЧ" xfId="1071" xr:uid="{00000000-0005-0000-0000-00002E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь" xfId="1072" xr:uid="{00000000-0005-0000-0000-00002F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Август" xfId="1073" xr:uid="{00000000-0005-0000-0000-000030040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Дистанц." xfId="1074" xr:uid="{00000000-0005-0000-0000-000031040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Индив." xfId="1075" xr:uid="{00000000-0005-0000-0000-000032040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_КБУ" xfId="1076" xr:uid="{00000000-0005-0000-0000-000033040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_КБУ" xfId="1077" xr:uid="{00000000-0005-0000-0000-000034040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_КРН" xfId="1078" xr:uid="{00000000-0005-0000-0000-000035040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_ОПШ" xfId="1079" xr:uid="{00000000-0005-0000-0000-000036040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июль_СР" xfId="1080" xr:uid="{00000000-0005-0000-0000-000037040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь" xfId="1081" xr:uid="{00000000-0005-0000-0000-000038040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_1" xfId="1082" xr:uid="{00000000-0005-0000-0000-000039040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Август" xfId="1083" xr:uid="{00000000-0005-0000-0000-00003A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Дистанц." xfId="1084" xr:uid="{00000000-0005-0000-0000-00003B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Индив." xfId="1085" xr:uid="{00000000-0005-0000-0000-00003C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_КБУ" xfId="1086" xr:uid="{00000000-0005-0000-0000-00003D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август" xfId="1087" xr:uid="{00000000-0005-0000-0000-00003E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август_Дистанц." xfId="1088" xr:uid="{00000000-0005-0000-0000-00003F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август_Индив." xfId="1089" xr:uid="{00000000-0005-0000-0000-000040040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БЕЛ" xfId="1090" xr:uid="{00000000-0005-0000-0000-000041040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ" xfId="1091" xr:uid="{00000000-0005-0000-0000-000042040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ_БЕЛ" xfId="1092" xr:uid="{00000000-0005-0000-0000-000043040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ_РЕЧ" xfId="1093" xr:uid="{00000000-0005-0000-0000-000044040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ" xfId="1094" xr:uid="{00000000-0005-0000-0000-000045040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ_БЕЛ" xfId="1095" xr:uid="{00000000-0005-0000-0000-000046040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ_РЕЧ" xfId="1096" xr:uid="{00000000-0005-0000-0000-000047040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБДИЗ" xfId="1097" xr:uid="{00000000-0005-0000-0000-000048040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ" xfId="1098" xr:uid="{00000000-0005-0000-0000-000049040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1099" xr:uid="{00000000-0005-0000-0000-00004A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1100" xr:uid="{00000000-0005-0000-0000-00004B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Дети" xfId="1101" xr:uid="{00000000-0005-0000-0000-00004C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Дистанц." xfId="1102" xr:uid="{00000000-0005-0000-0000-00004D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив." xfId="1103" xr:uid="{00000000-0005-0000-0000-00004E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив._БЕЛ" xfId="1104" xr:uid="{00000000-0005-0000-0000-00004F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив._РЕЧ" xfId="1105" xr:uid="{00000000-0005-0000-0000-000050040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь" xfId="1106" xr:uid="{00000000-0005-0000-0000-000051040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Август" xfId="1107" xr:uid="{00000000-0005-0000-0000-000052040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Дистанц." xfId="1108" xr:uid="{00000000-0005-0000-0000-000053040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Индив." xfId="1109" xr:uid="{00000000-0005-0000-0000-000054040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_КБУ" xfId="1110" xr:uid="{00000000-0005-0000-0000-000055040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_КБУ" xfId="1111" xr:uid="{00000000-0005-0000-0000-000056040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_КРН" xfId="1112" xr:uid="{00000000-0005-0000-0000-000057040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_ОПШ" xfId="1113" xr:uid="{00000000-0005-0000-0000-000058040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Июнь_СР" xfId="1114" xr:uid="{00000000-0005-0000-0000-000059040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_КБУ" xfId="1115" xr:uid="{00000000-0005-0000-0000-00005A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_КРН" xfId="1116" xr:uid="{00000000-0005-0000-0000-00005B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май" xfId="1117" xr:uid="{00000000-0005-0000-0000-00005C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Август" xfId="1118" xr:uid="{00000000-0005-0000-0000-00005D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Август_Дистанц." xfId="1119" xr:uid="{00000000-0005-0000-0000-00005E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Август_Индив." xfId="1120" xr:uid="{00000000-0005-0000-0000-00005F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_БЕЛ" xfId="1121" xr:uid="{00000000-0005-0000-0000-000060040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ" xfId="1122" xr:uid="{00000000-0005-0000-0000-000061040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ_БЕЛ" xfId="1123" xr:uid="{00000000-0005-0000-0000-000062040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ_РЕЧ" xfId="1124" xr:uid="{00000000-0005-0000-0000-000063040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБДИЗ" xfId="1125" xr:uid="{00000000-0005-0000-0000-000064040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ" xfId="1126" xr:uid="{00000000-0005-0000-0000-000065040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1127" xr:uid="{00000000-0005-0000-0000-000066040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1128" xr:uid="{00000000-0005-0000-0000-000067040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Дети" xfId="1129" xr:uid="{00000000-0005-0000-0000-000068040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Дистанц." xfId="1130" xr:uid="{00000000-0005-0000-0000-000069040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Индив." xfId="1131" xr:uid="{00000000-0005-0000-0000-00006A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Индив._БЕЛ" xfId="1132" xr:uid="{00000000-0005-0000-0000-00006B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Индив._РЕЧ" xfId="1133" xr:uid="{00000000-0005-0000-0000-00006C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь" xfId="1134" xr:uid="{00000000-0005-0000-0000-00006D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Август" xfId="1135" xr:uid="{00000000-0005-0000-0000-00006E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Дистанц." xfId="1136" xr:uid="{00000000-0005-0000-0000-00006F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Индив." xfId="1137" xr:uid="{00000000-0005-0000-0000-000070040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_КБУ" xfId="1138" xr:uid="{00000000-0005-0000-0000-000071040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_КБУ" xfId="1139" xr:uid="{00000000-0005-0000-0000-000072040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_КРН" xfId="1140" xr:uid="{00000000-0005-0000-0000-000073040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_ОПШ" xfId="1141" xr:uid="{00000000-0005-0000-0000-000074040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_Май_СР" xfId="1142" xr:uid="{00000000-0005-0000-0000-000075040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_ОПШ" xfId="1143" xr:uid="{00000000-0005-0000-0000-000076040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_РЕЧ" xfId="1144" xr:uid="{00000000-0005-0000-0000-000077040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_РЕЧ_БЕЛ" xfId="1145" xr:uid="{00000000-0005-0000-0000-000078040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_РЕЧ_РЕЧ" xfId="1146" xr:uid="{00000000-0005-0000-0000-000079040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СИ" xfId="1147" xr:uid="{00000000-0005-0000-0000-00007A040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СИ_БЕЛ" xfId="1148" xr:uid="{00000000-0005-0000-0000-00007B040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СИ_РЕЧ" xfId="1149" xr:uid="{00000000-0005-0000-0000-00007C040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СР" xfId="1150" xr:uid="{00000000-0005-0000-0000-00007D040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СУБД" xfId="1151" xr:uid="{00000000-0005-0000-0000-00007E040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СУБД_БЕЛ" xfId="1152" xr:uid="{00000000-0005-0000-0000-00007F040000}"/>
-    <cellStyle name="_СЧДОГ_Февраль_СУБД_РЕЧ" xfId="1153" xr:uid="{00000000-0005-0000-0000-000080040000}"/>
-    <cellStyle name="_СЧДОГ_ФШ" xfId="1154" xr:uid="{00000000-0005-0000-0000-000081040000}"/>
-    <cellStyle name="_СЧДОГ_ФШ_БЕЛ" xfId="1155" xr:uid="{00000000-0005-0000-0000-000082040000}"/>
-    <cellStyle name="_СЧДОГ_ФШ_РЕЧ" xfId="1156" xr:uid="{00000000-0005-0000-0000-000083040000}"/>
-    <cellStyle name="_ТЕК" xfId="1157" xr:uid="{00000000-0005-0000-0000-000084040000}"/>
-    <cellStyle name="_ТЕК_БЕЛ" xfId="1158" xr:uid="{00000000-0005-0000-0000-000085040000}"/>
-    <cellStyle name="_ТЕК_РЕЧ" xfId="1159" xr:uid="{00000000-0005-0000-0000-000086040000}"/>
-    <cellStyle name="_ТОР" xfId="1160" xr:uid="{00000000-0005-0000-0000-000087040000}"/>
-    <cellStyle name="_ТОР_БЕЛ" xfId="1161" xr:uid="{00000000-0005-0000-0000-000088040000}"/>
-    <cellStyle name="_ТОР_РЕЧ" xfId="1162" xr:uid="{00000000-0005-0000-0000-000089040000}"/>
-    <cellStyle name="_Февраль" xfId="1163" xr:uid="{00000000-0005-0000-0000-00008A040000}"/>
-    <cellStyle name="_Февраль_Август" xfId="1164" xr:uid="{00000000-0005-0000-0000-00008B040000}"/>
-    <cellStyle name="_Февраль_Август_Дистанц." xfId="1165" xr:uid="{00000000-0005-0000-0000-00008C040000}"/>
-    <cellStyle name="_Февраль_Август_Индив." xfId="1166" xr:uid="{00000000-0005-0000-0000-00008D040000}"/>
-    <cellStyle name="_Февраль_АКАД" xfId="1167" xr:uid="{00000000-0005-0000-0000-00008E040000}"/>
-    <cellStyle name="_Февраль_АКАД_БЕЛ" xfId="1168" xr:uid="{00000000-0005-0000-0000-00008F040000}"/>
-    <cellStyle name="_Февраль_АКАД_РЕЧ" xfId="1169" xr:uid="{00000000-0005-0000-0000-000090040000}"/>
-    <cellStyle name="_Февраль_Б9560" xfId="1170" xr:uid="{00000000-0005-0000-0000-000091040000}"/>
-    <cellStyle name="_Февраль_Б9560_БЕЛ" xfId="1171" xr:uid="{00000000-0005-0000-0000-000092040000}"/>
-    <cellStyle name="_Февраль_Б9560_РЕЧ" xfId="1172" xr:uid="{00000000-0005-0000-0000-000093040000}"/>
-    <cellStyle name="_Февраль_БЕЛ" xfId="1173" xr:uid="{00000000-0005-0000-0000-000094040000}"/>
-    <cellStyle name="_Февраль_БИНТ" xfId="1174" xr:uid="{00000000-0005-0000-0000-000095040000}"/>
-    <cellStyle name="_Февраль_БИНТ_БЕЛ" xfId="1175" xr:uid="{00000000-0005-0000-0000-000096040000}"/>
-    <cellStyle name="_Февраль_БИНТ_РЕЧ" xfId="1176" xr:uid="{00000000-0005-0000-0000-000097040000}"/>
-    <cellStyle name="_Февраль_БУХ" xfId="1177" xr:uid="{00000000-0005-0000-0000-000098040000}"/>
-    <cellStyle name="_Февраль_БУХ_БЕЛ" xfId="1178" xr:uid="{00000000-0005-0000-0000-000099040000}"/>
-    <cellStyle name="_Февраль_БУХ_РЕЧ" xfId="1179" xr:uid="{00000000-0005-0000-0000-00009A040000}"/>
-    <cellStyle name="_Февраль_ВЕБДИЗ" xfId="1180" xr:uid="{00000000-0005-0000-0000-00009B040000}"/>
-    <cellStyle name="_Февраль_ВЕБМАСТ" xfId="1181" xr:uid="{00000000-0005-0000-0000-00009C040000}"/>
-    <cellStyle name="_Февраль_ВЕБМАСТ_БЕЛ" xfId="1182" xr:uid="{00000000-0005-0000-0000-00009D040000}"/>
-    <cellStyle name="_Февраль_ВЕБМАСТ_РЕЧ" xfId="1183" xr:uid="{00000000-0005-0000-0000-00009E040000}"/>
-    <cellStyle name="_Февраль_Дети" xfId="1184" xr:uid="{00000000-0005-0000-0000-00009F040000}"/>
-    <cellStyle name="_Февраль_Дистанц." xfId="1185" xr:uid="{00000000-0005-0000-0000-0000A0040000}"/>
-    <cellStyle name="_Февраль_Индив." xfId="1186" xr:uid="{00000000-0005-0000-0000-0000A1040000}"/>
-    <cellStyle name="_Февраль_Индив._БЕЛ" xfId="1187" xr:uid="{00000000-0005-0000-0000-0000A2040000}"/>
-    <cellStyle name="_Февраль_Индив._РЕЧ" xfId="1188" xr:uid="{00000000-0005-0000-0000-0000A3040000}"/>
-    <cellStyle name="_Февраль_Июль" xfId="1189" xr:uid="{00000000-0005-0000-0000-0000A4040000}"/>
-    <cellStyle name="_Февраль_Июль_Август" xfId="1190" xr:uid="{00000000-0005-0000-0000-0000A5040000}"/>
-    <cellStyle name="_Февраль_Июль_Август_Дистанц." xfId="1191" xr:uid="{00000000-0005-0000-0000-0000A6040000}"/>
-    <cellStyle name="_Февраль_Июль_Август_Индив." xfId="1192" xr:uid="{00000000-0005-0000-0000-0000A7040000}"/>
-    <cellStyle name="_Февраль_Июль_БЕЛ" xfId="1193" xr:uid="{00000000-0005-0000-0000-0000A8040000}"/>
-    <cellStyle name="_Февраль_Июль_БИНТ" xfId="1194" xr:uid="{00000000-0005-0000-0000-0000A9040000}"/>
-    <cellStyle name="_Февраль_Июль_БИНТ_БЕЛ" xfId="1195" xr:uid="{00000000-0005-0000-0000-0000AA040000}"/>
-    <cellStyle name="_Февраль_Июль_БИНТ_РЕЧ" xfId="1196" xr:uid="{00000000-0005-0000-0000-0000AB040000}"/>
-    <cellStyle name="_Февраль_Июль_ВЕБДИЗ" xfId="1197" xr:uid="{00000000-0005-0000-0000-0000AC040000}"/>
-    <cellStyle name="_Февраль_Июль_ВЕБМАСТ" xfId="1198" xr:uid="{00000000-0005-0000-0000-0000AD040000}"/>
-    <cellStyle name="_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1199" xr:uid="{00000000-0005-0000-0000-0000AE040000}"/>
-    <cellStyle name="_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1200" xr:uid="{00000000-0005-0000-0000-0000AF040000}"/>
-    <cellStyle name="_Февраль_Июль_Дети" xfId="1201" xr:uid="{00000000-0005-0000-0000-0000B0040000}"/>
-    <cellStyle name="_Февраль_Июль_Дистанц." xfId="1202" xr:uid="{00000000-0005-0000-0000-0000B1040000}"/>
-    <cellStyle name="_Февраль_Июль_Индив." xfId="1203" xr:uid="{00000000-0005-0000-0000-0000B2040000}"/>
-    <cellStyle name="_Февраль_Июль_Индив._БЕЛ" xfId="1204" xr:uid="{00000000-0005-0000-0000-0000B3040000}"/>
-    <cellStyle name="_Февраль_Июль_Индив._РЕЧ" xfId="1205" xr:uid="{00000000-0005-0000-0000-0000B4040000}"/>
-    <cellStyle name="_Февраль_Июль_Июнь" xfId="1206" xr:uid="{00000000-0005-0000-0000-0000B5040000}"/>
-    <cellStyle name="_Февраль_Июль_Июнь_Август" xfId="1207" xr:uid="{00000000-0005-0000-0000-0000B6040000}"/>
-    <cellStyle name="_Февраль_Июль_Июнь_Дистанц." xfId="1208" xr:uid="{00000000-0005-0000-0000-0000B7040000}"/>
-    <cellStyle name="_Февраль_Июль_Июнь_Индив." xfId="1209" xr:uid="{00000000-0005-0000-0000-0000B8040000}"/>
-    <cellStyle name="_Февраль_Июль_Июнь_КБУ" xfId="1210" xr:uid="{00000000-0005-0000-0000-0000B9040000}"/>
-    <cellStyle name="_Февраль_Июль_КБУ" xfId="1211" xr:uid="{00000000-0005-0000-0000-0000BA040000}"/>
-    <cellStyle name="_Февраль_Июль_КРН" xfId="1212" xr:uid="{00000000-0005-0000-0000-0000BB040000}"/>
-    <cellStyle name="_Февраль_Июль_ОПШ" xfId="1213" xr:uid="{00000000-0005-0000-0000-0000BC040000}"/>
-    <cellStyle name="_Февраль_Июль_СР" xfId="1214" xr:uid="{00000000-0005-0000-0000-0000BD040000}"/>
-    <cellStyle name="_Февраль_Июнь" xfId="1215" xr:uid="{00000000-0005-0000-0000-0000BE040000}"/>
-    <cellStyle name="_Февраль_Июнь_1" xfId="1216" xr:uid="{00000000-0005-0000-0000-0000BF040000}"/>
-    <cellStyle name="_Февраль_Июнь_1_Август" xfId="1217" xr:uid="{00000000-0005-0000-0000-0000C0040000}"/>
-    <cellStyle name="_Февраль_Июнь_1_Дистанц." xfId="1218" xr:uid="{00000000-0005-0000-0000-0000C1040000}"/>
-    <cellStyle name="_Февраль_Июнь_1_Индив." xfId="1219" xr:uid="{00000000-0005-0000-0000-0000C2040000}"/>
-    <cellStyle name="_Февраль_Июнь_1_КБУ" xfId="1220" xr:uid="{00000000-0005-0000-0000-0000C3040000}"/>
-    <cellStyle name="_Февраль_Июнь_Август" xfId="1221" xr:uid="{00000000-0005-0000-0000-0000C4040000}"/>
-    <cellStyle name="_Февраль_Июнь_Август_Дистанц." xfId="1222" xr:uid="{00000000-0005-0000-0000-0000C5040000}"/>
-    <cellStyle name="_Февраль_Июнь_Август_Индив." xfId="1223" xr:uid="{00000000-0005-0000-0000-0000C6040000}"/>
-    <cellStyle name="_Февраль_Июнь_БЕЛ" xfId="1224" xr:uid="{00000000-0005-0000-0000-0000C7040000}"/>
-    <cellStyle name="_Февраль_Июнь_БИНТ" xfId="1225" xr:uid="{00000000-0005-0000-0000-0000C8040000}"/>
-    <cellStyle name="_Февраль_Июнь_БИНТ_БЕЛ" xfId="1226" xr:uid="{00000000-0005-0000-0000-0000C9040000}"/>
-    <cellStyle name="_Февраль_Июнь_БИНТ_РЕЧ" xfId="1227" xr:uid="{00000000-0005-0000-0000-0000CA040000}"/>
-    <cellStyle name="_Февраль_Июнь_БУХ" xfId="1228" xr:uid="{00000000-0005-0000-0000-0000CB040000}"/>
-    <cellStyle name="_Февраль_Июнь_БУХ_БЕЛ" xfId="1229" xr:uid="{00000000-0005-0000-0000-0000CC040000}"/>
-    <cellStyle name="_Февраль_Июнь_БУХ_РЕЧ" xfId="1230" xr:uid="{00000000-0005-0000-0000-0000CD040000}"/>
-    <cellStyle name="_Февраль_Июнь_ВЕБДИЗ" xfId="1231" xr:uid="{00000000-0005-0000-0000-0000CE040000}"/>
-    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ" xfId="1232" xr:uid="{00000000-0005-0000-0000-0000CF040000}"/>
-    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1233" xr:uid="{00000000-0005-0000-0000-0000D0040000}"/>
-    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1234" xr:uid="{00000000-0005-0000-0000-0000D1040000}"/>
-    <cellStyle name="_Февраль_Июнь_Дети" xfId="1235" xr:uid="{00000000-0005-0000-0000-0000D2040000}"/>
-    <cellStyle name="_Февраль_Июнь_Дистанц." xfId="1236" xr:uid="{00000000-0005-0000-0000-0000D3040000}"/>
-    <cellStyle name="_Февраль_Июнь_Индив." xfId="1237" xr:uid="{00000000-0005-0000-0000-0000D4040000}"/>
-    <cellStyle name="_Февраль_Июнь_Индив._БЕЛ" xfId="1238" xr:uid="{00000000-0005-0000-0000-0000D5040000}"/>
-    <cellStyle name="_Февраль_Июнь_Индив._РЕЧ" xfId="1239" xr:uid="{00000000-0005-0000-0000-0000D6040000}"/>
-    <cellStyle name="_Февраль_Июнь_Июнь" xfId="1240" xr:uid="{00000000-0005-0000-0000-0000D7040000}"/>
-    <cellStyle name="_Февраль_Июнь_Июнь_Август" xfId="1241" xr:uid="{00000000-0005-0000-0000-0000D8040000}"/>
-    <cellStyle name="_Февраль_Июнь_Июнь_Дистанц." xfId="1242" xr:uid="{00000000-0005-0000-0000-0000D9040000}"/>
-    <cellStyle name="_Февраль_Июнь_Июнь_Индив." xfId="1243" xr:uid="{00000000-0005-0000-0000-0000DA040000}"/>
-    <cellStyle name="_Февраль_Июнь_Июнь_КБУ" xfId="1244" xr:uid="{00000000-0005-0000-0000-0000DB040000}"/>
-    <cellStyle name="_Февраль_Июнь_КБУ" xfId="1245" xr:uid="{00000000-0005-0000-0000-0000DC040000}"/>
-    <cellStyle name="_Февраль_Июнь_КРН" xfId="1246" xr:uid="{00000000-0005-0000-0000-0000DD040000}"/>
-    <cellStyle name="_Февраль_Июнь_ОПШ" xfId="1247" xr:uid="{00000000-0005-0000-0000-0000DE040000}"/>
-    <cellStyle name="_Февраль_Июнь_СР" xfId="1248" xr:uid="{00000000-0005-0000-0000-0000DF040000}"/>
-    <cellStyle name="_Февраль_КБУ" xfId="1249" xr:uid="{00000000-0005-0000-0000-0000E0040000}"/>
-    <cellStyle name="_Февраль_КРН" xfId="1250" xr:uid="{00000000-0005-0000-0000-0000E1040000}"/>
-    <cellStyle name="_Февраль_Май" xfId="1251" xr:uid="{00000000-0005-0000-0000-0000E2040000}"/>
-    <cellStyle name="_Февраль_Май_Август" xfId="1252" xr:uid="{00000000-0005-0000-0000-0000E3040000}"/>
-    <cellStyle name="_Февраль_Май_Август_Дистанц." xfId="1253" xr:uid="{00000000-0005-0000-0000-0000E4040000}"/>
-    <cellStyle name="_Февраль_Май_Август_Индив." xfId="1254" xr:uid="{00000000-0005-0000-0000-0000E5040000}"/>
-    <cellStyle name="_Февраль_Май_БЕЛ" xfId="1255" xr:uid="{00000000-0005-0000-0000-0000E6040000}"/>
-    <cellStyle name="_Февраль_Май_БИНТ" xfId="1256" xr:uid="{00000000-0005-0000-0000-0000E7040000}"/>
-    <cellStyle name="_Февраль_Май_БИНТ_БЕЛ" xfId="1257" xr:uid="{00000000-0005-0000-0000-0000E8040000}"/>
-    <cellStyle name="_Февраль_Май_БИНТ_РЕЧ" xfId="1258" xr:uid="{00000000-0005-0000-0000-0000E9040000}"/>
-    <cellStyle name="_Февраль_Май_ВЕБДИЗ" xfId="1259" xr:uid="{00000000-0005-0000-0000-0000EA040000}"/>
-    <cellStyle name="_Февраль_Май_ВЕБМАСТ" xfId="1260" xr:uid="{00000000-0005-0000-0000-0000EB040000}"/>
-    <cellStyle name="_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1261" xr:uid="{00000000-0005-0000-0000-0000EC040000}"/>
-    <cellStyle name="_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1262" xr:uid="{00000000-0005-0000-0000-0000ED040000}"/>
-    <cellStyle name="_Февраль_Май_Дети" xfId="1263" xr:uid="{00000000-0005-0000-0000-0000EE040000}"/>
-    <cellStyle name="_Февраль_Май_Дистанц." xfId="1264" xr:uid="{00000000-0005-0000-0000-0000EF040000}"/>
-    <cellStyle name="_Февраль_Май_Индив." xfId="1265" xr:uid="{00000000-0005-0000-0000-0000F0040000}"/>
-    <cellStyle name="_Февраль_Май_Индив._БЕЛ" xfId="1266" xr:uid="{00000000-0005-0000-0000-0000F1040000}"/>
-    <cellStyle name="_Февраль_Май_Индив._РЕЧ" xfId="1267" xr:uid="{00000000-0005-0000-0000-0000F2040000}"/>
-    <cellStyle name="_Февраль_Май_Июнь" xfId="1268" xr:uid="{00000000-0005-0000-0000-0000F3040000}"/>
-    <cellStyle name="_Февраль_Май_Июнь_Август" xfId="1269" xr:uid="{00000000-0005-0000-0000-0000F4040000}"/>
-    <cellStyle name="_Февраль_Май_Июнь_Дистанц." xfId="1270" xr:uid="{00000000-0005-0000-0000-0000F5040000}"/>
-    <cellStyle name="_Февраль_Май_Июнь_Индив." xfId="1271" xr:uid="{00000000-0005-0000-0000-0000F6040000}"/>
-    <cellStyle name="_Февраль_Май_Июнь_КБУ" xfId="1272" xr:uid="{00000000-0005-0000-0000-0000F7040000}"/>
-    <cellStyle name="_Февраль_Май_КБУ" xfId="1273" xr:uid="{00000000-0005-0000-0000-0000F8040000}"/>
-    <cellStyle name="_Февраль_Май_КРН" xfId="1274" xr:uid="{00000000-0005-0000-0000-0000F9040000}"/>
-    <cellStyle name="_Февраль_Май_ОПШ" xfId="1275" xr:uid="{00000000-0005-0000-0000-0000FA040000}"/>
-    <cellStyle name="_Февраль_Май_СР" xfId="1276" xr:uid="{00000000-0005-0000-0000-0000FB040000}"/>
-    <cellStyle name="_Февраль_ОПШ" xfId="1277" xr:uid="{00000000-0005-0000-0000-0000FC040000}"/>
-    <cellStyle name="_Февраль_РЕЧ" xfId="1278" xr:uid="{00000000-0005-0000-0000-0000FD040000}"/>
-    <cellStyle name="_Февраль_РЕЧ_БЕЛ" xfId="1279" xr:uid="{00000000-0005-0000-0000-0000FE040000}"/>
-    <cellStyle name="_Февраль_РЕЧ_РЕЧ" xfId="1280" xr:uid="{00000000-0005-0000-0000-0000FF040000}"/>
-    <cellStyle name="_Февраль_СИ" xfId="1281" xr:uid="{00000000-0005-0000-0000-000000050000}"/>
-    <cellStyle name="_Февраль_СИ_БЕЛ" xfId="1282" xr:uid="{00000000-0005-0000-0000-000001050000}"/>
-    <cellStyle name="_Февраль_СИ_РЕЧ" xfId="1283" xr:uid="{00000000-0005-0000-0000-000002050000}"/>
-    <cellStyle name="_Февраль_СР" xfId="1284" xr:uid="{00000000-0005-0000-0000-000003050000}"/>
-    <cellStyle name="_Февраль_СУБД" xfId="1285" xr:uid="{00000000-0005-0000-0000-000004050000}"/>
-    <cellStyle name="_Февраль_СУБД_БЕЛ" xfId="1286" xr:uid="{00000000-0005-0000-0000-000005050000}"/>
-    <cellStyle name="_Февраль_СУБД_РЕЧ" xfId="1287" xr:uid="{00000000-0005-0000-0000-000006050000}"/>
-    <cellStyle name="_ФШ" xfId="1288" xr:uid="{00000000-0005-0000-0000-000007050000}"/>
-    <cellStyle name="_ФШ_Апрель" xfId="1289" xr:uid="{00000000-0005-0000-0000-000008050000}"/>
-    <cellStyle name="_ФШ_Апрель_БЕЛ" xfId="1290" xr:uid="{00000000-0005-0000-0000-000009050000}"/>
-    <cellStyle name="_ФШ_Апрель_РЕЧ" xfId="1291" xr:uid="{00000000-0005-0000-0000-00000A050000}"/>
-    <cellStyle name="_ФШ_БЕЛ" xfId="1292" xr:uid="{00000000-0005-0000-0000-00000B050000}"/>
-    <cellStyle name="_ФШ_Июль" xfId="1293" xr:uid="{00000000-0005-0000-0000-00000C050000}"/>
-    <cellStyle name="_ФШ_Июль_БЕЛ" xfId="1294" xr:uid="{00000000-0005-0000-0000-00000D050000}"/>
-    <cellStyle name="_ФШ_Июль_РЕЧ" xfId="1295" xr:uid="{00000000-0005-0000-0000-00000E050000}"/>
-    <cellStyle name="_ФШ_Июнь" xfId="1296" xr:uid="{00000000-0005-0000-0000-00000F050000}"/>
-    <cellStyle name="_ФШ_Июнь_БЕЛ" xfId="1297" xr:uid="{00000000-0005-0000-0000-000010050000}"/>
-    <cellStyle name="_ФШ_Июнь_РЕЧ" xfId="1298" xr:uid="{00000000-0005-0000-0000-000011050000}"/>
-    <cellStyle name="_ФШ_Май" xfId="1299" xr:uid="{00000000-0005-0000-0000-000012050000}"/>
-    <cellStyle name="_ФШ_Май_БЕЛ" xfId="1300" xr:uid="{00000000-0005-0000-0000-000013050000}"/>
-    <cellStyle name="_ФШ_Май_РЕЧ" xfId="1301" xr:uid="{00000000-0005-0000-0000-000014050000}"/>
-    <cellStyle name="_ФШ_РЕЧ" xfId="1302" xr:uid="{00000000-0005-0000-0000-000015050000}"/>
-    <cellStyle name="_ФШ_Февраль" xfId="1303" xr:uid="{00000000-0005-0000-0000-000016050000}"/>
-    <cellStyle name="_ФШ_Февраль_БЕЛ" xfId="1304" xr:uid="{00000000-0005-0000-0000-000017050000}"/>
-    <cellStyle name="_ФШ_Февраль_РЕЧ" xfId="1305" xr:uid="{00000000-0005-0000-0000-000018050000}"/>
-    <cellStyle name="_ФШ_Январь" xfId="1306" xr:uid="{00000000-0005-0000-0000-000019050000}"/>
-    <cellStyle name="_ФШ_Январь_БЕЛ" xfId="1307" xr:uid="{00000000-0005-0000-0000-00001A050000}"/>
-    <cellStyle name="_ФШ_Январь_РЕЧ" xfId="1308" xr:uid="{00000000-0005-0000-0000-00001B050000}"/>
-    <cellStyle name="_Январь" xfId="1309" xr:uid="{00000000-0005-0000-0000-00001C050000}"/>
-    <cellStyle name="_Январь_3ДМ" xfId="1310" xr:uid="{00000000-0005-0000-0000-00001D050000}"/>
-    <cellStyle name="_Январь_3ДМ_БЕЛ" xfId="1311" xr:uid="{00000000-0005-0000-0000-00001E050000}"/>
-    <cellStyle name="_Январь_3ДМ_РЕЧ" xfId="1312" xr:uid="{00000000-0005-0000-0000-00001F050000}"/>
-    <cellStyle name="_Январь_Август" xfId="1313" xr:uid="{00000000-0005-0000-0000-000020050000}"/>
-    <cellStyle name="_Январь_Август_Дистанц." xfId="1314" xr:uid="{00000000-0005-0000-0000-000021050000}"/>
-    <cellStyle name="_Январь_Август_Индив." xfId="1315" xr:uid="{00000000-0005-0000-0000-000022050000}"/>
-    <cellStyle name="_Январь_АКАД" xfId="1316" xr:uid="{00000000-0005-0000-0000-000023050000}"/>
-    <cellStyle name="_Январь_АКАД_БЕЛ" xfId="1317" xr:uid="{00000000-0005-0000-0000-000024050000}"/>
-    <cellStyle name="_Январь_АКАД_РЕЧ" xfId="1318" xr:uid="{00000000-0005-0000-0000-000025050000}"/>
-    <cellStyle name="_Январь_Апрель" xfId="1319" xr:uid="{00000000-0005-0000-0000-000026050000}"/>
-    <cellStyle name="_Январь_Апрель_3ДМ" xfId="1320" xr:uid="{00000000-0005-0000-0000-000027050000}"/>
-    <cellStyle name="_Январь_Апрель_3ДМ_БЕЛ" xfId="1321" xr:uid="{00000000-0005-0000-0000-000028050000}"/>
-    <cellStyle name="_Январь_Апрель_3ДМ_РЕЧ" xfId="1322" xr:uid="{00000000-0005-0000-0000-000029050000}"/>
-    <cellStyle name="_Январь_Апрель_Август" xfId="1323" xr:uid="{00000000-0005-0000-0000-00002A050000}"/>
-    <cellStyle name="_Январь_Апрель_Август_Дистанц." xfId="1324" xr:uid="{00000000-0005-0000-0000-00002B050000}"/>
-    <cellStyle name="_Январь_Апрель_Август_Индив." xfId="1325" xr:uid="{00000000-0005-0000-0000-00002C050000}"/>
-    <cellStyle name="_Январь_Апрель_АКАД" xfId="1326" xr:uid="{00000000-0005-0000-0000-00002D050000}"/>
-    <cellStyle name="_Январь_Апрель_АКАД_БЕЛ" xfId="1327" xr:uid="{00000000-0005-0000-0000-00002E050000}"/>
-    <cellStyle name="_Январь_Апрель_АКАД_РЕЧ" xfId="1328" xr:uid="{00000000-0005-0000-0000-00002F050000}"/>
-    <cellStyle name="_Январь_Апрель_Б9560" xfId="1329" xr:uid="{00000000-0005-0000-0000-000030050000}"/>
-    <cellStyle name="_Январь_Апрель_Б9560_БЕЛ" xfId="1330" xr:uid="{00000000-0005-0000-0000-000031050000}"/>
-    <cellStyle name="_Январь_Апрель_Б9560_РЕЧ" xfId="1331" xr:uid="{00000000-0005-0000-0000-000032050000}"/>
-    <cellStyle name="_Январь_Апрель_БЕЛ" xfId="1332" xr:uid="{00000000-0005-0000-0000-000033050000}"/>
-    <cellStyle name="_Январь_Апрель_БИНТ" xfId="1333" xr:uid="{00000000-0005-0000-0000-000034050000}"/>
-    <cellStyle name="_Январь_Апрель_БИНТ_БЕЛ" xfId="1334" xr:uid="{00000000-0005-0000-0000-000035050000}"/>
-    <cellStyle name="_Январь_Апрель_БИНТ_РЕЧ" xfId="1335" xr:uid="{00000000-0005-0000-0000-000036050000}"/>
-    <cellStyle name="_Январь_Апрель_БУХ" xfId="1336" xr:uid="{00000000-0005-0000-0000-000037050000}"/>
-    <cellStyle name="_Январь_Апрель_БУХ_БЕЛ" xfId="1337" xr:uid="{00000000-0005-0000-0000-000038050000}"/>
-    <cellStyle name="_Январь_Апрель_БУХ_РЕЧ" xfId="1338" xr:uid="{00000000-0005-0000-0000-000039050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБДИЗ" xfId="1339" xr:uid="{00000000-0005-0000-0000-00003A050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБДИЗ_БЕЛ" xfId="1340" xr:uid="{00000000-0005-0000-0000-00003B050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБДИЗ_РЕЧ" xfId="1341" xr:uid="{00000000-0005-0000-0000-00003C050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБМАСТ" xfId="1342" xr:uid="{00000000-0005-0000-0000-00003D050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБМАСТ_БЕЛ" xfId="1343" xr:uid="{00000000-0005-0000-0000-00003E050000}"/>
-    <cellStyle name="_Январь_Апрель_ВЕБМАСТ_РЕЧ" xfId="1344" xr:uid="{00000000-0005-0000-0000-00003F050000}"/>
-    <cellStyle name="_Январь_Апрель_ВУЕ" xfId="1345" xr:uid="{00000000-0005-0000-0000-000040050000}"/>
-    <cellStyle name="_Январь_Апрель_ВУЕ_БЕЛ" xfId="1346" xr:uid="{00000000-0005-0000-0000-000041050000}"/>
-    <cellStyle name="_Январь_Апрель_ВУЕ_РЕЧ" xfId="1347" xr:uid="{00000000-0005-0000-0000-000042050000}"/>
-    <cellStyle name="_Январь_Апрель_Дети" xfId="1348" xr:uid="{00000000-0005-0000-0000-000043050000}"/>
-    <cellStyle name="_Январь_Апрель_Дети_БЕЛ" xfId="1349" xr:uid="{00000000-0005-0000-0000-000044050000}"/>
-    <cellStyle name="_Январь_Апрель_Дети_РЕЧ" xfId="1350" xr:uid="{00000000-0005-0000-0000-000045050000}"/>
-    <cellStyle name="_Январь_Апрель_Дистанц." xfId="1351" xr:uid="{00000000-0005-0000-0000-000046050000}"/>
-    <cellStyle name="_Январь_Апрель_Индив." xfId="1352" xr:uid="{00000000-0005-0000-0000-000047050000}"/>
-    <cellStyle name="_Январь_Апрель_Индив._БЕЛ" xfId="1353" xr:uid="{00000000-0005-0000-0000-000048050000}"/>
-    <cellStyle name="_Январь_Апрель_Индив._РЕЧ" xfId="1354" xr:uid="{00000000-0005-0000-0000-000049050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль" xfId="1355" xr:uid="{00000000-0005-0000-0000-00004A050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Август" xfId="1356" xr:uid="{00000000-0005-0000-0000-00004B050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Август_Дистанц." xfId="1357" xr:uid="{00000000-0005-0000-0000-00004C050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Август_Индив." xfId="1358" xr:uid="{00000000-0005-0000-0000-00004D050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_БЕЛ" xfId="1359" xr:uid="{00000000-0005-0000-0000-00004E050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_БИНТ" xfId="1360" xr:uid="{00000000-0005-0000-0000-00004F050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_БИНТ_БЕЛ" xfId="1361" xr:uid="{00000000-0005-0000-0000-000050050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_БИНТ_РЕЧ" xfId="1362" xr:uid="{00000000-0005-0000-0000-000051050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_ВЕБДИЗ" xfId="1363" xr:uid="{00000000-0005-0000-0000-000052050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ" xfId="1364" xr:uid="{00000000-0005-0000-0000-000053050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ_БЕЛ" xfId="1365" xr:uid="{00000000-0005-0000-0000-000054050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ_РЕЧ" xfId="1366" xr:uid="{00000000-0005-0000-0000-000055050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Дети" xfId="1367" xr:uid="{00000000-0005-0000-0000-000056050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Дистанц." xfId="1368" xr:uid="{00000000-0005-0000-0000-000057050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Индив." xfId="1369" xr:uid="{00000000-0005-0000-0000-000058050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Индив._БЕЛ" xfId="1370" xr:uid="{00000000-0005-0000-0000-000059050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Индив._РЕЧ" xfId="1371" xr:uid="{00000000-0005-0000-0000-00005A050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Июнь" xfId="1372" xr:uid="{00000000-0005-0000-0000-00005B050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Июнь_Август" xfId="1373" xr:uid="{00000000-0005-0000-0000-00005C050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Июнь_Дистанц." xfId="1374" xr:uid="{00000000-0005-0000-0000-00005D050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Июнь_Индив." xfId="1375" xr:uid="{00000000-0005-0000-0000-00005E050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_Июнь_КБУ" xfId="1376" xr:uid="{00000000-0005-0000-0000-00005F050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_КБУ" xfId="1377" xr:uid="{00000000-0005-0000-0000-000060050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_КРН" xfId="1378" xr:uid="{00000000-0005-0000-0000-000061050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_ОПШ" xfId="1379" xr:uid="{00000000-0005-0000-0000-000062050000}"/>
-    <cellStyle name="_Январь_Апрель_Июль_СР" xfId="1380" xr:uid="{00000000-0005-0000-0000-000063050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь" xfId="1381" xr:uid="{00000000-0005-0000-0000-000064050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_1" xfId="1382" xr:uid="{00000000-0005-0000-0000-000065050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_1_Август" xfId="1383" xr:uid="{00000000-0005-0000-0000-000066050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_1_Дистанц." xfId="1384" xr:uid="{00000000-0005-0000-0000-000067050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_1_Индив." xfId="1385" xr:uid="{00000000-0005-0000-0000-000068050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_1_КБУ" xfId="1386" xr:uid="{00000000-0005-0000-0000-000069050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Август" xfId="1387" xr:uid="{00000000-0005-0000-0000-00006A050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Август_Дистанц." xfId="1388" xr:uid="{00000000-0005-0000-0000-00006B050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Август_Индив." xfId="1389" xr:uid="{00000000-0005-0000-0000-00006C050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БЕЛ" xfId="1390" xr:uid="{00000000-0005-0000-0000-00006D050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БИНТ" xfId="1391" xr:uid="{00000000-0005-0000-0000-00006E050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БИНТ_БЕЛ" xfId="1392" xr:uid="{00000000-0005-0000-0000-00006F050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БИНТ_РЕЧ" xfId="1393" xr:uid="{00000000-0005-0000-0000-000070050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БУХ" xfId="1394" xr:uid="{00000000-0005-0000-0000-000071050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БУХ_БЕЛ" xfId="1395" xr:uid="{00000000-0005-0000-0000-000072050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_БУХ_РЕЧ" xfId="1396" xr:uid="{00000000-0005-0000-0000-000073050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_ВЕБДИЗ" xfId="1397" xr:uid="{00000000-0005-0000-0000-000074050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ" xfId="1398" xr:uid="{00000000-0005-0000-0000-000075050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ_БЕЛ" xfId="1399" xr:uid="{00000000-0005-0000-0000-000076050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ_РЕЧ" xfId="1400" xr:uid="{00000000-0005-0000-0000-000077050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Дети" xfId="1401" xr:uid="{00000000-0005-0000-0000-000078050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Дистанц." xfId="1402" xr:uid="{00000000-0005-0000-0000-000079050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Индив." xfId="1403" xr:uid="{00000000-0005-0000-0000-00007A050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Индив._БЕЛ" xfId="1404" xr:uid="{00000000-0005-0000-0000-00007B050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Индив._РЕЧ" xfId="1405" xr:uid="{00000000-0005-0000-0000-00007C050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Июнь" xfId="1406" xr:uid="{00000000-0005-0000-0000-00007D050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Август" xfId="1407" xr:uid="{00000000-0005-0000-0000-00007E050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Дистанц." xfId="1408" xr:uid="{00000000-0005-0000-0000-00007F050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Индив." xfId="1409" xr:uid="{00000000-0005-0000-0000-000080050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_Июнь_КБУ" xfId="1410" xr:uid="{00000000-0005-0000-0000-000081050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_КБУ" xfId="1411" xr:uid="{00000000-0005-0000-0000-000082050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_КРН" xfId="1412" xr:uid="{00000000-0005-0000-0000-000083050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_ОПШ" xfId="1413" xr:uid="{00000000-0005-0000-0000-000084050000}"/>
-    <cellStyle name="_Январь_Апрель_Июнь_СР" xfId="1414" xr:uid="{00000000-0005-0000-0000-000085050000}"/>
-    <cellStyle name="_Январь_Апрель_КБУ" xfId="1415" xr:uid="{00000000-0005-0000-0000-000086050000}"/>
-    <cellStyle name="_Январь_Апрель_КБУ_БЕЛ" xfId="1416" xr:uid="{00000000-0005-0000-0000-000087050000}"/>
-    <cellStyle name="_Январь_Апрель_КБУ_РЕЧ" xfId="1417" xr:uid="{00000000-0005-0000-0000-000088050000}"/>
-    <cellStyle name="_Январь_Апрель_КРН" xfId="1418" xr:uid="{00000000-0005-0000-0000-000089050000}"/>
-    <cellStyle name="_Январь_Апрель_Май" xfId="1419" xr:uid="{00000000-0005-0000-0000-00008A050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1" xfId="1420" xr:uid="{00000000-0005-0000-0000-00008B050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Август" xfId="1421" xr:uid="{00000000-0005-0000-0000-00008C050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Август_Дистанц." xfId="1422" xr:uid="{00000000-0005-0000-0000-00008D050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Август_Индив." xfId="1423" xr:uid="{00000000-0005-0000-0000-00008E050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_БЕЛ" xfId="1424" xr:uid="{00000000-0005-0000-0000-00008F050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_БИНТ" xfId="1425" xr:uid="{00000000-0005-0000-0000-000090050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_БИНТ_БЕЛ" xfId="1426" xr:uid="{00000000-0005-0000-0000-000091050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_БИНТ_РЕЧ" xfId="1427" xr:uid="{00000000-0005-0000-0000-000092050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_ВЕБДИЗ" xfId="1428" xr:uid="{00000000-0005-0000-0000-000093050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ" xfId="1429" xr:uid="{00000000-0005-0000-0000-000094050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ_БЕЛ" xfId="1430" xr:uid="{00000000-0005-0000-0000-000095050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ_РЕЧ" xfId="1431" xr:uid="{00000000-0005-0000-0000-000096050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Дети" xfId="1432" xr:uid="{00000000-0005-0000-0000-000097050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Дистанц." xfId="1433" xr:uid="{00000000-0005-0000-0000-000098050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Индив." xfId="1434" xr:uid="{00000000-0005-0000-0000-000099050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Индив._БЕЛ" xfId="1435" xr:uid="{00000000-0005-0000-0000-00009A050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Индив._РЕЧ" xfId="1436" xr:uid="{00000000-0005-0000-0000-00009B050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Июнь" xfId="1437" xr:uid="{00000000-0005-0000-0000-00009C050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Август" xfId="1438" xr:uid="{00000000-0005-0000-0000-00009D050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Дистанц." xfId="1439" xr:uid="{00000000-0005-0000-0000-00009E050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Индив." xfId="1440" xr:uid="{00000000-0005-0000-0000-00009F050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_Июнь_КБУ" xfId="1441" xr:uid="{00000000-0005-0000-0000-0000A0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_КБУ" xfId="1442" xr:uid="{00000000-0005-0000-0000-0000A1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_КРН" xfId="1443" xr:uid="{00000000-0005-0000-0000-0000A2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_ОПШ" xfId="1444" xr:uid="{00000000-0005-0000-0000-0000A3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_1_СР" xfId="1445" xr:uid="{00000000-0005-0000-0000-0000A4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Август" xfId="1446" xr:uid="{00000000-0005-0000-0000-0000A5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Август_Дистанц." xfId="1447" xr:uid="{00000000-0005-0000-0000-0000A6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Август_Индив." xfId="1448" xr:uid="{00000000-0005-0000-0000-0000A7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_АКАД" xfId="1449" xr:uid="{00000000-0005-0000-0000-0000A8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_АКАД_БЕЛ" xfId="1450" xr:uid="{00000000-0005-0000-0000-0000A9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_АКАД_РЕЧ" xfId="1451" xr:uid="{00000000-0005-0000-0000-0000AA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Б9560" xfId="1452" xr:uid="{00000000-0005-0000-0000-0000AB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Б9560_БЕЛ" xfId="1453" xr:uid="{00000000-0005-0000-0000-0000AC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Б9560_РЕЧ" xfId="1454" xr:uid="{00000000-0005-0000-0000-0000AD050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БЕЛ" xfId="1455" xr:uid="{00000000-0005-0000-0000-0000AE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БИНТ" xfId="1456" xr:uid="{00000000-0005-0000-0000-0000AF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БИНТ_БЕЛ" xfId="1457" xr:uid="{00000000-0005-0000-0000-0000B0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БИНТ_РЕЧ" xfId="1458" xr:uid="{00000000-0005-0000-0000-0000B1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БУХ" xfId="1459" xr:uid="{00000000-0005-0000-0000-0000B2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БУХ_БЕЛ" xfId="1460" xr:uid="{00000000-0005-0000-0000-0000B3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_БУХ_РЕЧ" xfId="1461" xr:uid="{00000000-0005-0000-0000-0000B4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_ВЕБДИЗ" xfId="1462" xr:uid="{00000000-0005-0000-0000-0000B5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ" xfId="1463" xr:uid="{00000000-0005-0000-0000-0000B6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ_БЕЛ" xfId="1464" xr:uid="{00000000-0005-0000-0000-0000B7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ_РЕЧ" xfId="1465" xr:uid="{00000000-0005-0000-0000-0000B8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Дети" xfId="1466" xr:uid="{00000000-0005-0000-0000-0000B9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Дистанц." xfId="1467" xr:uid="{00000000-0005-0000-0000-0000BA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Индив." xfId="1468" xr:uid="{00000000-0005-0000-0000-0000BB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Индив._БЕЛ" xfId="1469" xr:uid="{00000000-0005-0000-0000-0000BC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Индив._РЕЧ" xfId="1470" xr:uid="{00000000-0005-0000-0000-0000BD050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль" xfId="1471" xr:uid="{00000000-0005-0000-0000-0000BE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Август" xfId="1472" xr:uid="{00000000-0005-0000-0000-0000BF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Август_Дистанц." xfId="1473" xr:uid="{00000000-0005-0000-0000-0000C0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Август_Индив." xfId="1474" xr:uid="{00000000-0005-0000-0000-0000C1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_БЕЛ" xfId="1475" xr:uid="{00000000-0005-0000-0000-0000C2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ" xfId="1476" xr:uid="{00000000-0005-0000-0000-0000C3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ_БЕЛ" xfId="1477" xr:uid="{00000000-0005-0000-0000-0000C4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ_РЕЧ" xfId="1478" xr:uid="{00000000-0005-0000-0000-0000C5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБДИЗ" xfId="1479" xr:uid="{00000000-0005-0000-0000-0000C6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ" xfId="1480" xr:uid="{00000000-0005-0000-0000-0000C7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="1481" xr:uid="{00000000-0005-0000-0000-0000C8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="1482" xr:uid="{00000000-0005-0000-0000-0000C9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Дети" xfId="1483" xr:uid="{00000000-0005-0000-0000-0000CA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Дистанц." xfId="1484" xr:uid="{00000000-0005-0000-0000-0000CB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Индив." xfId="1485" xr:uid="{00000000-0005-0000-0000-0000CC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Индив._БЕЛ" xfId="1486" xr:uid="{00000000-0005-0000-0000-0000CD050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Индив._РЕЧ" xfId="1487" xr:uid="{00000000-0005-0000-0000-0000CE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь" xfId="1488" xr:uid="{00000000-0005-0000-0000-0000CF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Август" xfId="1489" xr:uid="{00000000-0005-0000-0000-0000D0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Дистанц." xfId="1490" xr:uid="{00000000-0005-0000-0000-0000D1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Индив." xfId="1491" xr:uid="{00000000-0005-0000-0000-0000D2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_КБУ" xfId="1492" xr:uid="{00000000-0005-0000-0000-0000D3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_КБУ" xfId="1493" xr:uid="{00000000-0005-0000-0000-0000D4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_КРН" xfId="1494" xr:uid="{00000000-0005-0000-0000-0000D5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_ОПШ" xfId="1495" xr:uid="{00000000-0005-0000-0000-0000D6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июль_СР" xfId="1496" xr:uid="{00000000-0005-0000-0000-0000D7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь" xfId="1497" xr:uid="{00000000-0005-0000-0000-0000D8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_1" xfId="1498" xr:uid="{00000000-0005-0000-0000-0000D9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Август" xfId="1499" xr:uid="{00000000-0005-0000-0000-0000DA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Дистанц." xfId="1500" xr:uid="{00000000-0005-0000-0000-0000DB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Индив." xfId="1501" xr:uid="{00000000-0005-0000-0000-0000DC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_1_КБУ" xfId="1502" xr:uid="{00000000-0005-0000-0000-0000DD050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Август" xfId="1503" xr:uid="{00000000-0005-0000-0000-0000DE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Август_Дистанц." xfId="1504" xr:uid="{00000000-0005-0000-0000-0000DF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Август_Индив." xfId="1505" xr:uid="{00000000-0005-0000-0000-0000E0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БЕЛ" xfId="1506" xr:uid="{00000000-0005-0000-0000-0000E1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ" xfId="1507" xr:uid="{00000000-0005-0000-0000-0000E2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ_БЕЛ" xfId="1508" xr:uid="{00000000-0005-0000-0000-0000E3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ_РЕЧ" xfId="1509" xr:uid="{00000000-0005-0000-0000-0000E4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ" xfId="1510" xr:uid="{00000000-0005-0000-0000-0000E5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ_БЕЛ" xfId="1511" xr:uid="{00000000-0005-0000-0000-0000E6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ_РЕЧ" xfId="1512" xr:uid="{00000000-0005-0000-0000-0000E7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБДИЗ" xfId="1513" xr:uid="{00000000-0005-0000-0000-0000E8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ" xfId="1514" xr:uid="{00000000-0005-0000-0000-0000E9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="1515" xr:uid="{00000000-0005-0000-0000-0000EA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="1516" xr:uid="{00000000-0005-0000-0000-0000EB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Дети" xfId="1517" xr:uid="{00000000-0005-0000-0000-0000EC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Дистанц." xfId="1518" xr:uid="{00000000-0005-0000-0000-0000ED050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив." xfId="1519" xr:uid="{00000000-0005-0000-0000-0000EE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив._БЕЛ" xfId="1520" xr:uid="{00000000-0005-0000-0000-0000EF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив._РЕЧ" xfId="1521" xr:uid="{00000000-0005-0000-0000-0000F0050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь" xfId="1522" xr:uid="{00000000-0005-0000-0000-0000F1050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Август" xfId="1523" xr:uid="{00000000-0005-0000-0000-0000F2050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Дистанц." xfId="1524" xr:uid="{00000000-0005-0000-0000-0000F3050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Индив." xfId="1525" xr:uid="{00000000-0005-0000-0000-0000F4050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_КБУ" xfId="1526" xr:uid="{00000000-0005-0000-0000-0000F5050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_КБУ" xfId="1527" xr:uid="{00000000-0005-0000-0000-0000F6050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_КРН" xfId="1528" xr:uid="{00000000-0005-0000-0000-0000F7050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_ОПШ" xfId="1529" xr:uid="{00000000-0005-0000-0000-0000F8050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Июнь_СР" xfId="1530" xr:uid="{00000000-0005-0000-0000-0000F9050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_КБУ" xfId="1531" xr:uid="{00000000-0005-0000-0000-0000FA050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_КРН" xfId="1532" xr:uid="{00000000-0005-0000-0000-0000FB050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май" xfId="1533" xr:uid="{00000000-0005-0000-0000-0000FC050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Август" xfId="1534" xr:uid="{00000000-0005-0000-0000-0000FD050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Август_Дистанц." xfId="1535" xr:uid="{00000000-0005-0000-0000-0000FE050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Август_Индив." xfId="1536" xr:uid="{00000000-0005-0000-0000-0000FF050000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_БЕЛ" xfId="1537" xr:uid="{00000000-0005-0000-0000-000000060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ" xfId="1538" xr:uid="{00000000-0005-0000-0000-000001060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ_БЕЛ" xfId="1539" xr:uid="{00000000-0005-0000-0000-000002060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ_РЕЧ" xfId="1540" xr:uid="{00000000-0005-0000-0000-000003060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБДИЗ" xfId="1541" xr:uid="{00000000-0005-0000-0000-000004060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ" xfId="1542" xr:uid="{00000000-0005-0000-0000-000005060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ_БЕЛ" xfId="1543" xr:uid="{00000000-0005-0000-0000-000006060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ_РЕЧ" xfId="1544" xr:uid="{00000000-0005-0000-0000-000007060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Дети" xfId="1545" xr:uid="{00000000-0005-0000-0000-000008060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Дистанц." xfId="1546" xr:uid="{00000000-0005-0000-0000-000009060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Индив." xfId="1547" xr:uid="{00000000-0005-0000-0000-00000A060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Индив._БЕЛ" xfId="1548" xr:uid="{00000000-0005-0000-0000-00000B060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Индив._РЕЧ" xfId="1549" xr:uid="{00000000-0005-0000-0000-00000C060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Июнь" xfId="1550" xr:uid="{00000000-0005-0000-0000-00000D060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Август" xfId="1551" xr:uid="{00000000-0005-0000-0000-00000E060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Дистанц." xfId="1552" xr:uid="{00000000-0005-0000-0000-00000F060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Индив." xfId="1553" xr:uid="{00000000-0005-0000-0000-000010060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_КБУ" xfId="1554" xr:uid="{00000000-0005-0000-0000-000011060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_КБУ" xfId="1555" xr:uid="{00000000-0005-0000-0000-000012060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_КРН" xfId="1556" xr:uid="{00000000-0005-0000-0000-000013060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_ОПШ" xfId="1557" xr:uid="{00000000-0005-0000-0000-000014060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_Май_СР" xfId="1558" xr:uid="{00000000-0005-0000-0000-000015060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_ОПШ" xfId="1559" xr:uid="{00000000-0005-0000-0000-000016060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_РЕЧ" xfId="1560" xr:uid="{00000000-0005-0000-0000-000017060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_РЕЧ_БЕЛ" xfId="1561" xr:uid="{00000000-0005-0000-0000-000018060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_РЕЧ_РЕЧ" xfId="1562" xr:uid="{00000000-0005-0000-0000-000019060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СИ" xfId="1563" xr:uid="{00000000-0005-0000-0000-00001A060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СИ_БЕЛ" xfId="1564" xr:uid="{00000000-0005-0000-0000-00001B060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СИ_РЕЧ" xfId="1565" xr:uid="{00000000-0005-0000-0000-00001C060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СР" xfId="1566" xr:uid="{00000000-0005-0000-0000-00001D060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СУБД" xfId="1567" xr:uid="{00000000-0005-0000-0000-00001E060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СУБД_БЕЛ" xfId="1568" xr:uid="{00000000-0005-0000-0000-00001F060000}"/>
-    <cellStyle name="_Январь_Апрель_Май_СУБД_РЕЧ" xfId="1569" xr:uid="{00000000-0005-0000-0000-000020060000}"/>
-    <cellStyle name="_Январь_Апрель_НТ" xfId="1570" xr:uid="{00000000-0005-0000-0000-000021060000}"/>
-    <cellStyle name="_Январь_Апрель_НТ_БЕЛ" xfId="1571" xr:uid="{00000000-0005-0000-0000-000022060000}"/>
-    <cellStyle name="_Январь_Апрель_НТ_РЕЧ" xfId="1572" xr:uid="{00000000-0005-0000-0000-000023060000}"/>
-    <cellStyle name="_Январь_Апрель_ОПШ" xfId="1573" xr:uid="{00000000-0005-0000-0000-000024060000}"/>
-    <cellStyle name="_Январь_Апрель_Офис" xfId="1574" xr:uid="{00000000-0005-0000-0000-000025060000}"/>
-    <cellStyle name="_Январь_Апрель_Офис_БЕЛ" xfId="1575" xr:uid="{00000000-0005-0000-0000-000026060000}"/>
-    <cellStyle name="_Январь_Апрель_Офис_РЕЧ" xfId="1576" xr:uid="{00000000-0005-0000-0000-000027060000}"/>
-    <cellStyle name="_Январь_Апрель_РЕЧ" xfId="1577" xr:uid="{00000000-0005-0000-0000-000028060000}"/>
-    <cellStyle name="_Январь_Апрель_РЕЧ_БЕЛ" xfId="1578" xr:uid="{00000000-0005-0000-0000-000029060000}"/>
-    <cellStyle name="_Январь_Апрель_РЕЧ_РЕЧ" xfId="1579" xr:uid="{00000000-0005-0000-0000-00002A060000}"/>
-    <cellStyle name="_Январь_Апрель_СИ" xfId="1580" xr:uid="{00000000-0005-0000-0000-00002B060000}"/>
-    <cellStyle name="_Январь_Апрель_СИ_БЕЛ" xfId="1581" xr:uid="{00000000-0005-0000-0000-00002C060000}"/>
-    <cellStyle name="_Январь_Апрель_СИ_РЕЧ" xfId="1582" xr:uid="{00000000-0005-0000-0000-00002D060000}"/>
-    <cellStyle name="_Январь_Апрель_СИС" xfId="1583" xr:uid="{00000000-0005-0000-0000-00002E060000}"/>
-    <cellStyle name="_Январь_Апрель_СИС_БЕЛ" xfId="1584" xr:uid="{00000000-0005-0000-0000-00002F060000}"/>
-    <cellStyle name="_Январь_Апрель_СИС_РЕЧ" xfId="1585" xr:uid="{00000000-0005-0000-0000-000030060000}"/>
-    <cellStyle name="_Январь_Апрель_СР" xfId="1586" xr:uid="{00000000-0005-0000-0000-000031060000}"/>
-    <cellStyle name="_Январь_Апрель_СУБД" xfId="1587" xr:uid="{00000000-0005-0000-0000-000032060000}"/>
-    <cellStyle name="_Январь_Апрель_СУБД_БЕЛ" xfId="1588" xr:uid="{00000000-0005-0000-0000-000033060000}"/>
-    <cellStyle name="_Январь_Апрель_СУБД_РЕЧ" xfId="1589" xr:uid="{00000000-0005-0000-0000-000034060000}"/>
-    <cellStyle name="_Январь_Апрель_ТЕК" xfId="1590" xr:uid="{00000000-0005-0000-0000-000035060000}"/>
-    <cellStyle name="_Январь_Апрель_ТЕК_БЕЛ" xfId="1591" xr:uid="{00000000-0005-0000-0000-000036060000}"/>
-    <cellStyle name="_Январь_Апрель_ТЕК_РЕЧ" xfId="1592" xr:uid="{00000000-0005-0000-0000-000037060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль" xfId="1593" xr:uid="{00000000-0005-0000-0000-000038060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Август" xfId="1594" xr:uid="{00000000-0005-0000-0000-000039060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Август_Дистанц." xfId="1595" xr:uid="{00000000-0005-0000-0000-00003A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Август_Индив." xfId="1596" xr:uid="{00000000-0005-0000-0000-00003B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_АКАД" xfId="1597" xr:uid="{00000000-0005-0000-0000-00003C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_АКАД_БЕЛ" xfId="1598" xr:uid="{00000000-0005-0000-0000-00003D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_АКАД_РЕЧ" xfId="1599" xr:uid="{00000000-0005-0000-0000-00003E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Б9560" xfId="1600" xr:uid="{00000000-0005-0000-0000-00003F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Б9560_БЕЛ" xfId="1601" xr:uid="{00000000-0005-0000-0000-000040060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Б9560_РЕЧ" xfId="1602" xr:uid="{00000000-0005-0000-0000-000041060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БЕЛ" xfId="1603" xr:uid="{00000000-0005-0000-0000-000042060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БИНТ" xfId="1604" xr:uid="{00000000-0005-0000-0000-000043060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БИНТ_БЕЛ" xfId="1605" xr:uid="{00000000-0005-0000-0000-000044060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БИНТ_РЕЧ" xfId="1606" xr:uid="{00000000-0005-0000-0000-000045060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БУХ" xfId="1607" xr:uid="{00000000-0005-0000-0000-000046060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БУХ_БЕЛ" xfId="1608" xr:uid="{00000000-0005-0000-0000-000047060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_БУХ_РЕЧ" xfId="1609" xr:uid="{00000000-0005-0000-0000-000048060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_ВЕБДИЗ" xfId="1610" xr:uid="{00000000-0005-0000-0000-000049060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ" xfId="1611" xr:uid="{00000000-0005-0000-0000-00004A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ_БЕЛ" xfId="1612" xr:uid="{00000000-0005-0000-0000-00004B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ_РЕЧ" xfId="1613" xr:uid="{00000000-0005-0000-0000-00004C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Дети" xfId="1614" xr:uid="{00000000-0005-0000-0000-00004D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Дистанц." xfId="1615" xr:uid="{00000000-0005-0000-0000-00004E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Индив." xfId="1616" xr:uid="{00000000-0005-0000-0000-00004F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Индив._БЕЛ" xfId="1617" xr:uid="{00000000-0005-0000-0000-000050060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Индив._РЕЧ" xfId="1618" xr:uid="{00000000-0005-0000-0000-000051060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль" xfId="1619" xr:uid="{00000000-0005-0000-0000-000052060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август" xfId="1620" xr:uid="{00000000-0005-0000-0000-000053060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август_Дистанц." xfId="1621" xr:uid="{00000000-0005-0000-0000-000054060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август_Индив." xfId="1622" xr:uid="{00000000-0005-0000-0000-000055060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_БЕЛ" xfId="1623" xr:uid="{00000000-0005-0000-0000-000056060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ" xfId="1624" xr:uid="{00000000-0005-0000-0000-000057060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ_БЕЛ" xfId="1625" xr:uid="{00000000-0005-0000-0000-000058060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ_РЕЧ" xfId="1626" xr:uid="{00000000-0005-0000-0000-000059060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБДИЗ" xfId="1627" xr:uid="{00000000-0005-0000-0000-00005A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ" xfId="1628" xr:uid="{00000000-0005-0000-0000-00005B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1629" xr:uid="{00000000-0005-0000-0000-00005C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1630" xr:uid="{00000000-0005-0000-0000-00005D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Дети" xfId="1631" xr:uid="{00000000-0005-0000-0000-00005E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Дистанц." xfId="1632" xr:uid="{00000000-0005-0000-0000-00005F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив." xfId="1633" xr:uid="{00000000-0005-0000-0000-000060060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив._БЕЛ" xfId="1634" xr:uid="{00000000-0005-0000-0000-000061060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив._РЕЧ" xfId="1635" xr:uid="{00000000-0005-0000-0000-000062060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь" xfId="1636" xr:uid="{00000000-0005-0000-0000-000063060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Август" xfId="1637" xr:uid="{00000000-0005-0000-0000-000064060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Дистанц." xfId="1638" xr:uid="{00000000-0005-0000-0000-000065060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Индив." xfId="1639" xr:uid="{00000000-0005-0000-0000-000066060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_КБУ" xfId="1640" xr:uid="{00000000-0005-0000-0000-000067060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_КБУ" xfId="1641" xr:uid="{00000000-0005-0000-0000-000068060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_КРН" xfId="1642" xr:uid="{00000000-0005-0000-0000-000069060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_ОПШ" xfId="1643" xr:uid="{00000000-0005-0000-0000-00006A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июль_СР" xfId="1644" xr:uid="{00000000-0005-0000-0000-00006B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь" xfId="1645" xr:uid="{00000000-0005-0000-0000-00006C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1" xfId="1646" xr:uid="{00000000-0005-0000-0000-00006D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Август" xfId="1647" xr:uid="{00000000-0005-0000-0000-00006E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Дистанц." xfId="1648" xr:uid="{00000000-0005-0000-0000-00006F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Индив." xfId="1649" xr:uid="{00000000-0005-0000-0000-000070060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_КБУ" xfId="1650" xr:uid="{00000000-0005-0000-0000-000071060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август" xfId="1651" xr:uid="{00000000-0005-0000-0000-000072060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август_Дистанц." xfId="1652" xr:uid="{00000000-0005-0000-0000-000073060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август_Индив." xfId="1653" xr:uid="{00000000-0005-0000-0000-000074060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БЕЛ" xfId="1654" xr:uid="{00000000-0005-0000-0000-000075060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ" xfId="1655" xr:uid="{00000000-0005-0000-0000-000076060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ_БЕЛ" xfId="1656" xr:uid="{00000000-0005-0000-0000-000077060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ_РЕЧ" xfId="1657" xr:uid="{00000000-0005-0000-0000-000078060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ" xfId="1658" xr:uid="{00000000-0005-0000-0000-000079060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ_БЕЛ" xfId="1659" xr:uid="{00000000-0005-0000-0000-00007A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ_РЕЧ" xfId="1660" xr:uid="{00000000-0005-0000-0000-00007B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБДИЗ" xfId="1661" xr:uid="{00000000-0005-0000-0000-00007C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ" xfId="1662" xr:uid="{00000000-0005-0000-0000-00007D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1663" xr:uid="{00000000-0005-0000-0000-00007E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1664" xr:uid="{00000000-0005-0000-0000-00007F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Дети" xfId="1665" xr:uid="{00000000-0005-0000-0000-000080060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Дистанц." xfId="1666" xr:uid="{00000000-0005-0000-0000-000081060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив." xfId="1667" xr:uid="{00000000-0005-0000-0000-000082060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив._БЕЛ" xfId="1668" xr:uid="{00000000-0005-0000-0000-000083060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив._РЕЧ" xfId="1669" xr:uid="{00000000-0005-0000-0000-000084060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь" xfId="1670" xr:uid="{00000000-0005-0000-0000-000085060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Август" xfId="1671" xr:uid="{00000000-0005-0000-0000-000086060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Дистанц." xfId="1672" xr:uid="{00000000-0005-0000-0000-000087060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Индив." xfId="1673" xr:uid="{00000000-0005-0000-0000-000088060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_КБУ" xfId="1674" xr:uid="{00000000-0005-0000-0000-000089060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_КБУ" xfId="1675" xr:uid="{00000000-0005-0000-0000-00008A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_КРН" xfId="1676" xr:uid="{00000000-0005-0000-0000-00008B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ОПШ" xfId="1677" xr:uid="{00000000-0005-0000-0000-00008C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Июнь_СР" xfId="1678" xr:uid="{00000000-0005-0000-0000-00008D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_КБУ" xfId="1679" xr:uid="{00000000-0005-0000-0000-00008E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_КРН" xfId="1680" xr:uid="{00000000-0005-0000-0000-00008F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май" xfId="1681" xr:uid="{00000000-0005-0000-0000-000090060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Август" xfId="1682" xr:uid="{00000000-0005-0000-0000-000091060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Август_Дистанц." xfId="1683" xr:uid="{00000000-0005-0000-0000-000092060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Август_Индив." xfId="1684" xr:uid="{00000000-0005-0000-0000-000093060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_БЕЛ" xfId="1685" xr:uid="{00000000-0005-0000-0000-000094060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ" xfId="1686" xr:uid="{00000000-0005-0000-0000-000095060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ_БЕЛ" xfId="1687" xr:uid="{00000000-0005-0000-0000-000096060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ_РЕЧ" xfId="1688" xr:uid="{00000000-0005-0000-0000-000097060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБДИЗ" xfId="1689" xr:uid="{00000000-0005-0000-0000-000098060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ" xfId="1690" xr:uid="{00000000-0005-0000-0000-000099060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1691" xr:uid="{00000000-0005-0000-0000-00009A060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1692" xr:uid="{00000000-0005-0000-0000-00009B060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Дети" xfId="1693" xr:uid="{00000000-0005-0000-0000-00009C060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Дистанц." xfId="1694" xr:uid="{00000000-0005-0000-0000-00009D060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив." xfId="1695" xr:uid="{00000000-0005-0000-0000-00009E060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив._БЕЛ" xfId="1696" xr:uid="{00000000-0005-0000-0000-00009F060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив._РЕЧ" xfId="1697" xr:uid="{00000000-0005-0000-0000-0000A0060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь" xfId="1698" xr:uid="{00000000-0005-0000-0000-0000A1060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Август" xfId="1699" xr:uid="{00000000-0005-0000-0000-0000A2060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Дистанц." xfId="1700" xr:uid="{00000000-0005-0000-0000-0000A3060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Индив." xfId="1701" xr:uid="{00000000-0005-0000-0000-0000A4060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_КБУ" xfId="1702" xr:uid="{00000000-0005-0000-0000-0000A5060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_КБУ" xfId="1703" xr:uid="{00000000-0005-0000-0000-0000A6060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_КРН" xfId="1704" xr:uid="{00000000-0005-0000-0000-0000A7060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_ОПШ" xfId="1705" xr:uid="{00000000-0005-0000-0000-0000A8060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_Май_СР" xfId="1706" xr:uid="{00000000-0005-0000-0000-0000A9060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_ОПШ" xfId="1707" xr:uid="{00000000-0005-0000-0000-0000AA060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ" xfId="1708" xr:uid="{00000000-0005-0000-0000-0000AB060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ_БЕЛ" xfId="1709" xr:uid="{00000000-0005-0000-0000-0000AC060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ_РЕЧ" xfId="1710" xr:uid="{00000000-0005-0000-0000-0000AD060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СИ" xfId="1711" xr:uid="{00000000-0005-0000-0000-0000AE060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СИ_БЕЛ" xfId="1712" xr:uid="{00000000-0005-0000-0000-0000AF060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СИ_РЕЧ" xfId="1713" xr:uid="{00000000-0005-0000-0000-0000B0060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СР" xfId="1714" xr:uid="{00000000-0005-0000-0000-0000B1060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СУБД" xfId="1715" xr:uid="{00000000-0005-0000-0000-0000B2060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СУБД_БЕЛ" xfId="1716" xr:uid="{00000000-0005-0000-0000-0000B3060000}"/>
-    <cellStyle name="_Январь_Апрель_Февраль_СУБД_РЕЧ" xfId="1717" xr:uid="{00000000-0005-0000-0000-0000B4060000}"/>
-    <cellStyle name="_Январь_Апрель_ФШ" xfId="1718" xr:uid="{00000000-0005-0000-0000-0000B5060000}"/>
-    <cellStyle name="_Январь_Апрель_ФШ_БЕЛ" xfId="1719" xr:uid="{00000000-0005-0000-0000-0000B6060000}"/>
-    <cellStyle name="_Январь_Апрель_ФШ_РЕЧ" xfId="1720" xr:uid="{00000000-0005-0000-0000-0000B7060000}"/>
-    <cellStyle name="_Январь_Б9560" xfId="1721" xr:uid="{00000000-0005-0000-0000-0000B8060000}"/>
-    <cellStyle name="_Январь_Б9560_БЕЛ" xfId="1722" xr:uid="{00000000-0005-0000-0000-0000B9060000}"/>
-    <cellStyle name="_Январь_Б9560_РЕЧ" xfId="1723" xr:uid="{00000000-0005-0000-0000-0000BA060000}"/>
-    <cellStyle name="_Январь_БЕЛ" xfId="1724" xr:uid="{00000000-0005-0000-0000-0000BB060000}"/>
-    <cellStyle name="_Январь_БЕЛ_БЕЛ" xfId="1725" xr:uid="{00000000-0005-0000-0000-0000BC060000}"/>
-    <cellStyle name="_Январь_БЕЛ_РЕЧ" xfId="1726" xr:uid="{00000000-0005-0000-0000-0000BD060000}"/>
-    <cellStyle name="_Январь_БИНТ" xfId="1727" xr:uid="{00000000-0005-0000-0000-0000BE060000}"/>
-    <cellStyle name="_Январь_БИНТ_БЕЛ" xfId="1728" xr:uid="{00000000-0005-0000-0000-0000BF060000}"/>
-    <cellStyle name="_Январь_БИНТ_РЕЧ" xfId="1729" xr:uid="{00000000-0005-0000-0000-0000C0060000}"/>
-    <cellStyle name="_Январь_БУХ" xfId="1730" xr:uid="{00000000-0005-0000-0000-0000C1060000}"/>
-    <cellStyle name="_Январь_БУХ_БЕЛ" xfId="1731" xr:uid="{00000000-0005-0000-0000-0000C2060000}"/>
-    <cellStyle name="_Январь_БУХ_РЕЧ" xfId="1732" xr:uid="{00000000-0005-0000-0000-0000C3060000}"/>
-    <cellStyle name="_Январь_ВЕБДИЗ" xfId="1733" xr:uid="{00000000-0005-0000-0000-0000C4060000}"/>
-    <cellStyle name="_Январь_ВЕБДИЗ_БЕЛ" xfId="1734" xr:uid="{00000000-0005-0000-0000-0000C5060000}"/>
-    <cellStyle name="_Январь_ВЕБДИЗ_РЕЧ" xfId="1735" xr:uid="{00000000-0005-0000-0000-0000C6060000}"/>
-    <cellStyle name="_Январь_ВЕБМАСТ" xfId="1736" xr:uid="{00000000-0005-0000-0000-0000C7060000}"/>
-    <cellStyle name="_Январь_ВЕБМАСТ_БЕЛ" xfId="1737" xr:uid="{00000000-0005-0000-0000-0000C8060000}"/>
-    <cellStyle name="_Январь_ВЕБМАСТ_РЕЧ" xfId="1738" xr:uid="{00000000-0005-0000-0000-0000C9060000}"/>
-    <cellStyle name="_Январь_ВУЕ" xfId="1739" xr:uid="{00000000-0005-0000-0000-0000CA060000}"/>
-    <cellStyle name="_Январь_ВУЕ_БЕЛ" xfId="1740" xr:uid="{00000000-0005-0000-0000-0000CB060000}"/>
-    <cellStyle name="_Январь_ВУЕ_РЕЧ" xfId="1741" xr:uid="{00000000-0005-0000-0000-0000CC060000}"/>
-    <cellStyle name="_Январь_Дети" xfId="1742" xr:uid="{00000000-0005-0000-0000-0000CD060000}"/>
-    <cellStyle name="_Январь_Дети_БЕЛ" xfId="1743" xr:uid="{00000000-0005-0000-0000-0000CE060000}"/>
-    <cellStyle name="_Январь_Дети_РЕЧ" xfId="1744" xr:uid="{00000000-0005-0000-0000-0000CF060000}"/>
-    <cellStyle name="_Январь_Дистанц." xfId="1745" xr:uid="{00000000-0005-0000-0000-0000D0060000}"/>
-    <cellStyle name="_Январь_Заявление" xfId="1746" xr:uid="{00000000-0005-0000-0000-0000D1060000}"/>
-    <cellStyle name="_Январь_Заявление_БЕЛ" xfId="1747" xr:uid="{00000000-0005-0000-0000-0000D2060000}"/>
-    <cellStyle name="_Январь_Заявление_РЕЧ" xfId="1748" xr:uid="{00000000-0005-0000-0000-0000D3060000}"/>
-    <cellStyle name="_Январь_Индив." xfId="1749" xr:uid="{00000000-0005-0000-0000-0000D4060000}"/>
-    <cellStyle name="_Январь_Индив._БЕЛ" xfId="1750" xr:uid="{00000000-0005-0000-0000-0000D5060000}"/>
-    <cellStyle name="_Январь_Индив._РЕЧ" xfId="1751" xr:uid="{00000000-0005-0000-0000-0000D6060000}"/>
-    <cellStyle name="_Январь_ИНТ" xfId="1752" xr:uid="{00000000-0005-0000-0000-0000D7060000}"/>
-    <cellStyle name="_Январь_ИНТ_БЕЛ" xfId="1753" xr:uid="{00000000-0005-0000-0000-0000D8060000}"/>
-    <cellStyle name="_Январь_ИНТ_РЕЧ" xfId="1754" xr:uid="{00000000-0005-0000-0000-0000D9060000}"/>
-    <cellStyle name="_Январь_Июль" xfId="1755" xr:uid="{00000000-0005-0000-0000-0000DA060000}"/>
-    <cellStyle name="_Январь_Июль_Август" xfId="1756" xr:uid="{00000000-0005-0000-0000-0000DB060000}"/>
-    <cellStyle name="_Январь_Июль_Август_Дистанц." xfId="1757" xr:uid="{00000000-0005-0000-0000-0000DC060000}"/>
-    <cellStyle name="_Январь_Июль_Август_Индив." xfId="1758" xr:uid="{00000000-0005-0000-0000-0000DD060000}"/>
-    <cellStyle name="_Январь_Июль_БЕЛ" xfId="1759" xr:uid="{00000000-0005-0000-0000-0000DE060000}"/>
-    <cellStyle name="_Январь_Июль_БИНТ" xfId="1760" xr:uid="{00000000-0005-0000-0000-0000DF060000}"/>
-    <cellStyle name="_Январь_Июль_БИНТ_БЕЛ" xfId="1761" xr:uid="{00000000-0005-0000-0000-0000E0060000}"/>
-    <cellStyle name="_Январь_Июль_БИНТ_РЕЧ" xfId="1762" xr:uid="{00000000-0005-0000-0000-0000E1060000}"/>
-    <cellStyle name="_Январь_Июль_ВЕБДИЗ" xfId="1763" xr:uid="{00000000-0005-0000-0000-0000E2060000}"/>
-    <cellStyle name="_Январь_Июль_ВЕБМАСТ" xfId="1764" xr:uid="{00000000-0005-0000-0000-0000E3060000}"/>
-    <cellStyle name="_Январь_Июль_ВЕБМАСТ_БЕЛ" xfId="1765" xr:uid="{00000000-0005-0000-0000-0000E4060000}"/>
-    <cellStyle name="_Январь_Июль_ВЕБМАСТ_РЕЧ" xfId="1766" xr:uid="{00000000-0005-0000-0000-0000E5060000}"/>
-    <cellStyle name="_Январь_Июль_Дети" xfId="1767" xr:uid="{00000000-0005-0000-0000-0000E6060000}"/>
-    <cellStyle name="_Январь_Июль_Дистанц." xfId="1768" xr:uid="{00000000-0005-0000-0000-0000E7060000}"/>
-    <cellStyle name="_Январь_Июль_Индив." xfId="1769" xr:uid="{00000000-0005-0000-0000-0000E8060000}"/>
-    <cellStyle name="_Январь_Июль_Индив._БЕЛ" xfId="1770" xr:uid="{00000000-0005-0000-0000-0000E9060000}"/>
-    <cellStyle name="_Январь_Июль_Индив._РЕЧ" xfId="1771" xr:uid="{00000000-0005-0000-0000-0000EA060000}"/>
-    <cellStyle name="_Январь_Июль_Июнь" xfId="1772" xr:uid="{00000000-0005-0000-0000-0000EB060000}"/>
-    <cellStyle name="_Январь_Июль_Июнь_Август" xfId="1773" xr:uid="{00000000-0005-0000-0000-0000EC060000}"/>
-    <cellStyle name="_Январь_Июль_Июнь_Дистанц." xfId="1774" xr:uid="{00000000-0005-0000-0000-0000ED060000}"/>
-    <cellStyle name="_Январь_Июль_Июнь_Индив." xfId="1775" xr:uid="{00000000-0005-0000-0000-0000EE060000}"/>
-    <cellStyle name="_Январь_Июль_Июнь_КБУ" xfId="1776" xr:uid="{00000000-0005-0000-0000-0000EF060000}"/>
-    <cellStyle name="_Январь_Июль_КБУ" xfId="1777" xr:uid="{00000000-0005-0000-0000-0000F0060000}"/>
-    <cellStyle name="_Январь_Июль_КРН" xfId="1778" xr:uid="{00000000-0005-0000-0000-0000F1060000}"/>
-    <cellStyle name="_Январь_Июль_ОПШ" xfId="1779" xr:uid="{00000000-0005-0000-0000-0000F2060000}"/>
-    <cellStyle name="_Январь_Июль_СР" xfId="1780" xr:uid="{00000000-0005-0000-0000-0000F3060000}"/>
-    <cellStyle name="_Январь_Июнь" xfId="1781" xr:uid="{00000000-0005-0000-0000-0000F4060000}"/>
-    <cellStyle name="_Январь_Июнь_1" xfId="1782" xr:uid="{00000000-0005-0000-0000-0000F5060000}"/>
-    <cellStyle name="_Январь_Июнь_1_Август" xfId="1783" xr:uid="{00000000-0005-0000-0000-0000F6060000}"/>
-    <cellStyle name="_Январь_Июнь_1_Дистанц." xfId="1784" xr:uid="{00000000-0005-0000-0000-0000F7060000}"/>
-    <cellStyle name="_Январь_Июнь_1_Индив." xfId="1785" xr:uid="{00000000-0005-0000-0000-0000F8060000}"/>
-    <cellStyle name="_Январь_Июнь_1_КБУ" xfId="1786" xr:uid="{00000000-0005-0000-0000-0000F9060000}"/>
-    <cellStyle name="_Январь_Июнь_Август" xfId="1787" xr:uid="{00000000-0005-0000-0000-0000FA060000}"/>
-    <cellStyle name="_Январь_Июнь_Август_Дистанц." xfId="1788" xr:uid="{00000000-0005-0000-0000-0000FB060000}"/>
-    <cellStyle name="_Январь_Июнь_Август_Индив." xfId="1789" xr:uid="{00000000-0005-0000-0000-0000FC060000}"/>
-    <cellStyle name="_Январь_Июнь_БЕЛ" xfId="1790" xr:uid="{00000000-0005-0000-0000-0000FD060000}"/>
-    <cellStyle name="_Январь_Июнь_БИНТ" xfId="1791" xr:uid="{00000000-0005-0000-0000-0000FE060000}"/>
-    <cellStyle name="_Январь_Июнь_БИНТ_БЕЛ" xfId="1792" xr:uid="{00000000-0005-0000-0000-0000FF060000}"/>
-    <cellStyle name="_Январь_Июнь_БИНТ_РЕЧ" xfId="1793" xr:uid="{00000000-0005-0000-0000-000000070000}"/>
-    <cellStyle name="_Январь_Июнь_БУХ" xfId="1794" xr:uid="{00000000-0005-0000-0000-000001070000}"/>
-    <cellStyle name="_Январь_Июнь_БУХ_БЕЛ" xfId="1795" xr:uid="{00000000-0005-0000-0000-000002070000}"/>
-    <cellStyle name="_Январь_Июнь_БУХ_РЕЧ" xfId="1796" xr:uid="{00000000-0005-0000-0000-000003070000}"/>
-    <cellStyle name="_Январь_Июнь_ВЕБДИЗ" xfId="1797" xr:uid="{00000000-0005-0000-0000-000004070000}"/>
-    <cellStyle name="_Январь_Июнь_ВЕБМАСТ" xfId="1798" xr:uid="{00000000-0005-0000-0000-000005070000}"/>
-    <cellStyle name="_Январь_Июнь_ВЕБМАСТ_БЕЛ" xfId="1799" xr:uid="{00000000-0005-0000-0000-000006070000}"/>
-    <cellStyle name="_Январь_Июнь_ВЕБМАСТ_РЕЧ" xfId="1800" xr:uid="{00000000-0005-0000-0000-000007070000}"/>
-    <cellStyle name="_Январь_Июнь_Дети" xfId="1801" xr:uid="{00000000-0005-0000-0000-000008070000}"/>
-    <cellStyle name="_Январь_Июнь_Дистанц." xfId="1802" xr:uid="{00000000-0005-0000-0000-000009070000}"/>
-    <cellStyle name="_Январь_Июнь_Индив." xfId="1803" xr:uid="{00000000-0005-0000-0000-00000A070000}"/>
-    <cellStyle name="_Январь_Июнь_Индив._БЕЛ" xfId="1804" xr:uid="{00000000-0005-0000-0000-00000B070000}"/>
-    <cellStyle name="_Январь_Июнь_Индив._РЕЧ" xfId="1805" xr:uid="{00000000-0005-0000-0000-00000C070000}"/>
-    <cellStyle name="_Январь_Июнь_Июнь" xfId="1806" xr:uid="{00000000-0005-0000-0000-00000D070000}"/>
-    <cellStyle name="_Январь_Июнь_Июнь_Август" xfId="1807" xr:uid="{00000000-0005-0000-0000-00000E070000}"/>
-    <cellStyle name="_Январь_Июнь_Июнь_Дистанц." xfId="1808" xr:uid="{00000000-0005-0000-0000-00000F070000}"/>
-    <cellStyle name="_Январь_Июнь_Июнь_Индив." xfId="1809" xr:uid="{00000000-0005-0000-0000-000010070000}"/>
-    <cellStyle name="_Январь_Июнь_Июнь_КБУ" xfId="1810" xr:uid="{00000000-0005-0000-0000-000011070000}"/>
-    <cellStyle name="_Январь_Июнь_КБУ" xfId="1811" xr:uid="{00000000-0005-0000-0000-000012070000}"/>
-    <cellStyle name="_Январь_Июнь_КРН" xfId="1812" xr:uid="{00000000-0005-0000-0000-000013070000}"/>
-    <cellStyle name="_Январь_Июнь_ОПШ" xfId="1813" xr:uid="{00000000-0005-0000-0000-000014070000}"/>
-    <cellStyle name="_Январь_Июнь_СР" xfId="1814" xr:uid="{00000000-0005-0000-0000-000015070000}"/>
-    <cellStyle name="_Январь_КБУ" xfId="1815" xr:uid="{00000000-0005-0000-0000-000016070000}"/>
-    <cellStyle name="_Январь_КБУ_БЕЛ" xfId="1816" xr:uid="{00000000-0005-0000-0000-000017070000}"/>
-    <cellStyle name="_Январь_КБУ_РЕЧ" xfId="1817" xr:uid="{00000000-0005-0000-0000-000018070000}"/>
-    <cellStyle name="_Январь_Консультация" xfId="1818" xr:uid="{00000000-0005-0000-0000-000019070000}"/>
-    <cellStyle name="_Январь_Консультация_БЕЛ" xfId="1819" xr:uid="{00000000-0005-0000-0000-00001A070000}"/>
-    <cellStyle name="_Январь_Консультация_РЕЧ" xfId="1820" xr:uid="{00000000-0005-0000-0000-00001B070000}"/>
-    <cellStyle name="_Январь_КРН" xfId="1821" xr:uid="{00000000-0005-0000-0000-00001C070000}"/>
-    <cellStyle name="_Январь_КРН_БЕЛ" xfId="1822" xr:uid="{00000000-0005-0000-0000-00001D070000}"/>
-    <cellStyle name="_Январь_КРН_РЕЧ" xfId="1823" xr:uid="{00000000-0005-0000-0000-00001E070000}"/>
-    <cellStyle name="_Январь_ЛСХ" xfId="1824" xr:uid="{00000000-0005-0000-0000-00001F070000}"/>
-    <cellStyle name="_Январь_ЛСХ_БЕЛ" xfId="1825" xr:uid="{00000000-0005-0000-0000-000020070000}"/>
-    <cellStyle name="_Январь_ЛСХ_РЕЧ" xfId="1826" xr:uid="{00000000-0005-0000-0000-000021070000}"/>
-    <cellStyle name="_Январь_Май" xfId="1827" xr:uid="{00000000-0005-0000-0000-000022070000}"/>
-    <cellStyle name="_Январь_Май_1" xfId="1828" xr:uid="{00000000-0005-0000-0000-000023070000}"/>
-    <cellStyle name="_Январь_Май_1_Август" xfId="1829" xr:uid="{00000000-0005-0000-0000-000024070000}"/>
-    <cellStyle name="_Январь_Май_1_Август_Дистанц." xfId="1830" xr:uid="{00000000-0005-0000-0000-000025070000}"/>
-    <cellStyle name="_Январь_Май_1_Август_Индив." xfId="1831" xr:uid="{00000000-0005-0000-0000-000026070000}"/>
-    <cellStyle name="_Январь_Май_1_БЕЛ" xfId="1832" xr:uid="{00000000-0005-0000-0000-000027070000}"/>
-    <cellStyle name="_Январь_Май_1_БИНТ" xfId="1833" xr:uid="{00000000-0005-0000-0000-000028070000}"/>
-    <cellStyle name="_Январь_Май_1_БИНТ_БЕЛ" xfId="1834" xr:uid="{00000000-0005-0000-0000-000029070000}"/>
-    <cellStyle name="_Январь_Май_1_БИНТ_РЕЧ" xfId="1835" xr:uid="{00000000-0005-0000-0000-00002A070000}"/>
-    <cellStyle name="_Январь_Май_1_ВЕБДИЗ" xfId="1836" xr:uid="{00000000-0005-0000-0000-00002B070000}"/>
-    <cellStyle name="_Январь_Май_1_ВЕБМАСТ" xfId="1837" xr:uid="{00000000-0005-0000-0000-00002C070000}"/>
-    <cellStyle name="_Январь_Май_1_ВЕБМАСТ_БЕЛ" xfId="1838" xr:uid="{00000000-0005-0000-0000-00002D070000}"/>
-    <cellStyle name="_Январь_Май_1_ВЕБМАСТ_РЕЧ" xfId="1839" xr:uid="{00000000-0005-0000-0000-00002E070000}"/>
-    <cellStyle name="_Январь_Май_1_Дети" xfId="1840" xr:uid="{00000000-0005-0000-0000-00002F070000}"/>
-    <cellStyle name="_Январь_Май_1_Дистанц." xfId="1841" xr:uid="{00000000-0005-0000-0000-000030070000}"/>
-    <cellStyle name="_Январь_Май_1_Индив." xfId="1842" xr:uid="{00000000-0005-0000-0000-000031070000}"/>
-    <cellStyle name="_Январь_Май_1_Индив._БЕЛ" xfId="1843" xr:uid="{00000000-0005-0000-0000-000032070000}"/>
-    <cellStyle name="_Январь_Май_1_Индив._РЕЧ" xfId="1844" xr:uid="{00000000-0005-0000-0000-000033070000}"/>
-    <cellStyle name="_Январь_Май_1_Июнь" xfId="1845" xr:uid="{00000000-0005-0000-0000-000034070000}"/>
-    <cellStyle name="_Январь_Май_1_Июнь_Август" xfId="1846" xr:uid="{00000000-0005-0000-0000-000035070000}"/>
-    <cellStyle name="_Январь_Май_1_Июнь_Дистанц." xfId="1847" xr:uid="{00000000-0005-0000-0000-000036070000}"/>
-    <cellStyle name="_Январь_Май_1_Июнь_Индив." xfId="1848" xr:uid="{00000000-0005-0000-0000-000037070000}"/>
-    <cellStyle name="_Январь_Май_1_Июнь_КБУ" xfId="1849" xr:uid="{00000000-0005-0000-0000-000038070000}"/>
-    <cellStyle name="_Январь_Май_1_КБУ" xfId="1850" xr:uid="{00000000-0005-0000-0000-000039070000}"/>
-    <cellStyle name="_Январь_Май_1_КРН" xfId="1851" xr:uid="{00000000-0005-0000-0000-00003A070000}"/>
-    <cellStyle name="_Январь_Май_1_ОПШ" xfId="1852" xr:uid="{00000000-0005-0000-0000-00003B070000}"/>
-    <cellStyle name="_Январь_Май_1_СР" xfId="1853" xr:uid="{00000000-0005-0000-0000-00003C070000}"/>
-    <cellStyle name="_Январь_Май_Август" xfId="1854" xr:uid="{00000000-0005-0000-0000-00003D070000}"/>
-    <cellStyle name="_Январь_Май_Август_Дистанц." xfId="1855" xr:uid="{00000000-0005-0000-0000-00003E070000}"/>
-    <cellStyle name="_Январь_Май_Август_Индив." xfId="1856" xr:uid="{00000000-0005-0000-0000-00003F070000}"/>
-    <cellStyle name="_Январь_Май_АКАД" xfId="1857" xr:uid="{00000000-0005-0000-0000-000040070000}"/>
-    <cellStyle name="_Январь_Май_АКАД_БЕЛ" xfId="1858" xr:uid="{00000000-0005-0000-0000-000041070000}"/>
-    <cellStyle name="_Январь_Май_АКАД_РЕЧ" xfId="1859" xr:uid="{00000000-0005-0000-0000-000042070000}"/>
-    <cellStyle name="_Январь_Май_Б9560" xfId="1860" xr:uid="{00000000-0005-0000-0000-000043070000}"/>
-    <cellStyle name="_Январь_Май_Б9560_БЕЛ" xfId="1861" xr:uid="{00000000-0005-0000-0000-000044070000}"/>
-    <cellStyle name="_Январь_Май_Б9560_РЕЧ" xfId="1862" xr:uid="{00000000-0005-0000-0000-000045070000}"/>
-    <cellStyle name="_Январь_Май_БЕЛ" xfId="1863" xr:uid="{00000000-0005-0000-0000-000046070000}"/>
-    <cellStyle name="_Январь_Май_БИНТ" xfId="1864" xr:uid="{00000000-0005-0000-0000-000047070000}"/>
-    <cellStyle name="_Январь_Май_БИНТ_БЕЛ" xfId="1865" xr:uid="{00000000-0005-0000-0000-000048070000}"/>
-    <cellStyle name="_Январь_Май_БИНТ_РЕЧ" xfId="1866" xr:uid="{00000000-0005-0000-0000-000049070000}"/>
-    <cellStyle name="_Январь_Май_БУХ" xfId="1867" xr:uid="{00000000-0005-0000-0000-00004A070000}"/>
-    <cellStyle name="_Январь_Май_БУХ_БЕЛ" xfId="1868" xr:uid="{00000000-0005-0000-0000-00004B070000}"/>
-    <cellStyle name="_Январь_Май_БУХ_РЕЧ" xfId="1869" xr:uid="{00000000-0005-0000-0000-00004C070000}"/>
-    <cellStyle name="_Январь_Май_ВЕБДИЗ" xfId="1870" xr:uid="{00000000-0005-0000-0000-00004D070000}"/>
-    <cellStyle name="_Январь_Май_ВЕБМАСТ" xfId="1871" xr:uid="{00000000-0005-0000-0000-00004E070000}"/>
-    <cellStyle name="_Январь_Май_ВЕБМАСТ_БЕЛ" xfId="1872" xr:uid="{00000000-0005-0000-0000-00004F070000}"/>
-    <cellStyle name="_Январь_Май_ВЕБМАСТ_РЕЧ" xfId="1873" xr:uid="{00000000-0005-0000-0000-000050070000}"/>
-    <cellStyle name="_Январь_Май_Дети" xfId="1874" xr:uid="{00000000-0005-0000-0000-000051070000}"/>
-    <cellStyle name="_Январь_Май_Дистанц." xfId="1875" xr:uid="{00000000-0005-0000-0000-000052070000}"/>
-    <cellStyle name="_Январь_Май_Индив." xfId="1876" xr:uid="{00000000-0005-0000-0000-000053070000}"/>
-    <cellStyle name="_Январь_Май_Индив._БЕЛ" xfId="1877" xr:uid="{00000000-0005-0000-0000-000054070000}"/>
-    <cellStyle name="_Январь_Май_Индив._РЕЧ" xfId="1878" xr:uid="{00000000-0005-0000-0000-000055070000}"/>
-    <cellStyle name="_Январь_Май_Июль" xfId="1879" xr:uid="{00000000-0005-0000-0000-000056070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Август" xfId="1880" xr:uid="{00000000-0005-0000-0000-000057070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Август_Дистанц." xfId="1881" xr:uid="{00000000-0005-0000-0000-000058070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Август_Индив." xfId="1882" xr:uid="{00000000-0005-0000-0000-000059070000}"/>
-    <cellStyle name="_Январь_Май_Июль_БЕЛ" xfId="1883" xr:uid="{00000000-0005-0000-0000-00005A070000}"/>
-    <cellStyle name="_Январь_Май_Июль_БИНТ" xfId="1884" xr:uid="{00000000-0005-0000-0000-00005B070000}"/>
-    <cellStyle name="_Январь_Май_Июль_БИНТ_БЕЛ" xfId="1885" xr:uid="{00000000-0005-0000-0000-00005C070000}"/>
-    <cellStyle name="_Январь_Май_Июль_БИНТ_РЕЧ" xfId="1886" xr:uid="{00000000-0005-0000-0000-00005D070000}"/>
-    <cellStyle name="_Январь_Май_Июль_ВЕБДИЗ" xfId="1887" xr:uid="{00000000-0005-0000-0000-00005E070000}"/>
-    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ" xfId="1888" xr:uid="{00000000-0005-0000-0000-00005F070000}"/>
-    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="1889" xr:uid="{00000000-0005-0000-0000-000060070000}"/>
-    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="1890" xr:uid="{00000000-0005-0000-0000-000061070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Дети" xfId="1891" xr:uid="{00000000-0005-0000-0000-000062070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Дистанц." xfId="1892" xr:uid="{00000000-0005-0000-0000-000063070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Индив." xfId="1893" xr:uid="{00000000-0005-0000-0000-000064070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Индив._БЕЛ" xfId="1894" xr:uid="{00000000-0005-0000-0000-000065070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Индив._РЕЧ" xfId="1895" xr:uid="{00000000-0005-0000-0000-000066070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Июнь" xfId="1896" xr:uid="{00000000-0005-0000-0000-000067070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Июнь_Август" xfId="1897" xr:uid="{00000000-0005-0000-0000-000068070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Июнь_Дистанц." xfId="1898" xr:uid="{00000000-0005-0000-0000-000069070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Июнь_Индив." xfId="1899" xr:uid="{00000000-0005-0000-0000-00006A070000}"/>
-    <cellStyle name="_Январь_Май_Июль_Июнь_КБУ" xfId="1900" xr:uid="{00000000-0005-0000-0000-00006B070000}"/>
-    <cellStyle name="_Январь_Май_Июль_КБУ" xfId="1901" xr:uid="{00000000-0005-0000-0000-00006C070000}"/>
-    <cellStyle name="_Январь_Май_Июль_КРН" xfId="1902" xr:uid="{00000000-0005-0000-0000-00006D070000}"/>
-    <cellStyle name="_Январь_Май_Июль_ОПШ" xfId="1903" xr:uid="{00000000-0005-0000-0000-00006E070000}"/>
-    <cellStyle name="_Январь_Май_Июль_СР" xfId="1904" xr:uid="{00000000-0005-0000-0000-00006F070000}"/>
-    <cellStyle name="_Январь_Май_Июнь" xfId="1905" xr:uid="{00000000-0005-0000-0000-000070070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_1" xfId="1906" xr:uid="{00000000-0005-0000-0000-000071070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_1_Август" xfId="1907" xr:uid="{00000000-0005-0000-0000-000072070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_1_Дистанц." xfId="1908" xr:uid="{00000000-0005-0000-0000-000073070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_1_Индив." xfId="1909" xr:uid="{00000000-0005-0000-0000-000074070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_1_КБУ" xfId="1910" xr:uid="{00000000-0005-0000-0000-000075070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Август" xfId="1911" xr:uid="{00000000-0005-0000-0000-000076070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Август_Дистанц." xfId="1912" xr:uid="{00000000-0005-0000-0000-000077070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Август_Индив." xfId="1913" xr:uid="{00000000-0005-0000-0000-000078070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БЕЛ" xfId="1914" xr:uid="{00000000-0005-0000-0000-000079070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БИНТ" xfId="1915" xr:uid="{00000000-0005-0000-0000-00007A070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БИНТ_БЕЛ" xfId="1916" xr:uid="{00000000-0005-0000-0000-00007B070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БИНТ_РЕЧ" xfId="1917" xr:uid="{00000000-0005-0000-0000-00007C070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БУХ" xfId="1918" xr:uid="{00000000-0005-0000-0000-00007D070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БУХ_БЕЛ" xfId="1919" xr:uid="{00000000-0005-0000-0000-00007E070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_БУХ_РЕЧ" xfId="1920" xr:uid="{00000000-0005-0000-0000-00007F070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_ВЕБДИЗ" xfId="1921" xr:uid="{00000000-0005-0000-0000-000080070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ" xfId="1922" xr:uid="{00000000-0005-0000-0000-000081070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="1923" xr:uid="{00000000-0005-0000-0000-000082070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="1924" xr:uid="{00000000-0005-0000-0000-000083070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Дети" xfId="1925" xr:uid="{00000000-0005-0000-0000-000084070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Дистанц." xfId="1926" xr:uid="{00000000-0005-0000-0000-000085070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Индив." xfId="1927" xr:uid="{00000000-0005-0000-0000-000086070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Индив._БЕЛ" xfId="1928" xr:uid="{00000000-0005-0000-0000-000087070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Индив._РЕЧ" xfId="1929" xr:uid="{00000000-0005-0000-0000-000088070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Июнь" xfId="1930" xr:uid="{00000000-0005-0000-0000-000089070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Июнь_Август" xfId="1931" xr:uid="{00000000-0005-0000-0000-00008A070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Июнь_Дистанц." xfId="1932" xr:uid="{00000000-0005-0000-0000-00008B070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Июнь_Индив." xfId="1933" xr:uid="{00000000-0005-0000-0000-00008C070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_Июнь_КБУ" xfId="1934" xr:uid="{00000000-0005-0000-0000-00008D070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_КБУ" xfId="1935" xr:uid="{00000000-0005-0000-0000-00008E070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_КРН" xfId="1936" xr:uid="{00000000-0005-0000-0000-00008F070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_ОПШ" xfId="1937" xr:uid="{00000000-0005-0000-0000-000090070000}"/>
-    <cellStyle name="_Январь_Май_Июнь_СР" xfId="1938" xr:uid="{00000000-0005-0000-0000-000091070000}"/>
-    <cellStyle name="_Январь_Май_КБУ" xfId="1939" xr:uid="{00000000-0005-0000-0000-000092070000}"/>
-    <cellStyle name="_Январь_Май_КРН" xfId="1940" xr:uid="{00000000-0005-0000-0000-000093070000}"/>
-    <cellStyle name="_Январь_Май_Май" xfId="1941" xr:uid="{00000000-0005-0000-0000-000094070000}"/>
-    <cellStyle name="_Январь_Май_Май_Август" xfId="1942" xr:uid="{00000000-0005-0000-0000-000095070000}"/>
-    <cellStyle name="_Январь_Май_Май_Август_Дистанц." xfId="1943" xr:uid="{00000000-0005-0000-0000-000096070000}"/>
-    <cellStyle name="_Январь_Май_Май_Август_Индив." xfId="1944" xr:uid="{00000000-0005-0000-0000-000097070000}"/>
-    <cellStyle name="_Январь_Май_Май_БЕЛ" xfId="1945" xr:uid="{00000000-0005-0000-0000-000098070000}"/>
-    <cellStyle name="_Январь_Май_Май_БИНТ" xfId="1946" xr:uid="{00000000-0005-0000-0000-000099070000}"/>
-    <cellStyle name="_Январь_Май_Май_БИНТ_БЕЛ" xfId="1947" xr:uid="{00000000-0005-0000-0000-00009A070000}"/>
-    <cellStyle name="_Январь_Май_Май_БИНТ_РЕЧ" xfId="1948" xr:uid="{00000000-0005-0000-0000-00009B070000}"/>
-    <cellStyle name="_Январь_Май_Май_ВЕБДИЗ" xfId="1949" xr:uid="{00000000-0005-0000-0000-00009C070000}"/>
-    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ" xfId="1950" xr:uid="{00000000-0005-0000-0000-00009D070000}"/>
-    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ_БЕЛ" xfId="1951" xr:uid="{00000000-0005-0000-0000-00009E070000}"/>
-    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ_РЕЧ" xfId="1952" xr:uid="{00000000-0005-0000-0000-00009F070000}"/>
-    <cellStyle name="_Январь_Май_Май_Дети" xfId="1953" xr:uid="{00000000-0005-0000-0000-0000A0070000}"/>
-    <cellStyle name="_Январь_Май_Май_Дистанц." xfId="1954" xr:uid="{00000000-0005-0000-0000-0000A1070000}"/>
-    <cellStyle name="_Январь_Май_Май_Индив." xfId="1955" xr:uid="{00000000-0005-0000-0000-0000A2070000}"/>
-    <cellStyle name="_Январь_Май_Май_Индив._БЕЛ" xfId="1956" xr:uid="{00000000-0005-0000-0000-0000A3070000}"/>
-    <cellStyle name="_Январь_Май_Май_Индив._РЕЧ" xfId="1957" xr:uid="{00000000-0005-0000-0000-0000A4070000}"/>
-    <cellStyle name="_Январь_Май_Май_Июнь" xfId="1958" xr:uid="{00000000-0005-0000-0000-0000A5070000}"/>
-    <cellStyle name="_Январь_Май_Май_Июнь_Август" xfId="1959" xr:uid="{00000000-0005-0000-0000-0000A6070000}"/>
-    <cellStyle name="_Январь_Май_Май_Июнь_Дистанц." xfId="1960" xr:uid="{00000000-0005-0000-0000-0000A7070000}"/>
-    <cellStyle name="_Январь_Май_Май_Июнь_Индив." xfId="1961" xr:uid="{00000000-0005-0000-0000-0000A8070000}"/>
-    <cellStyle name="_Январь_Май_Май_Июнь_КБУ" xfId="1962" xr:uid="{00000000-0005-0000-0000-0000A9070000}"/>
-    <cellStyle name="_Январь_Май_Май_КБУ" xfId="1963" xr:uid="{00000000-0005-0000-0000-0000AA070000}"/>
-    <cellStyle name="_Январь_Май_Май_КРН" xfId="1964" xr:uid="{00000000-0005-0000-0000-0000AB070000}"/>
-    <cellStyle name="_Январь_Май_Май_ОПШ" xfId="1965" xr:uid="{00000000-0005-0000-0000-0000AC070000}"/>
-    <cellStyle name="_Январь_Май_Май_СР" xfId="1966" xr:uid="{00000000-0005-0000-0000-0000AD070000}"/>
-    <cellStyle name="_Январь_Май_ОПШ" xfId="1967" xr:uid="{00000000-0005-0000-0000-0000AE070000}"/>
-    <cellStyle name="_Январь_Май_РЕЧ" xfId="1968" xr:uid="{00000000-0005-0000-0000-0000AF070000}"/>
-    <cellStyle name="_Январь_Май_РЕЧ_БЕЛ" xfId="1969" xr:uid="{00000000-0005-0000-0000-0000B0070000}"/>
-    <cellStyle name="_Январь_Май_РЕЧ_РЕЧ" xfId="1970" xr:uid="{00000000-0005-0000-0000-0000B1070000}"/>
-    <cellStyle name="_Январь_Май_СИ" xfId="1971" xr:uid="{00000000-0005-0000-0000-0000B2070000}"/>
-    <cellStyle name="_Январь_Май_СИ_БЕЛ" xfId="1972" xr:uid="{00000000-0005-0000-0000-0000B3070000}"/>
-    <cellStyle name="_Январь_Май_СИ_РЕЧ" xfId="1973" xr:uid="{00000000-0005-0000-0000-0000B4070000}"/>
-    <cellStyle name="_Январь_Май_СР" xfId="1974" xr:uid="{00000000-0005-0000-0000-0000B5070000}"/>
-    <cellStyle name="_Январь_Май_СУБД" xfId="1975" xr:uid="{00000000-0005-0000-0000-0000B6070000}"/>
-    <cellStyle name="_Январь_Май_СУБД_БЕЛ" xfId="1976" xr:uid="{00000000-0005-0000-0000-0000B7070000}"/>
-    <cellStyle name="_Январь_Май_СУБД_РЕЧ" xfId="1977" xr:uid="{00000000-0005-0000-0000-0000B8070000}"/>
-    <cellStyle name="_Январь_МП" xfId="1978" xr:uid="{00000000-0005-0000-0000-0000B9070000}"/>
-    <cellStyle name="_Январь_МП_БЕЛ" xfId="1979" xr:uid="{00000000-0005-0000-0000-0000BA070000}"/>
-    <cellStyle name="_Январь_МП_РЕЧ" xfId="1980" xr:uid="{00000000-0005-0000-0000-0000BB070000}"/>
-    <cellStyle name="_Январь_НТ" xfId="1981" xr:uid="{00000000-0005-0000-0000-0000BC070000}"/>
-    <cellStyle name="_Январь_НТ_БЕЛ" xfId="1982" xr:uid="{00000000-0005-0000-0000-0000BD070000}"/>
-    <cellStyle name="_Январь_НТ_РЕЧ" xfId="1983" xr:uid="{00000000-0005-0000-0000-0000BE070000}"/>
-    <cellStyle name="_Январь_ОПШ" xfId="1984" xr:uid="{00000000-0005-0000-0000-0000BF070000}"/>
-    <cellStyle name="_Январь_ОПШ_БЕЛ" xfId="1985" xr:uid="{00000000-0005-0000-0000-0000C0070000}"/>
-    <cellStyle name="_Январь_ОПШ_РЕЧ" xfId="1986" xr:uid="{00000000-0005-0000-0000-0000C1070000}"/>
-    <cellStyle name="_Январь_Офис" xfId="1987" xr:uid="{00000000-0005-0000-0000-0000C2070000}"/>
-    <cellStyle name="_Январь_Офис_БЕЛ" xfId="1988" xr:uid="{00000000-0005-0000-0000-0000C3070000}"/>
-    <cellStyle name="_Январь_Офис_РЕЧ" xfId="1989" xr:uid="{00000000-0005-0000-0000-0000C4070000}"/>
-    <cellStyle name="_Январь_ПРШ" xfId="1990" xr:uid="{00000000-0005-0000-0000-0000C5070000}"/>
-    <cellStyle name="_Январь_ПРШ_БЕЛ" xfId="1991" xr:uid="{00000000-0005-0000-0000-0000C6070000}"/>
-    <cellStyle name="_Январь_ПРШ_РЕЧ" xfId="1992" xr:uid="{00000000-0005-0000-0000-0000C7070000}"/>
-    <cellStyle name="_Январь_РЕЧ" xfId="1993" xr:uid="{00000000-0005-0000-0000-0000C8070000}"/>
-    <cellStyle name="_Январь_РЕЧ_БЕЛ" xfId="1994" xr:uid="{00000000-0005-0000-0000-0000C9070000}"/>
-    <cellStyle name="_Январь_РЕЧ_РЕЧ" xfId="1995" xr:uid="{00000000-0005-0000-0000-0000CA070000}"/>
-    <cellStyle name="_Январь_СВБ" xfId="1996" xr:uid="{00000000-0005-0000-0000-0000CB070000}"/>
-    <cellStyle name="_Январь_СВБ_БЕЛ" xfId="1997" xr:uid="{00000000-0005-0000-0000-0000CC070000}"/>
-    <cellStyle name="_Январь_СВБ_РЕЧ" xfId="1998" xr:uid="{00000000-0005-0000-0000-0000CD070000}"/>
-    <cellStyle name="_Январь_СИ" xfId="1999" xr:uid="{00000000-0005-0000-0000-0000CE070000}"/>
-    <cellStyle name="_Январь_СИ_БЕЛ" xfId="2000" xr:uid="{00000000-0005-0000-0000-0000CF070000}"/>
-    <cellStyle name="_Январь_СИ_РЕЧ" xfId="2001" xr:uid="{00000000-0005-0000-0000-0000D0070000}"/>
-    <cellStyle name="_Январь_СИС" xfId="2002" xr:uid="{00000000-0005-0000-0000-0000D1070000}"/>
-    <cellStyle name="_Январь_СИС_БЕЛ" xfId="2003" xr:uid="{00000000-0005-0000-0000-0000D2070000}"/>
-    <cellStyle name="_Январь_СИС_РЕЧ" xfId="2004" xr:uid="{00000000-0005-0000-0000-0000D3070000}"/>
-    <cellStyle name="_Январь_СР" xfId="2005" xr:uid="{00000000-0005-0000-0000-0000D4070000}"/>
-    <cellStyle name="_Январь_СУБД" xfId="2006" xr:uid="{00000000-0005-0000-0000-0000D5070000}"/>
-    <cellStyle name="_Январь_СУБД_БЕЛ" xfId="2007" xr:uid="{00000000-0005-0000-0000-0000D6070000}"/>
-    <cellStyle name="_Январь_СУБД_РЕЧ" xfId="2008" xr:uid="{00000000-0005-0000-0000-0000D7070000}"/>
-    <cellStyle name="_Январь_ТЕК" xfId="2009" xr:uid="{00000000-0005-0000-0000-0000D8070000}"/>
-    <cellStyle name="_Январь_ТЕК_БЕЛ" xfId="2010" xr:uid="{00000000-0005-0000-0000-0000D9070000}"/>
-    <cellStyle name="_Январь_ТЕК_РЕЧ" xfId="2011" xr:uid="{00000000-0005-0000-0000-0000DA070000}"/>
-    <cellStyle name="_Январь_ТОР" xfId="2012" xr:uid="{00000000-0005-0000-0000-0000DB070000}"/>
-    <cellStyle name="_Январь_ТОР_БЕЛ" xfId="2013" xr:uid="{00000000-0005-0000-0000-0000DC070000}"/>
-    <cellStyle name="_Январь_ТОР_РЕЧ" xfId="2014" xr:uid="{00000000-0005-0000-0000-0000DD070000}"/>
-    <cellStyle name="_Январь_Февраль" xfId="2015" xr:uid="{00000000-0005-0000-0000-0000DE070000}"/>
-    <cellStyle name="_Январь_Февраль_1" xfId="2016" xr:uid="{00000000-0005-0000-0000-0000DF070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Август" xfId="2017" xr:uid="{00000000-0005-0000-0000-0000E0070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Август_Дистанц." xfId="2018" xr:uid="{00000000-0005-0000-0000-0000E1070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Август_Индив." xfId="2019" xr:uid="{00000000-0005-0000-0000-0000E2070000}"/>
-    <cellStyle name="_Январь_Февраль_1_АКАД" xfId="2020" xr:uid="{00000000-0005-0000-0000-0000E3070000}"/>
-    <cellStyle name="_Январь_Февраль_1_АКАД_БЕЛ" xfId="2021" xr:uid="{00000000-0005-0000-0000-0000E4070000}"/>
-    <cellStyle name="_Январь_Февраль_1_АКАД_РЕЧ" xfId="2022" xr:uid="{00000000-0005-0000-0000-0000E5070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Б9560" xfId="2023" xr:uid="{00000000-0005-0000-0000-0000E6070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Б9560_БЕЛ" xfId="2024" xr:uid="{00000000-0005-0000-0000-0000E7070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Б9560_РЕЧ" xfId="2025" xr:uid="{00000000-0005-0000-0000-0000E8070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БЕЛ" xfId="2026" xr:uid="{00000000-0005-0000-0000-0000E9070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БИНТ" xfId="2027" xr:uid="{00000000-0005-0000-0000-0000EA070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БИНТ_БЕЛ" xfId="2028" xr:uid="{00000000-0005-0000-0000-0000EB070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БИНТ_РЕЧ" xfId="2029" xr:uid="{00000000-0005-0000-0000-0000EC070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БУХ" xfId="2030" xr:uid="{00000000-0005-0000-0000-0000ED070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БУХ_БЕЛ" xfId="2031" xr:uid="{00000000-0005-0000-0000-0000EE070000}"/>
-    <cellStyle name="_Январь_Февраль_1_БУХ_РЕЧ" xfId="2032" xr:uid="{00000000-0005-0000-0000-0000EF070000}"/>
-    <cellStyle name="_Январь_Февраль_1_ВЕБДИЗ" xfId="2033" xr:uid="{00000000-0005-0000-0000-0000F0070000}"/>
-    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ" xfId="2034" xr:uid="{00000000-0005-0000-0000-0000F1070000}"/>
-    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ_БЕЛ" xfId="2035" xr:uid="{00000000-0005-0000-0000-0000F2070000}"/>
-    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ_РЕЧ" xfId="2036" xr:uid="{00000000-0005-0000-0000-0000F3070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Дети" xfId="2037" xr:uid="{00000000-0005-0000-0000-0000F4070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Дистанц." xfId="2038" xr:uid="{00000000-0005-0000-0000-0000F5070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Индив." xfId="2039" xr:uid="{00000000-0005-0000-0000-0000F6070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Индив._БЕЛ" xfId="2040" xr:uid="{00000000-0005-0000-0000-0000F7070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Индив._РЕЧ" xfId="2041" xr:uid="{00000000-0005-0000-0000-0000F8070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль" xfId="2042" xr:uid="{00000000-0005-0000-0000-0000F9070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Август" xfId="2043" xr:uid="{00000000-0005-0000-0000-0000FA070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Август_Дистанц." xfId="2044" xr:uid="{00000000-0005-0000-0000-0000FB070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Август_Индив." xfId="2045" xr:uid="{00000000-0005-0000-0000-0000FC070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_БЕЛ" xfId="2046" xr:uid="{00000000-0005-0000-0000-0000FD070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ" xfId="2047" xr:uid="{00000000-0005-0000-0000-0000FE070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ_БЕЛ" xfId="2048" xr:uid="{00000000-0005-0000-0000-0000FF070000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ_РЕЧ" xfId="2049" xr:uid="{00000000-0005-0000-0000-000000080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБДИЗ" xfId="2050" xr:uid="{00000000-0005-0000-0000-000001080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ" xfId="2051" xr:uid="{00000000-0005-0000-0000-000002080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ_БЕЛ" xfId="2052" xr:uid="{00000000-0005-0000-0000-000003080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ_РЕЧ" xfId="2053" xr:uid="{00000000-0005-0000-0000-000004080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Дети" xfId="2054" xr:uid="{00000000-0005-0000-0000-000005080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Дистанц." xfId="2055" xr:uid="{00000000-0005-0000-0000-000006080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Индив." xfId="2056" xr:uid="{00000000-0005-0000-0000-000007080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Индив._БЕЛ" xfId="2057" xr:uid="{00000000-0005-0000-0000-000008080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Индив._РЕЧ" xfId="2058" xr:uid="{00000000-0005-0000-0000-000009080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Июнь" xfId="2059" xr:uid="{00000000-0005-0000-0000-00000A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Август" xfId="2060" xr:uid="{00000000-0005-0000-0000-00000B080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Дистанц." xfId="2061" xr:uid="{00000000-0005-0000-0000-00000C080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Индив." xfId="2062" xr:uid="{00000000-0005-0000-0000-00000D080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_КБУ" xfId="2063" xr:uid="{00000000-0005-0000-0000-00000E080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_КБУ" xfId="2064" xr:uid="{00000000-0005-0000-0000-00000F080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_КРН" xfId="2065" xr:uid="{00000000-0005-0000-0000-000010080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_ОПШ" xfId="2066" xr:uid="{00000000-0005-0000-0000-000011080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июль_СР" xfId="2067" xr:uid="{00000000-0005-0000-0000-000012080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь" xfId="2068" xr:uid="{00000000-0005-0000-0000-000013080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_1" xfId="2069" xr:uid="{00000000-0005-0000-0000-000014080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_1_Август" xfId="2070" xr:uid="{00000000-0005-0000-0000-000015080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_1_Дистанц." xfId="2071" xr:uid="{00000000-0005-0000-0000-000016080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_1_Индив." xfId="2072" xr:uid="{00000000-0005-0000-0000-000017080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_1_КБУ" xfId="2073" xr:uid="{00000000-0005-0000-0000-000018080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Август" xfId="2074" xr:uid="{00000000-0005-0000-0000-000019080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Август_Дистанц." xfId="2075" xr:uid="{00000000-0005-0000-0000-00001A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Август_Индив." xfId="2076" xr:uid="{00000000-0005-0000-0000-00001B080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БЕЛ" xfId="2077" xr:uid="{00000000-0005-0000-0000-00001C080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ" xfId="2078" xr:uid="{00000000-0005-0000-0000-00001D080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ_БЕЛ" xfId="2079" xr:uid="{00000000-0005-0000-0000-00001E080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ_РЕЧ" xfId="2080" xr:uid="{00000000-0005-0000-0000-00001F080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ" xfId="2081" xr:uid="{00000000-0005-0000-0000-000020080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ_БЕЛ" xfId="2082" xr:uid="{00000000-0005-0000-0000-000021080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ_РЕЧ" xfId="2083" xr:uid="{00000000-0005-0000-0000-000022080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБДИЗ" xfId="2084" xr:uid="{00000000-0005-0000-0000-000023080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ" xfId="2085" xr:uid="{00000000-0005-0000-0000-000024080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ_БЕЛ" xfId="2086" xr:uid="{00000000-0005-0000-0000-000025080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ_РЕЧ" xfId="2087" xr:uid="{00000000-0005-0000-0000-000026080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Дети" xfId="2088" xr:uid="{00000000-0005-0000-0000-000027080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Дистанц." xfId="2089" xr:uid="{00000000-0005-0000-0000-000028080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Индив." xfId="2090" xr:uid="{00000000-0005-0000-0000-000029080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Индив._БЕЛ" xfId="2091" xr:uid="{00000000-0005-0000-0000-00002A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Индив._РЕЧ" xfId="2092" xr:uid="{00000000-0005-0000-0000-00002B080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь" xfId="2093" xr:uid="{00000000-0005-0000-0000-00002C080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Август" xfId="2094" xr:uid="{00000000-0005-0000-0000-00002D080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Дистанц." xfId="2095" xr:uid="{00000000-0005-0000-0000-00002E080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Индив." xfId="2096" xr:uid="{00000000-0005-0000-0000-00002F080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_КБУ" xfId="2097" xr:uid="{00000000-0005-0000-0000-000030080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_КБУ" xfId="2098" xr:uid="{00000000-0005-0000-0000-000031080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_КРН" xfId="2099" xr:uid="{00000000-0005-0000-0000-000032080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_ОПШ" xfId="2100" xr:uid="{00000000-0005-0000-0000-000033080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Июнь_СР" xfId="2101" xr:uid="{00000000-0005-0000-0000-000034080000}"/>
-    <cellStyle name="_Январь_Февраль_1_КБУ" xfId="2102" xr:uid="{00000000-0005-0000-0000-000035080000}"/>
-    <cellStyle name="_Январь_Февраль_1_КРН" xfId="2103" xr:uid="{00000000-0005-0000-0000-000036080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май" xfId="2104" xr:uid="{00000000-0005-0000-0000-000037080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Август" xfId="2105" xr:uid="{00000000-0005-0000-0000-000038080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Август_Дистанц." xfId="2106" xr:uid="{00000000-0005-0000-0000-000039080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Август_Индив." xfId="2107" xr:uid="{00000000-0005-0000-0000-00003A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_БЕЛ" xfId="2108" xr:uid="{00000000-0005-0000-0000-00003B080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_БИНТ" xfId="2109" xr:uid="{00000000-0005-0000-0000-00003C080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_БИНТ_БЕЛ" xfId="2110" xr:uid="{00000000-0005-0000-0000-00003D080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_БИНТ_РЕЧ" xfId="2111" xr:uid="{00000000-0005-0000-0000-00003E080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_ВЕБДИЗ" xfId="2112" xr:uid="{00000000-0005-0000-0000-00003F080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ" xfId="2113" xr:uid="{00000000-0005-0000-0000-000040080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ_БЕЛ" xfId="2114" xr:uid="{00000000-0005-0000-0000-000041080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ_РЕЧ" xfId="2115" xr:uid="{00000000-0005-0000-0000-000042080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Дети" xfId="2116" xr:uid="{00000000-0005-0000-0000-000043080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Дистанц." xfId="2117" xr:uid="{00000000-0005-0000-0000-000044080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Индив." xfId="2118" xr:uid="{00000000-0005-0000-0000-000045080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Индив._БЕЛ" xfId="2119" xr:uid="{00000000-0005-0000-0000-000046080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Индив._РЕЧ" xfId="2120" xr:uid="{00000000-0005-0000-0000-000047080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Июнь" xfId="2121" xr:uid="{00000000-0005-0000-0000-000048080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Август" xfId="2122" xr:uid="{00000000-0005-0000-0000-000049080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Дистанц." xfId="2123" xr:uid="{00000000-0005-0000-0000-00004A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Индив." xfId="2124" xr:uid="{00000000-0005-0000-0000-00004B080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_Июнь_КБУ" xfId="2125" xr:uid="{00000000-0005-0000-0000-00004C080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_КБУ" xfId="2126" xr:uid="{00000000-0005-0000-0000-00004D080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_КРН" xfId="2127" xr:uid="{00000000-0005-0000-0000-00004E080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_ОПШ" xfId="2128" xr:uid="{00000000-0005-0000-0000-00004F080000}"/>
-    <cellStyle name="_Январь_Февраль_1_Май_СР" xfId="2129" xr:uid="{00000000-0005-0000-0000-000050080000}"/>
-    <cellStyle name="_Январь_Февраль_1_ОПШ" xfId="2130" xr:uid="{00000000-0005-0000-0000-000051080000}"/>
-    <cellStyle name="_Январь_Февраль_1_РЕЧ" xfId="2131" xr:uid="{00000000-0005-0000-0000-000052080000}"/>
-    <cellStyle name="_Январь_Февраль_1_РЕЧ_БЕЛ" xfId="2132" xr:uid="{00000000-0005-0000-0000-000053080000}"/>
-    <cellStyle name="_Январь_Февраль_1_РЕЧ_РЕЧ" xfId="2133" xr:uid="{00000000-0005-0000-0000-000054080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СИ" xfId="2134" xr:uid="{00000000-0005-0000-0000-000055080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СИ_БЕЛ" xfId="2135" xr:uid="{00000000-0005-0000-0000-000056080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СИ_РЕЧ" xfId="2136" xr:uid="{00000000-0005-0000-0000-000057080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СР" xfId="2137" xr:uid="{00000000-0005-0000-0000-000058080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СУБД" xfId="2138" xr:uid="{00000000-0005-0000-0000-000059080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СУБД_БЕЛ" xfId="2139" xr:uid="{00000000-0005-0000-0000-00005A080000}"/>
-    <cellStyle name="_Январь_Февраль_1_СУБД_РЕЧ" xfId="2140" xr:uid="{00000000-0005-0000-0000-00005B080000}"/>
-    <cellStyle name="_Январь_Февраль_БЕЛ" xfId="2141" xr:uid="{00000000-0005-0000-0000-00005C080000}"/>
-    <cellStyle name="_Январь_Февраль_РЕЧ" xfId="2142" xr:uid="{00000000-0005-0000-0000-00005D080000}"/>
-    <cellStyle name="_Январь_ФШ" xfId="2143" xr:uid="{00000000-0005-0000-0000-00005E080000}"/>
-    <cellStyle name="_Январь_ФШ_БЕЛ" xfId="2144" xr:uid="{00000000-0005-0000-0000-00005F080000}"/>
-    <cellStyle name="_Январь_ФШ_РЕЧ" xfId="2145" xr:uid="{00000000-0005-0000-0000-000060080000}"/>
-    <cellStyle name="Currency0" xfId="2146" xr:uid="{00000000-0005-0000-0000-000061080000}"/>
-    <cellStyle name="Euro" xfId="2147" xr:uid="{00000000-0005-0000-0000-000062080000}"/>
-    <cellStyle name="Normal1" xfId="2148" xr:uid="{00000000-0005-0000-0000-000063080000}"/>
-    <cellStyle name="Акцент1 2" xfId="2161" xr:uid="{00000000-0005-0000-0000-000064080000}"/>
-    <cellStyle name="Денежный [0] 2" xfId="2153" xr:uid="{00000000-0005-0000-0000-000065080000}"/>
-    <cellStyle name="Денежный 2" xfId="2154" xr:uid="{00000000-0005-0000-0000-000066080000}"/>
-    <cellStyle name="Денежный 2 2" xfId="2167" xr:uid="{00000000-0005-0000-0000-000067080000}"/>
+    <cellStyle name="_3ДМ" xfId="1"/>
+    <cellStyle name="_3ДМ_БЕЛ" xfId="2"/>
+    <cellStyle name="_3ДМ_РЕЧ" xfId="3"/>
+    <cellStyle name="_PRICE" xfId="4"/>
+    <cellStyle name="_Август" xfId="5"/>
+    <cellStyle name="_Август_Дистанц." xfId="6"/>
+    <cellStyle name="_Август_Индив." xfId="7"/>
+    <cellStyle name="_АКАД" xfId="8"/>
+    <cellStyle name="_АКАД_БЕЛ" xfId="9"/>
+    <cellStyle name="_АКАД_РЕЧ" xfId="10"/>
+    <cellStyle name="_Апрель" xfId="11"/>
+    <cellStyle name="_Апрель_3ДМ" xfId="12"/>
+    <cellStyle name="_Апрель_3ДМ_БЕЛ" xfId="13"/>
+    <cellStyle name="_Апрель_3ДМ_РЕЧ" xfId="14"/>
+    <cellStyle name="_Апрель_Август" xfId="15"/>
+    <cellStyle name="_Апрель_Август_Дистанц." xfId="16"/>
+    <cellStyle name="_Апрель_Август_Индив." xfId="17"/>
+    <cellStyle name="_Апрель_АКАД" xfId="18"/>
+    <cellStyle name="_Апрель_АКАД_БЕЛ" xfId="19"/>
+    <cellStyle name="_Апрель_АКАД_РЕЧ" xfId="20"/>
+    <cellStyle name="_Апрель_Б9560" xfId="21"/>
+    <cellStyle name="_Апрель_Б9560_БЕЛ" xfId="22"/>
+    <cellStyle name="_Апрель_Б9560_РЕЧ" xfId="23"/>
+    <cellStyle name="_Апрель_БЕЛ" xfId="24"/>
+    <cellStyle name="_Апрель_БИНТ" xfId="25"/>
+    <cellStyle name="_Апрель_БИНТ_БЕЛ" xfId="26"/>
+    <cellStyle name="_Апрель_БИНТ_РЕЧ" xfId="27"/>
+    <cellStyle name="_Апрель_БУХ" xfId="28"/>
+    <cellStyle name="_Апрель_БУХ_БЕЛ" xfId="29"/>
+    <cellStyle name="_Апрель_БУХ_РЕЧ" xfId="30"/>
+    <cellStyle name="_Апрель_ВЕБДИЗ" xfId="31"/>
+    <cellStyle name="_Апрель_ВЕБДИЗ_БЕЛ" xfId="32"/>
+    <cellStyle name="_Апрель_ВЕБДИЗ_РЕЧ" xfId="33"/>
+    <cellStyle name="_Апрель_ВЕБМАСТ" xfId="34"/>
+    <cellStyle name="_Апрель_ВЕБМАСТ_БЕЛ" xfId="35"/>
+    <cellStyle name="_Апрель_ВЕБМАСТ_РЕЧ" xfId="36"/>
+    <cellStyle name="_Апрель_ВУЕ" xfId="37"/>
+    <cellStyle name="_Апрель_ВУЕ_БЕЛ" xfId="38"/>
+    <cellStyle name="_Апрель_ВУЕ_РЕЧ" xfId="39"/>
+    <cellStyle name="_Апрель_Дети" xfId="40"/>
+    <cellStyle name="_Апрель_Дети_БЕЛ" xfId="41"/>
+    <cellStyle name="_Апрель_Дети_РЕЧ" xfId="42"/>
+    <cellStyle name="_Апрель_Дистанц." xfId="43"/>
+    <cellStyle name="_Апрель_Индив." xfId="44"/>
+    <cellStyle name="_Апрель_Индив._БЕЛ" xfId="45"/>
+    <cellStyle name="_Апрель_Индив._РЕЧ" xfId="46"/>
+    <cellStyle name="_Апрель_Июль" xfId="47"/>
+    <cellStyle name="_Апрель_Июль_Август" xfId="48"/>
+    <cellStyle name="_Апрель_Июль_Август_Дистанц." xfId="49"/>
+    <cellStyle name="_Апрель_Июль_Август_Индив." xfId="50"/>
+    <cellStyle name="_Апрель_Июль_БЕЛ" xfId="51"/>
+    <cellStyle name="_Апрель_Июль_БИНТ" xfId="52"/>
+    <cellStyle name="_Апрель_Июль_БИНТ_БЕЛ" xfId="53"/>
+    <cellStyle name="_Апрель_Июль_БИНТ_РЕЧ" xfId="54"/>
+    <cellStyle name="_Апрель_Июль_ВЕБДИЗ" xfId="55"/>
+    <cellStyle name="_Апрель_Июль_ВЕБМАСТ" xfId="56"/>
+    <cellStyle name="_Апрель_Июль_ВЕБМАСТ_БЕЛ" xfId="57"/>
+    <cellStyle name="_Апрель_Июль_ВЕБМАСТ_РЕЧ" xfId="58"/>
+    <cellStyle name="_Апрель_Июль_Дети" xfId="59"/>
+    <cellStyle name="_Апрель_Июль_Дистанц." xfId="60"/>
+    <cellStyle name="_Апрель_Июль_Индив." xfId="61"/>
+    <cellStyle name="_Апрель_Июль_Индив._БЕЛ" xfId="62"/>
+    <cellStyle name="_Апрель_Июль_Индив._РЕЧ" xfId="63"/>
+    <cellStyle name="_Апрель_Июль_Июнь" xfId="64"/>
+    <cellStyle name="_Апрель_Июль_Июнь_Август" xfId="65"/>
+    <cellStyle name="_Апрель_Июль_Июнь_Дистанц." xfId="66"/>
+    <cellStyle name="_Апрель_Июль_Июнь_Индив." xfId="67"/>
+    <cellStyle name="_Апрель_Июль_Июнь_КБУ" xfId="68"/>
+    <cellStyle name="_Апрель_Июль_Июнь_Май" xfId="69"/>
+    <cellStyle name="_Апрель_Июль_КБУ" xfId="70"/>
+    <cellStyle name="_Апрель_Июль_КРН" xfId="71"/>
+    <cellStyle name="_Апрель_Июль_Май" xfId="72"/>
+    <cellStyle name="_Апрель_Июль_ОПШ" xfId="73"/>
+    <cellStyle name="_Апрель_Июль_СР" xfId="74"/>
+    <cellStyle name="_Апрель_Июнь" xfId="75"/>
+    <cellStyle name="_Апрель_Июнь_1" xfId="76"/>
+    <cellStyle name="_Апрель_Июнь_1_Август" xfId="77"/>
+    <cellStyle name="_Апрель_Июнь_1_Дистанц." xfId="78"/>
+    <cellStyle name="_Апрель_Июнь_1_Индив." xfId="79"/>
+    <cellStyle name="_Апрель_Июнь_1_КБУ" xfId="80"/>
+    <cellStyle name="_Апрель_Июнь_1_Май" xfId="81"/>
+    <cellStyle name="_Апрель_Июнь_Август" xfId="82"/>
+    <cellStyle name="_Апрель_Июнь_Август_Дистанц." xfId="83"/>
+    <cellStyle name="_Апрель_Июнь_Август_Индив." xfId="84"/>
+    <cellStyle name="_Апрель_Июнь_БЕЛ" xfId="85"/>
+    <cellStyle name="_Апрель_Июнь_БИНТ" xfId="86"/>
+    <cellStyle name="_Апрель_Июнь_БИНТ_БЕЛ" xfId="87"/>
+    <cellStyle name="_Апрель_Июнь_БИНТ_РЕЧ" xfId="88"/>
+    <cellStyle name="_Апрель_Июнь_БУХ" xfId="89"/>
+    <cellStyle name="_Апрель_Июнь_БУХ_БЕЛ" xfId="90"/>
+    <cellStyle name="_Апрель_Июнь_БУХ_РЕЧ" xfId="91"/>
+    <cellStyle name="_Апрель_Июнь_ВЕБДИЗ" xfId="92"/>
+    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ" xfId="93"/>
+    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ_БЕЛ" xfId="94"/>
+    <cellStyle name="_Апрель_Июнь_ВЕБМАСТ_РЕЧ" xfId="95"/>
+    <cellStyle name="_Апрель_Июнь_Дети" xfId="96"/>
+    <cellStyle name="_Апрель_Июнь_Дистанц." xfId="97"/>
+    <cellStyle name="_Апрель_Июнь_Индив." xfId="98"/>
+    <cellStyle name="_Апрель_Июнь_Индив._БЕЛ" xfId="99"/>
+    <cellStyle name="_Апрель_Июнь_Индив._РЕЧ" xfId="100"/>
+    <cellStyle name="_Апрель_Июнь_Июнь" xfId="101"/>
+    <cellStyle name="_Апрель_Июнь_Июнь_Август" xfId="102"/>
+    <cellStyle name="_Апрель_Июнь_Июнь_Дистанц." xfId="103"/>
+    <cellStyle name="_Апрель_Июнь_Июнь_Индив." xfId="104"/>
+    <cellStyle name="_Апрель_Июнь_Июнь_КБУ" xfId="105"/>
+    <cellStyle name="_Апрель_Июнь_КБУ" xfId="106"/>
+    <cellStyle name="_Апрель_Июнь_КРН" xfId="107"/>
+    <cellStyle name="_Апрель_Июнь_Май" xfId="108"/>
+    <cellStyle name="_Апрель_Июнь_ОПШ" xfId="109"/>
+    <cellStyle name="_Апрель_Июнь_СР" xfId="110"/>
+    <cellStyle name="_Апрель_КБУ" xfId="111"/>
+    <cellStyle name="_Апрель_КБУ_БЕЛ" xfId="112"/>
+    <cellStyle name="_Апрель_КБУ_РЕЧ" xfId="113"/>
+    <cellStyle name="_Апрель_КРН" xfId="114"/>
+    <cellStyle name="_Апрель_Май" xfId="115"/>
+    <cellStyle name="_Апрель_Май_1" xfId="116"/>
+    <cellStyle name="_Апрель_Май_1_Август" xfId="117"/>
+    <cellStyle name="_Апрель_Май_1_Август_Дистанц." xfId="118"/>
+    <cellStyle name="_Апрель_Май_1_Август_Индив." xfId="119"/>
+    <cellStyle name="_Апрель_Май_1_БЕЛ" xfId="120"/>
+    <cellStyle name="_Апрель_Май_1_БИНТ" xfId="121"/>
+    <cellStyle name="_Апрель_Май_1_БИНТ_БЕЛ" xfId="122"/>
+    <cellStyle name="_Апрель_Май_1_БИНТ_РЕЧ" xfId="123"/>
+    <cellStyle name="_Апрель_Май_1_ВЕБДИЗ" xfId="124"/>
+    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ" xfId="125"/>
+    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ_БЕЛ" xfId="126"/>
+    <cellStyle name="_Апрель_Май_1_ВЕБМАСТ_РЕЧ" xfId="127"/>
+    <cellStyle name="_Апрель_Май_1_Дети" xfId="128"/>
+    <cellStyle name="_Апрель_Май_1_Дистанц." xfId="129"/>
+    <cellStyle name="_Апрель_Май_1_Индив." xfId="130"/>
+    <cellStyle name="_Апрель_Май_1_Индив._БЕЛ" xfId="131"/>
+    <cellStyle name="_Апрель_Май_1_Индив._РЕЧ" xfId="132"/>
+    <cellStyle name="_Апрель_Май_1_Июнь" xfId="133"/>
+    <cellStyle name="_Апрель_Май_1_Июнь_Август" xfId="134"/>
+    <cellStyle name="_Апрель_Май_1_Июнь_Дистанц." xfId="135"/>
+    <cellStyle name="_Апрель_Май_1_Июнь_Индив." xfId="136"/>
+    <cellStyle name="_Апрель_Май_1_Июнь_КБУ" xfId="137"/>
+    <cellStyle name="_Апрель_Май_1_КБУ" xfId="138"/>
+    <cellStyle name="_Апрель_Май_1_КРН" xfId="139"/>
+    <cellStyle name="_Апрель_Май_1_ОПШ" xfId="140"/>
+    <cellStyle name="_Апрель_Май_1_СР" xfId="141"/>
+    <cellStyle name="_Апрель_Май_2" xfId="142"/>
+    <cellStyle name="_Апрель_Май_Август" xfId="143"/>
+    <cellStyle name="_Апрель_Май_Август_Дистанц." xfId="144"/>
+    <cellStyle name="_Апрель_Май_Август_Индив." xfId="145"/>
+    <cellStyle name="_Апрель_Май_АКАД" xfId="146"/>
+    <cellStyle name="_Апрель_Май_АКАД_БЕЛ" xfId="147"/>
+    <cellStyle name="_Апрель_Май_АКАД_РЕЧ" xfId="148"/>
+    <cellStyle name="_Апрель_Май_Б9560" xfId="149"/>
+    <cellStyle name="_Апрель_Май_Б9560_БЕЛ" xfId="150"/>
+    <cellStyle name="_Апрель_Май_Б9560_РЕЧ" xfId="151"/>
+    <cellStyle name="_Апрель_Май_БЕЛ" xfId="152"/>
+    <cellStyle name="_Апрель_Май_БИНТ" xfId="153"/>
+    <cellStyle name="_Апрель_Май_БИНТ_БЕЛ" xfId="154"/>
+    <cellStyle name="_Апрель_Май_БИНТ_РЕЧ" xfId="155"/>
+    <cellStyle name="_Апрель_Май_БУХ" xfId="156"/>
+    <cellStyle name="_Апрель_Май_БУХ_БЕЛ" xfId="157"/>
+    <cellStyle name="_Апрель_Май_БУХ_РЕЧ" xfId="158"/>
+    <cellStyle name="_Апрель_Май_ВЕБДИЗ" xfId="159"/>
+    <cellStyle name="_Апрель_Май_ВЕБМАСТ" xfId="160"/>
+    <cellStyle name="_Апрель_Май_ВЕБМАСТ_БЕЛ" xfId="161"/>
+    <cellStyle name="_Апрель_Май_ВЕБМАСТ_РЕЧ" xfId="162"/>
+    <cellStyle name="_Апрель_Май_Дети" xfId="163"/>
+    <cellStyle name="_Апрель_Май_Дистанц." xfId="164"/>
+    <cellStyle name="_Апрель_Май_Индив." xfId="165"/>
+    <cellStyle name="_Апрель_Май_Индив._БЕЛ" xfId="166"/>
+    <cellStyle name="_Апрель_Май_Индив._РЕЧ" xfId="167"/>
+    <cellStyle name="_Апрель_Май_Июль" xfId="168"/>
+    <cellStyle name="_Апрель_Май_Июль_Август" xfId="169"/>
+    <cellStyle name="_Апрель_Май_Июль_Август_Дистанц." xfId="170"/>
+    <cellStyle name="_Апрель_Май_Июль_Август_Индив." xfId="171"/>
+    <cellStyle name="_Апрель_Май_Июль_БЕЛ" xfId="172"/>
+    <cellStyle name="_Апрель_Май_Июль_БИНТ" xfId="173"/>
+    <cellStyle name="_Апрель_Май_Июль_БИНТ_БЕЛ" xfId="174"/>
+    <cellStyle name="_Апрель_Май_Июль_БИНТ_РЕЧ" xfId="175"/>
+    <cellStyle name="_Апрель_Май_Июль_ВЕБДИЗ" xfId="176"/>
+    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ" xfId="177"/>
+    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="178"/>
+    <cellStyle name="_Апрель_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="179"/>
+    <cellStyle name="_Апрель_Май_Июль_Дети" xfId="180"/>
+    <cellStyle name="_Апрель_Май_Июль_Дистанц." xfId="181"/>
+    <cellStyle name="_Апрель_Май_Июль_Индив." xfId="182"/>
+    <cellStyle name="_Апрель_Май_Июль_Индив._БЕЛ" xfId="183"/>
+    <cellStyle name="_Апрель_Май_Июль_Индив._РЕЧ" xfId="184"/>
+    <cellStyle name="_Апрель_Май_Июль_Июнь" xfId="185"/>
+    <cellStyle name="_Апрель_Май_Июль_Июнь_Август" xfId="186"/>
+    <cellStyle name="_Апрель_Май_Июль_Июнь_Дистанц." xfId="187"/>
+    <cellStyle name="_Апрель_Май_Июль_Июнь_Индив." xfId="188"/>
+    <cellStyle name="_Апрель_Май_Июль_Июнь_КБУ" xfId="189"/>
+    <cellStyle name="_Апрель_Май_Июль_КБУ" xfId="190"/>
+    <cellStyle name="_Апрель_Май_Июль_КРН" xfId="191"/>
+    <cellStyle name="_Апрель_Май_Июль_ОПШ" xfId="192"/>
+    <cellStyle name="_Апрель_Май_Июль_СР" xfId="193"/>
+    <cellStyle name="_Апрель_Май_Июнь" xfId="194"/>
+    <cellStyle name="_Апрель_Май_Июнь_1" xfId="195"/>
+    <cellStyle name="_Апрель_Май_Июнь_1_Август" xfId="196"/>
+    <cellStyle name="_Апрель_Май_Июнь_1_Дистанц." xfId="197"/>
+    <cellStyle name="_Апрель_Май_Июнь_1_Индив." xfId="198"/>
+    <cellStyle name="_Апрель_Май_Июнь_1_КБУ" xfId="199"/>
+    <cellStyle name="_Апрель_Май_Июнь_Август" xfId="200"/>
+    <cellStyle name="_Апрель_Май_Июнь_Август_Дистанц." xfId="201"/>
+    <cellStyle name="_Апрель_Май_Июнь_Август_Индив." xfId="202"/>
+    <cellStyle name="_Апрель_Май_Июнь_БЕЛ" xfId="203"/>
+    <cellStyle name="_Апрель_Май_Июнь_БИНТ" xfId="204"/>
+    <cellStyle name="_Апрель_Май_Июнь_БИНТ_БЕЛ" xfId="205"/>
+    <cellStyle name="_Апрель_Май_Июнь_БИНТ_РЕЧ" xfId="206"/>
+    <cellStyle name="_Апрель_Май_Июнь_БУХ" xfId="207"/>
+    <cellStyle name="_Апрель_Май_Июнь_БУХ_БЕЛ" xfId="208"/>
+    <cellStyle name="_Апрель_Май_Июнь_БУХ_РЕЧ" xfId="209"/>
+    <cellStyle name="_Апрель_Май_Июнь_ВЕБДИЗ" xfId="210"/>
+    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ" xfId="211"/>
+    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="212"/>
+    <cellStyle name="_Апрель_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="213"/>
+    <cellStyle name="_Апрель_Май_Июнь_Дети" xfId="214"/>
+    <cellStyle name="_Апрель_Май_Июнь_Дистанц." xfId="215"/>
+    <cellStyle name="_Апрель_Май_Июнь_Индив." xfId="216"/>
+    <cellStyle name="_Апрель_Май_Июнь_Индив._БЕЛ" xfId="217"/>
+    <cellStyle name="_Апрель_Май_Июнь_Индив._РЕЧ" xfId="218"/>
+    <cellStyle name="_Апрель_Май_Июнь_Июнь" xfId="219"/>
+    <cellStyle name="_Апрель_Май_Июнь_Июнь_Август" xfId="220"/>
+    <cellStyle name="_Апрель_Май_Июнь_Июнь_Дистанц." xfId="221"/>
+    <cellStyle name="_Апрель_Май_Июнь_Июнь_Индив." xfId="222"/>
+    <cellStyle name="_Апрель_Май_Июнь_Июнь_КБУ" xfId="223"/>
+    <cellStyle name="_Апрель_Май_Июнь_КБУ" xfId="224"/>
+    <cellStyle name="_Апрель_Май_Июнь_КРН" xfId="225"/>
+    <cellStyle name="_Апрель_Май_Июнь_ОПШ" xfId="226"/>
+    <cellStyle name="_Апрель_Май_Июнь_СР" xfId="227"/>
+    <cellStyle name="_Апрель_Май_КБУ" xfId="228"/>
+    <cellStyle name="_Апрель_Май_КРН" xfId="229"/>
+    <cellStyle name="_Апрель_Май_Май" xfId="230"/>
+    <cellStyle name="_Апрель_Май_Май_Август" xfId="231"/>
+    <cellStyle name="_Апрель_Май_Май_Август_Дистанц." xfId="232"/>
+    <cellStyle name="_Апрель_Май_Май_Август_Индив." xfId="233"/>
+    <cellStyle name="_Апрель_Май_Май_БЕЛ" xfId="234"/>
+    <cellStyle name="_Апрель_Май_Май_БИНТ" xfId="235"/>
+    <cellStyle name="_Апрель_Май_Май_БИНТ_БЕЛ" xfId="236"/>
+    <cellStyle name="_Апрель_Май_Май_БИНТ_РЕЧ" xfId="237"/>
+    <cellStyle name="_Апрель_Май_Май_ВЕБДИЗ" xfId="238"/>
+    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ" xfId="239"/>
+    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ_БЕЛ" xfId="240"/>
+    <cellStyle name="_Апрель_Май_Май_ВЕБМАСТ_РЕЧ" xfId="241"/>
+    <cellStyle name="_Апрель_Май_Май_Дети" xfId="242"/>
+    <cellStyle name="_Апрель_Май_Май_Дистанц." xfId="243"/>
+    <cellStyle name="_Апрель_Май_Май_Индив." xfId="244"/>
+    <cellStyle name="_Апрель_Май_Май_Индив._БЕЛ" xfId="245"/>
+    <cellStyle name="_Апрель_Май_Май_Индив._РЕЧ" xfId="246"/>
+    <cellStyle name="_Апрель_Май_Май_Июнь" xfId="247"/>
+    <cellStyle name="_Апрель_Май_Май_Июнь_Август" xfId="248"/>
+    <cellStyle name="_Апрель_Май_Май_Июнь_Дистанц." xfId="249"/>
+    <cellStyle name="_Апрель_Май_Май_Июнь_Индив." xfId="250"/>
+    <cellStyle name="_Апрель_Май_Май_Июнь_КБУ" xfId="251"/>
+    <cellStyle name="_Апрель_Май_Май_КБУ" xfId="252"/>
+    <cellStyle name="_Апрель_Май_Май_КРН" xfId="253"/>
+    <cellStyle name="_Апрель_Май_Май_ОПШ" xfId="254"/>
+    <cellStyle name="_Апрель_Май_Май_СР" xfId="255"/>
+    <cellStyle name="_Апрель_Май_ОПШ" xfId="256"/>
+    <cellStyle name="_Апрель_Май_РЕЧ" xfId="257"/>
+    <cellStyle name="_Апрель_Май_РЕЧ_БЕЛ" xfId="258"/>
+    <cellStyle name="_Апрель_Май_РЕЧ_РЕЧ" xfId="259"/>
+    <cellStyle name="_Апрель_Май_СИ" xfId="260"/>
+    <cellStyle name="_Апрель_Май_СИ_БЕЛ" xfId="261"/>
+    <cellStyle name="_Апрель_Май_СИ_РЕЧ" xfId="262"/>
+    <cellStyle name="_Апрель_Май_СР" xfId="263"/>
+    <cellStyle name="_Апрель_Май_СУБД" xfId="264"/>
+    <cellStyle name="_Апрель_Май_СУБД_БЕЛ" xfId="265"/>
+    <cellStyle name="_Апрель_Май_СУБД_РЕЧ" xfId="266"/>
+    <cellStyle name="_Апрель_НТ" xfId="267"/>
+    <cellStyle name="_Апрель_НТ_БЕЛ" xfId="268"/>
+    <cellStyle name="_Апрель_НТ_РЕЧ" xfId="269"/>
+    <cellStyle name="_Апрель_ОПШ" xfId="270"/>
+    <cellStyle name="_Апрель_Офис" xfId="271"/>
+    <cellStyle name="_Апрель_Офис_БЕЛ" xfId="272"/>
+    <cellStyle name="_Апрель_Офис_РЕЧ" xfId="273"/>
+    <cellStyle name="_Апрель_РЕЧ" xfId="274"/>
+    <cellStyle name="_Апрель_РЕЧ_БЕЛ" xfId="275"/>
+    <cellStyle name="_Апрель_РЕЧ_РЕЧ" xfId="276"/>
+    <cellStyle name="_Апрель_СИ" xfId="277"/>
+    <cellStyle name="_Апрель_СИ_БЕЛ" xfId="278"/>
+    <cellStyle name="_Апрель_СИ_РЕЧ" xfId="279"/>
+    <cellStyle name="_Апрель_СИС" xfId="280"/>
+    <cellStyle name="_Апрель_СИС_БЕЛ" xfId="281"/>
+    <cellStyle name="_Апрель_СИС_РЕЧ" xfId="282"/>
+    <cellStyle name="_Апрель_СР" xfId="283"/>
+    <cellStyle name="_Апрель_СУБД" xfId="284"/>
+    <cellStyle name="_Апрель_СУБД_БЕЛ" xfId="285"/>
+    <cellStyle name="_Апрель_СУБД_РЕЧ" xfId="286"/>
+    <cellStyle name="_Апрель_ТЕК" xfId="287"/>
+    <cellStyle name="_Апрель_ТЕК_БЕЛ" xfId="288"/>
+    <cellStyle name="_Апрель_ТЕК_РЕЧ" xfId="289"/>
+    <cellStyle name="_Апрель_Февраль" xfId="290"/>
+    <cellStyle name="_Апрель_Февраль_Август" xfId="291"/>
+    <cellStyle name="_Апрель_Февраль_Август_Дистанц." xfId="292"/>
+    <cellStyle name="_Апрель_Февраль_Август_Индив." xfId="293"/>
+    <cellStyle name="_Апрель_Февраль_АКАД" xfId="294"/>
+    <cellStyle name="_Апрель_Февраль_АКАД_БЕЛ" xfId="295"/>
+    <cellStyle name="_Апрель_Февраль_АКАД_РЕЧ" xfId="296"/>
+    <cellStyle name="_Апрель_Февраль_Б9560" xfId="297"/>
+    <cellStyle name="_Апрель_Февраль_Б9560_БЕЛ" xfId="298"/>
+    <cellStyle name="_Апрель_Февраль_Б9560_РЕЧ" xfId="299"/>
+    <cellStyle name="_Апрель_Февраль_БЕЛ" xfId="300"/>
+    <cellStyle name="_Апрель_Февраль_БИНТ" xfId="301"/>
+    <cellStyle name="_Апрель_Февраль_БИНТ_БЕЛ" xfId="302"/>
+    <cellStyle name="_Апрель_Февраль_БИНТ_РЕЧ" xfId="303"/>
+    <cellStyle name="_Апрель_Февраль_БУХ" xfId="304"/>
+    <cellStyle name="_Апрель_Февраль_БУХ_БЕЛ" xfId="305"/>
+    <cellStyle name="_Апрель_Февраль_БУХ_РЕЧ" xfId="306"/>
+    <cellStyle name="_Апрель_Февраль_ВЕБДИЗ" xfId="307"/>
+    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ" xfId="308"/>
+    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ_БЕЛ" xfId="309"/>
+    <cellStyle name="_Апрель_Февраль_ВЕБМАСТ_РЕЧ" xfId="310"/>
+    <cellStyle name="_Апрель_Февраль_Дети" xfId="311"/>
+    <cellStyle name="_Апрель_Февраль_Дистанц." xfId="312"/>
+    <cellStyle name="_Апрель_Февраль_Индив." xfId="313"/>
+    <cellStyle name="_Апрель_Февраль_Индив._БЕЛ" xfId="314"/>
+    <cellStyle name="_Апрель_Февраль_Индив._РЕЧ" xfId="315"/>
+    <cellStyle name="_Апрель_Февраль_Июль" xfId="316"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Август" xfId="317"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Август_Дистанц." xfId="318"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Август_Индив." xfId="319"/>
+    <cellStyle name="_Апрель_Февраль_Июль_БЕЛ" xfId="320"/>
+    <cellStyle name="_Апрель_Февраль_Июль_БИНТ" xfId="321"/>
+    <cellStyle name="_Апрель_Февраль_Июль_БИНТ_БЕЛ" xfId="322"/>
+    <cellStyle name="_Апрель_Февраль_Июль_БИНТ_РЕЧ" xfId="323"/>
+    <cellStyle name="_Апрель_Февраль_Июль_ВЕБДИЗ" xfId="324"/>
+    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ" xfId="325"/>
+    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="326"/>
+    <cellStyle name="_Апрель_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="327"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Дети" xfId="328"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Дистанц." xfId="329"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Индив." xfId="330"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Индив._БЕЛ" xfId="331"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Индив._РЕЧ" xfId="332"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Июнь" xfId="333"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Август" xfId="334"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Дистанц." xfId="335"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Июнь_Индив." xfId="336"/>
+    <cellStyle name="_Апрель_Февраль_Июль_Июнь_КБУ" xfId="337"/>
+    <cellStyle name="_Апрель_Февраль_Июль_КБУ" xfId="338"/>
+    <cellStyle name="_Апрель_Февраль_Июль_КРН" xfId="339"/>
+    <cellStyle name="_Апрель_Февраль_Июль_ОПШ" xfId="340"/>
+    <cellStyle name="_Апрель_Февраль_Июль_СР" xfId="341"/>
+    <cellStyle name="_Апрель_Февраль_Июнь" xfId="342"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_1" xfId="343"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_1_Август" xfId="344"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_1_Дистанц." xfId="345"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_1_Индив." xfId="346"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_1_КБУ" xfId="347"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Август" xfId="348"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Август_Дистанц." xfId="349"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Август_Индив." xfId="350"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БЕЛ" xfId="351"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ" xfId="352"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ_БЕЛ" xfId="353"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БИНТ_РЕЧ" xfId="354"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БУХ" xfId="355"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БУХ_БЕЛ" xfId="356"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_БУХ_РЕЧ" xfId="357"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБДИЗ" xfId="358"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ" xfId="359"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="360"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="361"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Дети" xfId="362"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Дистанц." xfId="363"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Индив." xfId="364"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Индив._БЕЛ" xfId="365"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Индив._РЕЧ" xfId="366"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Июнь" xfId="367"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Август" xfId="368"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Дистанц." xfId="369"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_Индив." xfId="370"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_Июнь_КБУ" xfId="371"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_КБУ" xfId="372"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_КРН" xfId="373"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_ОПШ" xfId="374"/>
+    <cellStyle name="_Апрель_Февраль_Июнь_СР" xfId="375"/>
+    <cellStyle name="_Апрель_Февраль_КБУ" xfId="376"/>
+    <cellStyle name="_Апрель_Февраль_КРН" xfId="377"/>
+    <cellStyle name="_Апрель_Февраль_Май" xfId="378"/>
+    <cellStyle name="_Апрель_Февраль_Май_Август" xfId="379"/>
+    <cellStyle name="_Апрель_Февраль_Май_Август_Дистанц." xfId="380"/>
+    <cellStyle name="_Апрель_Февраль_Май_Август_Индив." xfId="381"/>
+    <cellStyle name="_Апрель_Февраль_Май_БЕЛ" xfId="382"/>
+    <cellStyle name="_Апрель_Февраль_Май_БИНТ" xfId="383"/>
+    <cellStyle name="_Апрель_Февраль_Май_БИНТ_БЕЛ" xfId="384"/>
+    <cellStyle name="_Апрель_Февраль_Май_БИНТ_РЕЧ" xfId="385"/>
+    <cellStyle name="_Апрель_Февраль_Май_ВЕБДИЗ" xfId="386"/>
+    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ" xfId="387"/>
+    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="388"/>
+    <cellStyle name="_Апрель_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="389"/>
+    <cellStyle name="_Апрель_Февраль_Май_Дети" xfId="390"/>
+    <cellStyle name="_Апрель_Февраль_Май_Дистанц." xfId="391"/>
+    <cellStyle name="_Апрель_Февраль_Май_Индив." xfId="392"/>
+    <cellStyle name="_Апрель_Февраль_Май_Индив._БЕЛ" xfId="393"/>
+    <cellStyle name="_Апрель_Февраль_Май_Индив._РЕЧ" xfId="394"/>
+    <cellStyle name="_Апрель_Февраль_Май_Июнь" xfId="395"/>
+    <cellStyle name="_Апрель_Февраль_Май_Июнь_Август" xfId="396"/>
+    <cellStyle name="_Апрель_Февраль_Май_Июнь_Дистанц." xfId="397"/>
+    <cellStyle name="_Апрель_Февраль_Май_Июнь_Индив." xfId="398"/>
+    <cellStyle name="_Апрель_Февраль_Май_Июнь_КБУ" xfId="399"/>
+    <cellStyle name="_Апрель_Февраль_Май_КБУ" xfId="400"/>
+    <cellStyle name="_Апрель_Февраль_Май_КРН" xfId="401"/>
+    <cellStyle name="_Апрель_Февраль_Май_ОПШ" xfId="402"/>
+    <cellStyle name="_Апрель_Февраль_Май_СР" xfId="403"/>
+    <cellStyle name="_Апрель_Февраль_ОПШ" xfId="404"/>
+    <cellStyle name="_Апрель_Февраль_РЕЧ" xfId="405"/>
+    <cellStyle name="_Апрель_Февраль_РЕЧ_БЕЛ" xfId="406"/>
+    <cellStyle name="_Апрель_Февраль_РЕЧ_РЕЧ" xfId="407"/>
+    <cellStyle name="_Апрель_Февраль_СИ" xfId="408"/>
+    <cellStyle name="_Апрель_Февраль_СИ_БЕЛ" xfId="409"/>
+    <cellStyle name="_Апрель_Февраль_СИ_РЕЧ" xfId="410"/>
+    <cellStyle name="_Апрель_Февраль_СР" xfId="411"/>
+    <cellStyle name="_Апрель_Февраль_СУБД" xfId="412"/>
+    <cellStyle name="_Апрель_Февраль_СУБД_БЕЛ" xfId="413"/>
+    <cellStyle name="_Апрель_Февраль_СУБД_РЕЧ" xfId="414"/>
+    <cellStyle name="_Апрель_ФШ" xfId="415"/>
+    <cellStyle name="_Апрель_ФШ_БЕЛ" xfId="416"/>
+    <cellStyle name="_Апрель_ФШ_РЕЧ" xfId="417"/>
+    <cellStyle name="_Б9560" xfId="418"/>
+    <cellStyle name="_Б9560_БЕЛ" xfId="419"/>
+    <cellStyle name="_Б9560_РЕЧ" xfId="420"/>
+    <cellStyle name="_БЕЛ" xfId="421"/>
+    <cellStyle name="_БЕЛ_БЕЛ" xfId="422"/>
+    <cellStyle name="_БЕЛ_РЕЧ" xfId="423"/>
+    <cellStyle name="_БИНТ" xfId="424"/>
+    <cellStyle name="_БИНТ_БЕЛ" xfId="425"/>
+    <cellStyle name="_БИНТ_РЕЧ" xfId="426"/>
+    <cellStyle name="_БУХ" xfId="427"/>
+    <cellStyle name="_БУХ_БЕЛ" xfId="428"/>
+    <cellStyle name="_БУХ_РЕЧ" xfId="429"/>
+    <cellStyle name="_ВЕБДИЗ" xfId="430"/>
+    <cellStyle name="_ВЕБДИЗ_БЕЛ" xfId="431"/>
+    <cellStyle name="_ВЕБДИЗ_РЕЧ" xfId="432"/>
+    <cellStyle name="_ВЕБМАСТ" xfId="433"/>
+    <cellStyle name="_ВЕБМАСТ_БЕЛ" xfId="434"/>
+    <cellStyle name="_ВЕБМАСТ_РЕЧ" xfId="435"/>
+    <cellStyle name="_ВУЕ" xfId="436"/>
+    <cellStyle name="_ВУЕ_БЕЛ" xfId="437"/>
+    <cellStyle name="_ВУЕ_РЕЧ" xfId="438"/>
+    <cellStyle name="_Дети" xfId="439"/>
+    <cellStyle name="_Дети_БЕЛ" xfId="440"/>
+    <cellStyle name="_Дети_РЕЧ" xfId="441"/>
+    <cellStyle name="_Дистанц." xfId="442"/>
+    <cellStyle name="_ДОГ НУДО частн" xfId="443"/>
+    <cellStyle name="_ДОГ НУДО частн_БЕЛ" xfId="444"/>
+    <cellStyle name="_ДОГ НУДО частн_РЕЧ" xfId="445"/>
+    <cellStyle name="_Заявление" xfId="446"/>
+    <cellStyle name="_Заявление_БЕЛ" xfId="447"/>
+    <cellStyle name="_Заявление_РЕЧ" xfId="448"/>
+    <cellStyle name="_Индив." xfId="449"/>
+    <cellStyle name="_Индив._БЕЛ" xfId="450"/>
+    <cellStyle name="_Индив._РЕЧ" xfId="451"/>
+    <cellStyle name="_ИНТ" xfId="452"/>
+    <cellStyle name="_ИНТ_БЕЛ" xfId="453"/>
+    <cellStyle name="_ИНТ_РЕЧ" xfId="454"/>
+    <cellStyle name="_Июль" xfId="455"/>
+    <cellStyle name="_Июль_Август" xfId="456"/>
+    <cellStyle name="_Июль_Август_Дистанц." xfId="457"/>
+    <cellStyle name="_Июль_Август_Индив." xfId="458"/>
+    <cellStyle name="_Июль_БЕЛ" xfId="459"/>
+    <cellStyle name="_Июль_БИНТ" xfId="460"/>
+    <cellStyle name="_Июль_БИНТ_БЕЛ" xfId="461"/>
+    <cellStyle name="_Июль_БИНТ_РЕЧ" xfId="462"/>
+    <cellStyle name="_Июль_ВЕБДИЗ" xfId="463"/>
+    <cellStyle name="_Июль_ВЕБМАСТ" xfId="464"/>
+    <cellStyle name="_Июль_ВЕБМАСТ_БЕЛ" xfId="465"/>
+    <cellStyle name="_Июль_ВЕБМАСТ_РЕЧ" xfId="466"/>
+    <cellStyle name="_Июль_Дети" xfId="467"/>
+    <cellStyle name="_Июль_Дистанц." xfId="468"/>
+    <cellStyle name="_Июль_Индив." xfId="469"/>
+    <cellStyle name="_Июль_Индив._БЕЛ" xfId="470"/>
+    <cellStyle name="_Июль_Индив._РЕЧ" xfId="471"/>
+    <cellStyle name="_Июль_Июнь" xfId="472"/>
+    <cellStyle name="_Июль_Июнь_Август" xfId="473"/>
+    <cellStyle name="_Июль_Июнь_Дистанц." xfId="474"/>
+    <cellStyle name="_Июль_Июнь_Индив." xfId="475"/>
+    <cellStyle name="_Июль_Июнь_КБУ" xfId="476"/>
+    <cellStyle name="_Июль_КБУ" xfId="477"/>
+    <cellStyle name="_Июль_КРН" xfId="478"/>
+    <cellStyle name="_Июль_ОПШ" xfId="479"/>
+    <cellStyle name="_Июль_СР" xfId="480"/>
+    <cellStyle name="_Июнь" xfId="481"/>
+    <cellStyle name="_Июнь_1" xfId="482"/>
+    <cellStyle name="_Июнь_1_Август" xfId="483"/>
+    <cellStyle name="_Июнь_1_Дистанц." xfId="484"/>
+    <cellStyle name="_Июнь_1_Индив." xfId="485"/>
+    <cellStyle name="_Июнь_1_КБУ" xfId="486"/>
+    <cellStyle name="_Июнь_Август" xfId="487"/>
+    <cellStyle name="_Июнь_Август_Дистанц." xfId="488"/>
+    <cellStyle name="_Июнь_Август_Индив." xfId="489"/>
+    <cellStyle name="_Июнь_БЕЛ" xfId="490"/>
+    <cellStyle name="_Июнь_БИНТ" xfId="491"/>
+    <cellStyle name="_Июнь_БИНТ_БЕЛ" xfId="492"/>
+    <cellStyle name="_Июнь_БИНТ_РЕЧ" xfId="493"/>
+    <cellStyle name="_Июнь_БУХ" xfId="494"/>
+    <cellStyle name="_Июнь_БУХ_БЕЛ" xfId="495"/>
+    <cellStyle name="_Июнь_БУХ_РЕЧ" xfId="496"/>
+    <cellStyle name="_Июнь_ВЕБДИЗ" xfId="497"/>
+    <cellStyle name="_Июнь_ВЕБМАСТ" xfId="498"/>
+    <cellStyle name="_Июнь_ВЕБМАСТ_БЕЛ" xfId="499"/>
+    <cellStyle name="_Июнь_ВЕБМАСТ_РЕЧ" xfId="500"/>
+    <cellStyle name="_Июнь_Дети" xfId="501"/>
+    <cellStyle name="_Июнь_Дистанц." xfId="502"/>
+    <cellStyle name="_Июнь_Индив." xfId="503"/>
+    <cellStyle name="_Июнь_Индив._БЕЛ" xfId="504"/>
+    <cellStyle name="_Июнь_Индив._РЕЧ" xfId="505"/>
+    <cellStyle name="_Июнь_Июнь" xfId="506"/>
+    <cellStyle name="_Июнь_Июнь_Август" xfId="507"/>
+    <cellStyle name="_Июнь_Июнь_Дистанц." xfId="508"/>
+    <cellStyle name="_Июнь_Июнь_Индив." xfId="509"/>
+    <cellStyle name="_Июнь_Июнь_КБУ" xfId="510"/>
+    <cellStyle name="_Июнь_КБУ" xfId="511"/>
+    <cellStyle name="_Июнь_КРН" xfId="512"/>
+    <cellStyle name="_Июнь_ОПШ" xfId="513"/>
+    <cellStyle name="_Июнь_СР" xfId="514"/>
+    <cellStyle name="_КБУ" xfId="515"/>
+    <cellStyle name="_КБУ_БЕЛ" xfId="516"/>
+    <cellStyle name="_КБУ_РЕЧ" xfId="517"/>
+    <cellStyle name="_Консультация" xfId="518"/>
+    <cellStyle name="_Консультация_БЕЛ" xfId="519"/>
+    <cellStyle name="_Консультация_РЕЧ" xfId="520"/>
+    <cellStyle name="_КРН" xfId="521"/>
+    <cellStyle name="_КРН_БЕЛ" xfId="522"/>
+    <cellStyle name="_КРН_РЕЧ" xfId="523"/>
+    <cellStyle name="_Лист1" xfId="524"/>
+    <cellStyle name="_ЛСХ" xfId="525"/>
+    <cellStyle name="_ЛСХ_БЕЛ" xfId="526"/>
+    <cellStyle name="_ЛСХ_РЕЧ" xfId="527"/>
+    <cellStyle name="_Май" xfId="528"/>
+    <cellStyle name="_Май_1" xfId="529"/>
+    <cellStyle name="_Май_1_Август" xfId="530"/>
+    <cellStyle name="_Май_1_Август_Дистанц." xfId="531"/>
+    <cellStyle name="_Май_1_Август_Индив." xfId="532"/>
+    <cellStyle name="_Май_1_БЕЛ" xfId="533"/>
+    <cellStyle name="_Май_1_БИНТ" xfId="534"/>
+    <cellStyle name="_Май_1_БИНТ_БЕЛ" xfId="535"/>
+    <cellStyle name="_Май_1_БИНТ_РЕЧ" xfId="536"/>
+    <cellStyle name="_Май_1_ВЕБДИЗ" xfId="537"/>
+    <cellStyle name="_Май_1_ВЕБМАСТ" xfId="538"/>
+    <cellStyle name="_Май_1_ВЕБМАСТ_БЕЛ" xfId="539"/>
+    <cellStyle name="_Май_1_ВЕБМАСТ_РЕЧ" xfId="540"/>
+    <cellStyle name="_Май_1_Дети" xfId="541"/>
+    <cellStyle name="_Май_1_Дистанц." xfId="542"/>
+    <cellStyle name="_Май_1_Индив." xfId="543"/>
+    <cellStyle name="_Май_1_Индив._БЕЛ" xfId="544"/>
+    <cellStyle name="_Май_1_Индив._РЕЧ" xfId="545"/>
+    <cellStyle name="_Май_1_Июнь" xfId="546"/>
+    <cellStyle name="_Май_1_Июнь_Август" xfId="547"/>
+    <cellStyle name="_Май_1_Июнь_Дистанц." xfId="548"/>
+    <cellStyle name="_Май_1_Июнь_Индив." xfId="549"/>
+    <cellStyle name="_Май_1_Июнь_КБУ" xfId="550"/>
+    <cellStyle name="_Май_1_КБУ" xfId="551"/>
+    <cellStyle name="_Май_1_КРН" xfId="552"/>
+    <cellStyle name="_Май_1_ОПШ" xfId="553"/>
+    <cellStyle name="_Май_1_СР" xfId="554"/>
+    <cellStyle name="_Май_Август" xfId="555"/>
+    <cellStyle name="_Май_Август_Дистанц." xfId="556"/>
+    <cellStyle name="_Май_Август_Индив." xfId="557"/>
+    <cellStyle name="_Май_АКАД" xfId="558"/>
+    <cellStyle name="_Май_АКАД_БЕЛ" xfId="559"/>
+    <cellStyle name="_Май_АКАД_РЕЧ" xfId="560"/>
+    <cellStyle name="_Май_Б9560" xfId="561"/>
+    <cellStyle name="_Май_Б9560_БЕЛ" xfId="562"/>
+    <cellStyle name="_Май_Б9560_РЕЧ" xfId="563"/>
+    <cellStyle name="_Май_БЕЛ" xfId="564"/>
+    <cellStyle name="_Май_БИНТ" xfId="565"/>
+    <cellStyle name="_Май_БИНТ_БЕЛ" xfId="566"/>
+    <cellStyle name="_Май_БИНТ_РЕЧ" xfId="567"/>
+    <cellStyle name="_Май_БУХ" xfId="568"/>
+    <cellStyle name="_Май_БУХ_БЕЛ" xfId="569"/>
+    <cellStyle name="_Май_БУХ_РЕЧ" xfId="570"/>
+    <cellStyle name="_Май_ВЕБДИЗ" xfId="571"/>
+    <cellStyle name="_Май_ВЕБМАСТ" xfId="572"/>
+    <cellStyle name="_Май_ВЕБМАСТ_БЕЛ" xfId="573"/>
+    <cellStyle name="_Май_ВЕБМАСТ_РЕЧ" xfId="574"/>
+    <cellStyle name="_Май_Дети" xfId="575"/>
+    <cellStyle name="_Май_Дистанц." xfId="576"/>
+    <cellStyle name="_Май_Индив." xfId="577"/>
+    <cellStyle name="_Май_Индив._БЕЛ" xfId="578"/>
+    <cellStyle name="_Май_Индив._РЕЧ" xfId="579"/>
+    <cellStyle name="_Май_Июль" xfId="580"/>
+    <cellStyle name="_Май_Июль_Август" xfId="581"/>
+    <cellStyle name="_Май_Июль_Август_Дистанц." xfId="582"/>
+    <cellStyle name="_Май_Июль_Август_Индив." xfId="583"/>
+    <cellStyle name="_Май_Июль_БЕЛ" xfId="584"/>
+    <cellStyle name="_Май_Июль_БИНТ" xfId="585"/>
+    <cellStyle name="_Май_Июль_БИНТ_БЕЛ" xfId="586"/>
+    <cellStyle name="_Май_Июль_БИНТ_РЕЧ" xfId="587"/>
+    <cellStyle name="_Май_Июль_ВЕБДИЗ" xfId="588"/>
+    <cellStyle name="_Май_Июль_ВЕБМАСТ" xfId="589"/>
+    <cellStyle name="_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="590"/>
+    <cellStyle name="_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="591"/>
+    <cellStyle name="_Май_Июль_Дети" xfId="592"/>
+    <cellStyle name="_Май_Июль_Дистанц." xfId="593"/>
+    <cellStyle name="_Май_Июль_Индив." xfId="594"/>
+    <cellStyle name="_Май_Июль_Индив._БЕЛ" xfId="595"/>
+    <cellStyle name="_Май_Июль_Индив._РЕЧ" xfId="596"/>
+    <cellStyle name="_Май_Июль_Июнь" xfId="597"/>
+    <cellStyle name="_Май_Июль_Июнь_Август" xfId="598"/>
+    <cellStyle name="_Май_Июль_Июнь_Дистанц." xfId="599"/>
+    <cellStyle name="_Май_Июль_Июнь_Индив." xfId="600"/>
+    <cellStyle name="_Май_Июль_Июнь_КБУ" xfId="601"/>
+    <cellStyle name="_Май_Июль_КБУ" xfId="602"/>
+    <cellStyle name="_Май_Июль_КРН" xfId="603"/>
+    <cellStyle name="_Май_Июль_ОПШ" xfId="604"/>
+    <cellStyle name="_Май_Июль_СР" xfId="605"/>
+    <cellStyle name="_Май_Июнь" xfId="606"/>
+    <cellStyle name="_Май_Июнь_1" xfId="607"/>
+    <cellStyle name="_Май_Июнь_1_Август" xfId="608"/>
+    <cellStyle name="_Май_Июнь_1_Дистанц." xfId="609"/>
+    <cellStyle name="_Май_Июнь_1_Индив." xfId="610"/>
+    <cellStyle name="_Май_Июнь_1_КБУ" xfId="611"/>
+    <cellStyle name="_Май_Июнь_Август" xfId="612"/>
+    <cellStyle name="_Май_Июнь_Август_Дистанц." xfId="613"/>
+    <cellStyle name="_Май_Июнь_Август_Индив." xfId="614"/>
+    <cellStyle name="_Май_Июнь_БЕЛ" xfId="615"/>
+    <cellStyle name="_Май_Июнь_БИНТ" xfId="616"/>
+    <cellStyle name="_Май_Июнь_БИНТ_БЕЛ" xfId="617"/>
+    <cellStyle name="_Май_Июнь_БИНТ_РЕЧ" xfId="618"/>
+    <cellStyle name="_Май_Июнь_БУХ" xfId="619"/>
+    <cellStyle name="_Май_Июнь_БУХ_БЕЛ" xfId="620"/>
+    <cellStyle name="_Май_Июнь_БУХ_РЕЧ" xfId="621"/>
+    <cellStyle name="_Май_Июнь_ВЕБДИЗ" xfId="622"/>
+    <cellStyle name="_Май_Июнь_ВЕБМАСТ" xfId="623"/>
+    <cellStyle name="_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="624"/>
+    <cellStyle name="_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="625"/>
+    <cellStyle name="_Май_Июнь_Дети" xfId="626"/>
+    <cellStyle name="_Май_Июнь_Дистанц." xfId="627"/>
+    <cellStyle name="_Май_Июнь_Индив." xfId="628"/>
+    <cellStyle name="_Май_Июнь_Индив._БЕЛ" xfId="629"/>
+    <cellStyle name="_Май_Июнь_Индив._РЕЧ" xfId="630"/>
+    <cellStyle name="_Май_Июнь_Июнь" xfId="631"/>
+    <cellStyle name="_Май_Июнь_Июнь_Август" xfId="632"/>
+    <cellStyle name="_Май_Июнь_Июнь_Дистанц." xfId="633"/>
+    <cellStyle name="_Май_Июнь_Июнь_Индив." xfId="634"/>
+    <cellStyle name="_Май_Июнь_Июнь_КБУ" xfId="635"/>
+    <cellStyle name="_Май_Июнь_КБУ" xfId="636"/>
+    <cellStyle name="_Май_Июнь_КРН" xfId="637"/>
+    <cellStyle name="_Май_Июнь_ОПШ" xfId="638"/>
+    <cellStyle name="_Май_Июнь_СР" xfId="639"/>
+    <cellStyle name="_Май_КБУ" xfId="640"/>
+    <cellStyle name="_Май_КРН" xfId="641"/>
+    <cellStyle name="_Май_Май" xfId="642"/>
+    <cellStyle name="_Май_Май_Август" xfId="643"/>
+    <cellStyle name="_Май_Май_Август_Дистанц." xfId="644"/>
+    <cellStyle name="_Май_Май_Август_Индив." xfId="645"/>
+    <cellStyle name="_Май_Май_БЕЛ" xfId="646"/>
+    <cellStyle name="_Май_Май_БИНТ" xfId="647"/>
+    <cellStyle name="_Май_Май_БИНТ_БЕЛ" xfId="648"/>
+    <cellStyle name="_Май_Май_БИНТ_РЕЧ" xfId="649"/>
+    <cellStyle name="_Май_Май_ВЕБДИЗ" xfId="650"/>
+    <cellStyle name="_Май_Май_ВЕБМАСТ" xfId="651"/>
+    <cellStyle name="_Май_Май_ВЕБМАСТ_БЕЛ" xfId="652"/>
+    <cellStyle name="_Май_Май_ВЕБМАСТ_РЕЧ" xfId="653"/>
+    <cellStyle name="_Май_Май_Дети" xfId="654"/>
+    <cellStyle name="_Май_Май_Дистанц." xfId="655"/>
+    <cellStyle name="_Май_Май_Индив." xfId="656"/>
+    <cellStyle name="_Май_Май_Индив._БЕЛ" xfId="657"/>
+    <cellStyle name="_Май_Май_Индив._РЕЧ" xfId="658"/>
+    <cellStyle name="_Май_Май_Июнь" xfId="659"/>
+    <cellStyle name="_Май_Май_Июнь_Август" xfId="660"/>
+    <cellStyle name="_Май_Май_Июнь_Дистанц." xfId="661"/>
+    <cellStyle name="_Май_Май_Июнь_Индив." xfId="662"/>
+    <cellStyle name="_Май_Май_Июнь_КБУ" xfId="663"/>
+    <cellStyle name="_Май_Май_КБУ" xfId="664"/>
+    <cellStyle name="_Май_Май_КРН" xfId="665"/>
+    <cellStyle name="_Май_Май_ОПШ" xfId="666"/>
+    <cellStyle name="_Май_Май_СР" xfId="667"/>
+    <cellStyle name="_Май_ОПШ" xfId="668"/>
+    <cellStyle name="_Май_РЕЧ" xfId="669"/>
+    <cellStyle name="_Май_РЕЧ_БЕЛ" xfId="670"/>
+    <cellStyle name="_Май_РЕЧ_РЕЧ" xfId="671"/>
+    <cellStyle name="_Май_СИ" xfId="672"/>
+    <cellStyle name="_Май_СИ_БЕЛ" xfId="673"/>
+    <cellStyle name="_Май_СИ_РЕЧ" xfId="674"/>
+    <cellStyle name="_Май_СР" xfId="675"/>
+    <cellStyle name="_Май_СУБД" xfId="676"/>
+    <cellStyle name="_Май_СУБД_БЕЛ" xfId="677"/>
+    <cellStyle name="_Май_СУБД_РЕЧ" xfId="678"/>
+    <cellStyle name="_МП" xfId="679"/>
+    <cellStyle name="_МП_БЕЛ" xfId="680"/>
+    <cellStyle name="_МП_РЕЧ" xfId="681"/>
+    <cellStyle name="_НТ" xfId="682"/>
+    <cellStyle name="_НТ_БЕЛ" xfId="683"/>
+    <cellStyle name="_НТ_РЕЧ" xfId="684"/>
+    <cellStyle name="_ОПШ" xfId="685"/>
+    <cellStyle name="_ОПШ_Апрель" xfId="686"/>
+    <cellStyle name="_ОПШ_Апрель_БЕЛ" xfId="687"/>
+    <cellStyle name="_ОПШ_Апрель_РЕЧ" xfId="688"/>
+    <cellStyle name="_ОПШ_БЕЛ" xfId="689"/>
+    <cellStyle name="_ОПШ_Июль" xfId="690"/>
+    <cellStyle name="_ОПШ_Июль_БЕЛ" xfId="691"/>
+    <cellStyle name="_ОПШ_Июль_РЕЧ" xfId="692"/>
+    <cellStyle name="_ОПШ_Июнь" xfId="693"/>
+    <cellStyle name="_ОПШ_Июнь_БЕЛ" xfId="694"/>
+    <cellStyle name="_ОПШ_Июнь_РЕЧ" xfId="695"/>
+    <cellStyle name="_ОПШ_Май" xfId="696"/>
+    <cellStyle name="_ОПШ_Май_БЕЛ" xfId="697"/>
+    <cellStyle name="_ОПШ_Май_РЕЧ" xfId="698"/>
+    <cellStyle name="_ОПШ_РЕЧ" xfId="699"/>
+    <cellStyle name="_ОПШ_Февраль" xfId="700"/>
+    <cellStyle name="_ОПШ_Февраль_БЕЛ" xfId="701"/>
+    <cellStyle name="_ОПШ_Февраль_РЕЧ" xfId="702"/>
+    <cellStyle name="_ОПШ_Январь" xfId="703"/>
+    <cellStyle name="_ОПШ_Январь_БЕЛ" xfId="704"/>
+    <cellStyle name="_ОПШ_Январь_РЕЧ" xfId="705"/>
+    <cellStyle name="_Офис" xfId="706"/>
+    <cellStyle name="_Офис_БЕЛ" xfId="707"/>
+    <cellStyle name="_Офис_РЕЧ" xfId="708"/>
+    <cellStyle name="_ПРШ" xfId="709"/>
+    <cellStyle name="_ПРШ_Апрель" xfId="710"/>
+    <cellStyle name="_ПРШ_Апрель_БЕЛ" xfId="711"/>
+    <cellStyle name="_ПРШ_Апрель_РЕЧ" xfId="712"/>
+    <cellStyle name="_ПРШ_БЕЛ" xfId="713"/>
+    <cellStyle name="_ПРШ_Июль" xfId="714"/>
+    <cellStyle name="_ПРШ_Июль_БЕЛ" xfId="715"/>
+    <cellStyle name="_ПРШ_Июль_РЕЧ" xfId="716"/>
+    <cellStyle name="_ПРШ_Июнь" xfId="717"/>
+    <cellStyle name="_ПРШ_Июнь_БЕЛ" xfId="718"/>
+    <cellStyle name="_ПРШ_Июнь_РЕЧ" xfId="719"/>
+    <cellStyle name="_ПРШ_Май" xfId="720"/>
+    <cellStyle name="_ПРШ_Май_БЕЛ" xfId="721"/>
+    <cellStyle name="_ПРШ_Май_РЕЧ" xfId="722"/>
+    <cellStyle name="_ПРШ_РЕЧ" xfId="723"/>
+    <cellStyle name="_ПРШ_Февраль" xfId="724"/>
+    <cellStyle name="_ПРШ_Февраль_БЕЛ" xfId="725"/>
+    <cellStyle name="_ПРШ_Февраль_РЕЧ" xfId="726"/>
+    <cellStyle name="_ПРШ_Январь" xfId="727"/>
+    <cellStyle name="_ПРШ_Январь_БЕЛ" xfId="728"/>
+    <cellStyle name="_ПРШ_Январь_РЕЧ" xfId="729"/>
+    <cellStyle name="_РЕЧ" xfId="730"/>
+    <cellStyle name="_РЕЧ_БЕЛ" xfId="731"/>
+    <cellStyle name="_РЕЧ_РЕЧ" xfId="732"/>
+    <cellStyle name="_СВБ" xfId="733"/>
+    <cellStyle name="_СВБ_БЕЛ" xfId="734"/>
+    <cellStyle name="_СВБ_РЕЧ" xfId="735"/>
+    <cellStyle name="_СИ" xfId="736"/>
+    <cellStyle name="_СИ_БЕЛ" xfId="737"/>
+    <cellStyle name="_СИ_РЕЧ" xfId="738"/>
+    <cellStyle name="_СИС" xfId="739"/>
+    <cellStyle name="_СИС_БЕЛ" xfId="740"/>
+    <cellStyle name="_СИС_РЕЧ" xfId="741"/>
+    <cellStyle name="_СР" xfId="742"/>
+    <cellStyle name="_СУБД" xfId="743"/>
+    <cellStyle name="_СУБД_БЕЛ" xfId="744"/>
+    <cellStyle name="_СУБД_РЕЧ" xfId="745"/>
+    <cellStyle name="_СЧ СПЕЦ" xfId="746"/>
+    <cellStyle name="_СЧ ЦКО" xfId="747"/>
+    <cellStyle name="_СЧ ЦКО_Лист1" xfId="748"/>
+    <cellStyle name="_СЧ ЦКО_Лист1_БЕЛ" xfId="749"/>
+    <cellStyle name="_СЧ ЦКО_Лист1_РЕЧ" xfId="750"/>
+    <cellStyle name="_СЧ ЦКО_СЧ СПЕЦ" xfId="751"/>
+    <cellStyle name="_СЧ ЦКО_СЧДОГ СПЕЦ" xfId="752"/>
+    <cellStyle name="_СЧДОГ" xfId="753"/>
+    <cellStyle name="_СЧДОГ СПЕЦ" xfId="754"/>
+    <cellStyle name="_СЧДОГ_1" xfId="755"/>
+    <cellStyle name="_СЧДОГ_3ДМ" xfId="756"/>
+    <cellStyle name="_СЧДОГ_3ДМ_БЕЛ" xfId="757"/>
+    <cellStyle name="_СЧДОГ_3ДМ_РЕЧ" xfId="758"/>
+    <cellStyle name="_СЧДОГ_Август" xfId="759"/>
+    <cellStyle name="_СЧДОГ_Август_Дистанц." xfId="760"/>
+    <cellStyle name="_СЧДОГ_Август_Индив." xfId="761"/>
+    <cellStyle name="_СЧДОГ_АКАД" xfId="762"/>
+    <cellStyle name="_СЧДОГ_АКАД_БЕЛ" xfId="763"/>
+    <cellStyle name="_СЧДОГ_АКАД_РЕЧ" xfId="764"/>
+    <cellStyle name="_СЧДОГ_Б9560" xfId="765"/>
+    <cellStyle name="_СЧДОГ_Б9560_БЕЛ" xfId="766"/>
+    <cellStyle name="_СЧДОГ_Б9560_РЕЧ" xfId="767"/>
+    <cellStyle name="_СЧДОГ_БЕЛ" xfId="768"/>
+    <cellStyle name="_СЧДОГ_БИНТ" xfId="769"/>
+    <cellStyle name="_СЧДОГ_БИНТ_БЕЛ" xfId="770"/>
+    <cellStyle name="_СЧДОГ_БИНТ_РЕЧ" xfId="771"/>
+    <cellStyle name="_СЧДОГ_БУХ" xfId="772"/>
+    <cellStyle name="_СЧДОГ_БУХ_БЕЛ" xfId="773"/>
+    <cellStyle name="_СЧДОГ_БУХ_РЕЧ" xfId="774"/>
+    <cellStyle name="_СЧДОГ_ВЕБДИЗ" xfId="775"/>
+    <cellStyle name="_СЧДОГ_ВЕБДИЗ_БЕЛ" xfId="776"/>
+    <cellStyle name="_СЧДОГ_ВЕБДИЗ_РЕЧ" xfId="777"/>
+    <cellStyle name="_СЧДОГ_ВЕБМАСТ" xfId="778"/>
+    <cellStyle name="_СЧДОГ_ВЕБМАСТ_БЕЛ" xfId="779"/>
+    <cellStyle name="_СЧДОГ_ВЕБМАСТ_РЕЧ" xfId="780"/>
+    <cellStyle name="_СЧДОГ_ВУЕ" xfId="781"/>
+    <cellStyle name="_СЧДОГ_ВУЕ_БЕЛ" xfId="782"/>
+    <cellStyle name="_СЧДОГ_ВУЕ_РЕЧ" xfId="783"/>
+    <cellStyle name="_СЧДОГ_Дети" xfId="784"/>
+    <cellStyle name="_СЧДОГ_Дети_БЕЛ" xfId="785"/>
+    <cellStyle name="_СЧДОГ_Дети_РЕЧ" xfId="786"/>
+    <cellStyle name="_СЧДОГ_Дистанц." xfId="787"/>
+    <cellStyle name="_СЧДОГ_Индив." xfId="788"/>
+    <cellStyle name="_СЧДОГ_Индив._БЕЛ" xfId="789"/>
+    <cellStyle name="_СЧДОГ_Индив._РЕЧ" xfId="790"/>
+    <cellStyle name="_СЧДОГ_Июль" xfId="791"/>
+    <cellStyle name="_СЧДОГ_Июль_Август" xfId="792"/>
+    <cellStyle name="_СЧДОГ_Июль_Август_Дистанц." xfId="793"/>
+    <cellStyle name="_СЧДОГ_Июль_Август_Индив." xfId="794"/>
+    <cellStyle name="_СЧДОГ_Июль_БЕЛ" xfId="795"/>
+    <cellStyle name="_СЧДОГ_Июль_БИНТ" xfId="796"/>
+    <cellStyle name="_СЧДОГ_Июль_БИНТ_БЕЛ" xfId="797"/>
+    <cellStyle name="_СЧДОГ_Июль_БИНТ_РЕЧ" xfId="798"/>
+    <cellStyle name="_СЧДОГ_Июль_ВЕБДИЗ" xfId="799"/>
+    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ" xfId="800"/>
+    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ_БЕЛ" xfId="801"/>
+    <cellStyle name="_СЧДОГ_Июль_ВЕБМАСТ_РЕЧ" xfId="802"/>
+    <cellStyle name="_СЧДОГ_Июль_Дети" xfId="803"/>
+    <cellStyle name="_СЧДОГ_Июль_Дистанц." xfId="804"/>
+    <cellStyle name="_СЧДОГ_Июль_Индив." xfId="805"/>
+    <cellStyle name="_СЧДОГ_Июль_Индив._БЕЛ" xfId="806"/>
+    <cellStyle name="_СЧДОГ_Июль_Индив._РЕЧ" xfId="807"/>
+    <cellStyle name="_СЧДОГ_Июль_Июнь" xfId="808"/>
+    <cellStyle name="_СЧДОГ_Июль_Июнь_Август" xfId="809"/>
+    <cellStyle name="_СЧДОГ_Июль_Июнь_Дистанц." xfId="810"/>
+    <cellStyle name="_СЧДОГ_Июль_Июнь_Индив." xfId="811"/>
+    <cellStyle name="_СЧДОГ_Июль_Июнь_КБУ" xfId="812"/>
+    <cellStyle name="_СЧДОГ_Июль_КБУ" xfId="813"/>
+    <cellStyle name="_СЧДОГ_Июль_КРН" xfId="814"/>
+    <cellStyle name="_СЧДОГ_Июль_ОПШ" xfId="815"/>
+    <cellStyle name="_СЧДОГ_Июль_СР" xfId="816"/>
+    <cellStyle name="_СЧДОГ_Июнь" xfId="817"/>
+    <cellStyle name="_СЧДОГ_Июнь_1" xfId="818"/>
+    <cellStyle name="_СЧДОГ_Июнь_1_Август" xfId="819"/>
+    <cellStyle name="_СЧДОГ_Июнь_1_Дистанц." xfId="820"/>
+    <cellStyle name="_СЧДОГ_Июнь_1_Индив." xfId="821"/>
+    <cellStyle name="_СЧДОГ_Июнь_1_КБУ" xfId="822"/>
+    <cellStyle name="_СЧДОГ_Июнь_Август" xfId="823"/>
+    <cellStyle name="_СЧДОГ_Июнь_Август_Дистанц." xfId="824"/>
+    <cellStyle name="_СЧДОГ_Июнь_Август_Индив." xfId="825"/>
+    <cellStyle name="_СЧДОГ_Июнь_БЕЛ" xfId="826"/>
+    <cellStyle name="_СЧДОГ_Июнь_БИНТ" xfId="827"/>
+    <cellStyle name="_СЧДОГ_Июнь_БИНТ_БЕЛ" xfId="828"/>
+    <cellStyle name="_СЧДОГ_Июнь_БИНТ_РЕЧ" xfId="829"/>
+    <cellStyle name="_СЧДОГ_Июнь_БУХ" xfId="830"/>
+    <cellStyle name="_СЧДОГ_Июнь_БУХ_БЕЛ" xfId="831"/>
+    <cellStyle name="_СЧДОГ_Июнь_БУХ_РЕЧ" xfId="832"/>
+    <cellStyle name="_СЧДОГ_Июнь_ВЕБДИЗ" xfId="833"/>
+    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ" xfId="834"/>
+    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ_БЕЛ" xfId="835"/>
+    <cellStyle name="_СЧДОГ_Июнь_ВЕБМАСТ_РЕЧ" xfId="836"/>
+    <cellStyle name="_СЧДОГ_Июнь_Дети" xfId="837"/>
+    <cellStyle name="_СЧДОГ_Июнь_Дистанц." xfId="838"/>
+    <cellStyle name="_СЧДОГ_Июнь_Индив." xfId="839"/>
+    <cellStyle name="_СЧДОГ_Июнь_Индив._БЕЛ" xfId="840"/>
+    <cellStyle name="_СЧДОГ_Июнь_Индив._РЕЧ" xfId="841"/>
+    <cellStyle name="_СЧДОГ_Июнь_Июнь" xfId="842"/>
+    <cellStyle name="_СЧДОГ_Июнь_Июнь_Август" xfId="843"/>
+    <cellStyle name="_СЧДОГ_Июнь_Июнь_Дистанц." xfId="844"/>
+    <cellStyle name="_СЧДОГ_Июнь_Июнь_Индив." xfId="845"/>
+    <cellStyle name="_СЧДОГ_Июнь_Июнь_КБУ" xfId="846"/>
+    <cellStyle name="_СЧДОГ_Июнь_КБУ" xfId="847"/>
+    <cellStyle name="_СЧДОГ_Июнь_КРН" xfId="848"/>
+    <cellStyle name="_СЧДОГ_Июнь_ОПШ" xfId="849"/>
+    <cellStyle name="_СЧДОГ_Июнь_СР" xfId="850"/>
+    <cellStyle name="_СЧДОГ_КБУ" xfId="851"/>
+    <cellStyle name="_СЧДОГ_КБУ_БЕЛ" xfId="852"/>
+    <cellStyle name="_СЧДОГ_КБУ_РЕЧ" xfId="853"/>
+    <cellStyle name="_СЧДОГ_КРН" xfId="854"/>
+    <cellStyle name="_СЧДОГ_Май" xfId="855"/>
+    <cellStyle name="_СЧДОГ_Май_1" xfId="856"/>
+    <cellStyle name="_СЧДОГ_Май_1_Август" xfId="857"/>
+    <cellStyle name="_СЧДОГ_Май_1_Август_Дистанц." xfId="858"/>
+    <cellStyle name="_СЧДОГ_Май_1_Август_Индив." xfId="859"/>
+    <cellStyle name="_СЧДОГ_Май_1_БЕЛ" xfId="860"/>
+    <cellStyle name="_СЧДОГ_Май_1_БИНТ" xfId="861"/>
+    <cellStyle name="_СЧДОГ_Май_1_БИНТ_БЕЛ" xfId="862"/>
+    <cellStyle name="_СЧДОГ_Май_1_БИНТ_РЕЧ" xfId="863"/>
+    <cellStyle name="_СЧДОГ_Май_1_ВЕБДИЗ" xfId="864"/>
+    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ" xfId="865"/>
+    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ_БЕЛ" xfId="866"/>
+    <cellStyle name="_СЧДОГ_Май_1_ВЕБМАСТ_РЕЧ" xfId="867"/>
+    <cellStyle name="_СЧДОГ_Май_1_Дети" xfId="868"/>
+    <cellStyle name="_СЧДОГ_Май_1_Дистанц." xfId="869"/>
+    <cellStyle name="_СЧДОГ_Май_1_Индив." xfId="870"/>
+    <cellStyle name="_СЧДОГ_Май_1_Индив._БЕЛ" xfId="871"/>
+    <cellStyle name="_СЧДОГ_Май_1_Индив._РЕЧ" xfId="872"/>
+    <cellStyle name="_СЧДОГ_Май_1_Июнь" xfId="873"/>
+    <cellStyle name="_СЧДОГ_Май_1_Июнь_Август" xfId="874"/>
+    <cellStyle name="_СЧДОГ_Май_1_Июнь_Дистанц." xfId="875"/>
+    <cellStyle name="_СЧДОГ_Май_1_Июнь_Индив." xfId="876"/>
+    <cellStyle name="_СЧДОГ_Май_1_Июнь_КБУ" xfId="877"/>
+    <cellStyle name="_СЧДОГ_Май_1_КБУ" xfId="878"/>
+    <cellStyle name="_СЧДОГ_Май_1_КРН" xfId="879"/>
+    <cellStyle name="_СЧДОГ_Май_1_ОПШ" xfId="880"/>
+    <cellStyle name="_СЧДОГ_Май_1_СР" xfId="881"/>
+    <cellStyle name="_СЧДОГ_Май_Август" xfId="882"/>
+    <cellStyle name="_СЧДОГ_Май_Август_Дистанц." xfId="883"/>
+    <cellStyle name="_СЧДОГ_Май_Август_Индив." xfId="884"/>
+    <cellStyle name="_СЧДОГ_Май_АКАД" xfId="885"/>
+    <cellStyle name="_СЧДОГ_Май_АКАД_БЕЛ" xfId="886"/>
+    <cellStyle name="_СЧДОГ_Май_АКАД_РЕЧ" xfId="887"/>
+    <cellStyle name="_СЧДОГ_Май_Б9560" xfId="888"/>
+    <cellStyle name="_СЧДОГ_Май_Б9560_БЕЛ" xfId="889"/>
+    <cellStyle name="_СЧДОГ_Май_Б9560_РЕЧ" xfId="890"/>
+    <cellStyle name="_СЧДОГ_Май_БЕЛ" xfId="891"/>
+    <cellStyle name="_СЧДОГ_Май_БИНТ" xfId="892"/>
+    <cellStyle name="_СЧДОГ_Май_БИНТ_БЕЛ" xfId="893"/>
+    <cellStyle name="_СЧДОГ_Май_БИНТ_РЕЧ" xfId="894"/>
+    <cellStyle name="_СЧДОГ_Май_БУХ" xfId="895"/>
+    <cellStyle name="_СЧДОГ_Май_БУХ_БЕЛ" xfId="896"/>
+    <cellStyle name="_СЧДОГ_Май_БУХ_РЕЧ" xfId="897"/>
+    <cellStyle name="_СЧДОГ_Май_ВЕБДИЗ" xfId="898"/>
+    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ" xfId="899"/>
+    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ_БЕЛ" xfId="900"/>
+    <cellStyle name="_СЧДОГ_Май_ВЕБМАСТ_РЕЧ" xfId="901"/>
+    <cellStyle name="_СЧДОГ_Май_Дети" xfId="902"/>
+    <cellStyle name="_СЧДОГ_Май_Дистанц." xfId="903"/>
+    <cellStyle name="_СЧДОГ_Май_Индив." xfId="904"/>
+    <cellStyle name="_СЧДОГ_Май_Индив._БЕЛ" xfId="905"/>
+    <cellStyle name="_СЧДОГ_Май_Индив._РЕЧ" xfId="906"/>
+    <cellStyle name="_СЧДОГ_Май_Июль" xfId="907"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Август" xfId="908"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Август_Дистанц." xfId="909"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Август_Индив." xfId="910"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_БЕЛ" xfId="911"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ" xfId="912"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ_БЕЛ" xfId="913"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_БИНТ_РЕЧ" xfId="914"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБДИЗ" xfId="915"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ" xfId="916"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="917"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="918"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Дети" xfId="919"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Дистанц." xfId="920"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Индив." xfId="921"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Индив._БЕЛ" xfId="922"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Индив._РЕЧ" xfId="923"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Июнь" xfId="924"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Август" xfId="925"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Дистанц." xfId="926"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_Индив." xfId="927"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_Июнь_КБУ" xfId="928"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_КБУ" xfId="929"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_КРН" xfId="930"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_ОПШ" xfId="931"/>
+    <cellStyle name="_СЧДОГ_Май_Июль_СР" xfId="932"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь" xfId="933"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_1" xfId="934"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_1_Август" xfId="935"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_1_Дистанц." xfId="936"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_1_Индив." xfId="937"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_1_КБУ" xfId="938"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Август" xfId="939"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Август_Дистанц." xfId="940"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Август_Индив." xfId="941"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БЕЛ" xfId="942"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ" xfId="943"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ_БЕЛ" xfId="944"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БИНТ_РЕЧ" xfId="945"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ" xfId="946"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ_БЕЛ" xfId="947"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_БУХ_РЕЧ" xfId="948"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБДИЗ" xfId="949"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ" xfId="950"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="951"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="952"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Дети" xfId="953"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Дистанц." xfId="954"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Индив." xfId="955"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Индив._БЕЛ" xfId="956"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Индив._РЕЧ" xfId="957"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь" xfId="958"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Август" xfId="959"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Дистанц." xfId="960"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_Индив." xfId="961"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_Июнь_КБУ" xfId="962"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_КБУ" xfId="963"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_КРН" xfId="964"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_ОПШ" xfId="965"/>
+    <cellStyle name="_СЧДОГ_Май_Июнь_СР" xfId="966"/>
+    <cellStyle name="_СЧДОГ_Май_КБУ" xfId="967"/>
+    <cellStyle name="_СЧДОГ_Май_КРН" xfId="968"/>
+    <cellStyle name="_СЧДОГ_Май_Май" xfId="969"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Август" xfId="970"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Август_Дистанц." xfId="971"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Август_Индив." xfId="972"/>
+    <cellStyle name="_СЧДОГ_Май_Май_БЕЛ" xfId="973"/>
+    <cellStyle name="_СЧДОГ_Май_Май_БИНТ" xfId="974"/>
+    <cellStyle name="_СЧДОГ_Май_Май_БИНТ_БЕЛ" xfId="975"/>
+    <cellStyle name="_СЧДОГ_Май_Май_БИНТ_РЕЧ" xfId="976"/>
+    <cellStyle name="_СЧДОГ_Май_Май_ВЕБДИЗ" xfId="977"/>
+    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ" xfId="978"/>
+    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ_БЕЛ" xfId="979"/>
+    <cellStyle name="_СЧДОГ_Май_Май_ВЕБМАСТ_РЕЧ" xfId="980"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Дети" xfId="981"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Дистанц." xfId="982"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Индив." xfId="983"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Индив._БЕЛ" xfId="984"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Индив._РЕЧ" xfId="985"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Июнь" xfId="986"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Август" xfId="987"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Дистанц." xfId="988"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Июнь_Индив." xfId="989"/>
+    <cellStyle name="_СЧДОГ_Май_Май_Июнь_КБУ" xfId="990"/>
+    <cellStyle name="_СЧДОГ_Май_Май_КБУ" xfId="991"/>
+    <cellStyle name="_СЧДОГ_Май_Май_КРН" xfId="992"/>
+    <cellStyle name="_СЧДОГ_Май_Май_ОПШ" xfId="993"/>
+    <cellStyle name="_СЧДОГ_Май_Май_СР" xfId="994"/>
+    <cellStyle name="_СЧДОГ_Май_ОПШ" xfId="995"/>
+    <cellStyle name="_СЧДОГ_Май_РЕЧ" xfId="996"/>
+    <cellStyle name="_СЧДОГ_Май_РЕЧ_БЕЛ" xfId="997"/>
+    <cellStyle name="_СЧДОГ_Май_РЕЧ_РЕЧ" xfId="998"/>
+    <cellStyle name="_СЧДОГ_Май_СИ" xfId="999"/>
+    <cellStyle name="_СЧДОГ_Май_СИ_БЕЛ" xfId="1000"/>
+    <cellStyle name="_СЧДОГ_Май_СИ_РЕЧ" xfId="1001"/>
+    <cellStyle name="_СЧДОГ_Май_СР" xfId="1002"/>
+    <cellStyle name="_СЧДОГ_Май_СУБД" xfId="1003"/>
+    <cellStyle name="_СЧДОГ_Май_СУБД_БЕЛ" xfId="1004"/>
+    <cellStyle name="_СЧДОГ_Май_СУБД_РЕЧ" xfId="1005"/>
+    <cellStyle name="_СЧДОГ_НТ" xfId="1006"/>
+    <cellStyle name="_СЧДОГ_НТ_БЕЛ" xfId="1007"/>
+    <cellStyle name="_СЧДОГ_НТ_РЕЧ" xfId="1008"/>
+    <cellStyle name="_СЧДОГ_ОПШ" xfId="1009"/>
+    <cellStyle name="_СЧДОГ_Офис" xfId="1010"/>
+    <cellStyle name="_СЧДОГ_Офис_БЕЛ" xfId="1011"/>
+    <cellStyle name="_СЧДОГ_Офис_РЕЧ" xfId="1012"/>
+    <cellStyle name="_СЧДОГ_РЕЧ" xfId="1013"/>
+    <cellStyle name="_СЧДОГ_РЕЧ_БЕЛ" xfId="1014"/>
+    <cellStyle name="_СЧДОГ_РЕЧ_РЕЧ" xfId="1015"/>
+    <cellStyle name="_СЧДОГ_СИ" xfId="1016"/>
+    <cellStyle name="_СЧДОГ_СИ_БЕЛ" xfId="1017"/>
+    <cellStyle name="_СЧДОГ_СИ_РЕЧ" xfId="1018"/>
+    <cellStyle name="_СЧДОГ_СИС" xfId="1019"/>
+    <cellStyle name="_СЧДОГ_СИС_БЕЛ" xfId="1020"/>
+    <cellStyle name="_СЧДОГ_СИС_РЕЧ" xfId="1021"/>
+    <cellStyle name="_СЧДОГ_СР" xfId="1022"/>
+    <cellStyle name="_СЧДОГ_СУБД" xfId="1023"/>
+    <cellStyle name="_СЧДОГ_СУБД_БЕЛ" xfId="1024"/>
+    <cellStyle name="_СЧДОГ_СУБД_РЕЧ" xfId="1025"/>
+    <cellStyle name="_СЧДОГ_ТЕК" xfId="1026"/>
+    <cellStyle name="_СЧДОГ_ТЕК_БЕЛ" xfId="1027"/>
+    <cellStyle name="_СЧДОГ_ТЕК_РЕЧ" xfId="1028"/>
+    <cellStyle name="_СЧДОГ_Февраль" xfId="1029"/>
+    <cellStyle name="_СЧДОГ_Февраль_Август" xfId="1030"/>
+    <cellStyle name="_СЧДОГ_Февраль_Август_Дистанц." xfId="1031"/>
+    <cellStyle name="_СЧДОГ_Февраль_Август_Индив." xfId="1032"/>
+    <cellStyle name="_СЧДОГ_Февраль_АКАД" xfId="1033"/>
+    <cellStyle name="_СЧДОГ_Февраль_АКАД_БЕЛ" xfId="1034"/>
+    <cellStyle name="_СЧДОГ_Февраль_АКАД_РЕЧ" xfId="1035"/>
+    <cellStyle name="_СЧДОГ_Февраль_Б9560" xfId="1036"/>
+    <cellStyle name="_СЧДОГ_Февраль_Б9560_БЕЛ" xfId="1037"/>
+    <cellStyle name="_СЧДОГ_Февраль_Б9560_РЕЧ" xfId="1038"/>
+    <cellStyle name="_СЧДОГ_Февраль_БЕЛ" xfId="1039"/>
+    <cellStyle name="_СЧДОГ_Февраль_БИНТ" xfId="1040"/>
+    <cellStyle name="_СЧДОГ_Февраль_БИНТ_БЕЛ" xfId="1041"/>
+    <cellStyle name="_СЧДОГ_Февраль_БИНТ_РЕЧ" xfId="1042"/>
+    <cellStyle name="_СЧДОГ_Февраль_БУХ" xfId="1043"/>
+    <cellStyle name="_СЧДОГ_Февраль_БУХ_БЕЛ" xfId="1044"/>
+    <cellStyle name="_СЧДОГ_Февраль_БУХ_РЕЧ" xfId="1045"/>
+    <cellStyle name="_СЧДОГ_Февраль_ВЕБДИЗ" xfId="1046"/>
+    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ" xfId="1047"/>
+    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ_БЕЛ" xfId="1048"/>
+    <cellStyle name="_СЧДОГ_Февраль_ВЕБМАСТ_РЕЧ" xfId="1049"/>
+    <cellStyle name="_СЧДОГ_Февраль_Дети" xfId="1050"/>
+    <cellStyle name="_СЧДОГ_Февраль_Дистанц." xfId="1051"/>
+    <cellStyle name="_СЧДОГ_Февраль_Индив." xfId="1052"/>
+    <cellStyle name="_СЧДОГ_Февраль_Индив._БЕЛ" xfId="1053"/>
+    <cellStyle name="_СЧДОГ_Февраль_Индив._РЕЧ" xfId="1054"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль" xfId="1055"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Август" xfId="1056"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Август_Дистанц." xfId="1057"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Август_Индив." xfId="1058"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_БЕЛ" xfId="1059"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ" xfId="1060"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ_БЕЛ" xfId="1061"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_БИНТ_РЕЧ" xfId="1062"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБДИЗ" xfId="1063"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ" xfId="1064"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1065"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1066"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Дети" xfId="1067"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Дистанц." xfId="1068"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив." xfId="1069"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив._БЕЛ" xfId="1070"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Индив._РЕЧ" xfId="1071"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь" xfId="1072"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Август" xfId="1073"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Дистанц." xfId="1074"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_Индив." xfId="1075"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_Июнь_КБУ" xfId="1076"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_КБУ" xfId="1077"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_КРН" xfId="1078"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_ОПШ" xfId="1079"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июль_СР" xfId="1080"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь" xfId="1081"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_1" xfId="1082"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Август" xfId="1083"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Дистанц." xfId="1084"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_Индив." xfId="1085"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_1_КБУ" xfId="1086"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август" xfId="1087"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август_Дистанц." xfId="1088"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Август_Индив." xfId="1089"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БЕЛ" xfId="1090"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ" xfId="1091"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ_БЕЛ" xfId="1092"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БИНТ_РЕЧ" xfId="1093"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ" xfId="1094"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ_БЕЛ" xfId="1095"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_БУХ_РЕЧ" xfId="1096"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБДИЗ" xfId="1097"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ" xfId="1098"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1099"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1100"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Дети" xfId="1101"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Дистанц." xfId="1102"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив." xfId="1103"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив._БЕЛ" xfId="1104"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Индив._РЕЧ" xfId="1105"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь" xfId="1106"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Август" xfId="1107"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Дистанц." xfId="1108"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_Индив." xfId="1109"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_Июнь_КБУ" xfId="1110"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_КБУ" xfId="1111"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_КРН" xfId="1112"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_ОПШ" xfId="1113"/>
+    <cellStyle name="_СЧДОГ_Февраль_Июнь_СР" xfId="1114"/>
+    <cellStyle name="_СЧДОГ_Февраль_КБУ" xfId="1115"/>
+    <cellStyle name="_СЧДОГ_Февраль_КРН" xfId="1116"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май" xfId="1117"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Август" xfId="1118"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Август_Дистанц." xfId="1119"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Август_Индив." xfId="1120"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_БЕЛ" xfId="1121"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ" xfId="1122"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ_БЕЛ" xfId="1123"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_БИНТ_РЕЧ" xfId="1124"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБДИЗ" xfId="1125"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ" xfId="1126"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1127"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1128"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Дети" xfId="1129"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Дистанц." xfId="1130"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Индив." xfId="1131"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Индив._БЕЛ" xfId="1132"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Индив._РЕЧ" xfId="1133"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь" xfId="1134"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Август" xfId="1135"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Дистанц." xfId="1136"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_Индив." xfId="1137"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_Июнь_КБУ" xfId="1138"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_КБУ" xfId="1139"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_КРН" xfId="1140"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_ОПШ" xfId="1141"/>
+    <cellStyle name="_СЧДОГ_Февраль_Май_СР" xfId="1142"/>
+    <cellStyle name="_СЧДОГ_Февраль_ОПШ" xfId="1143"/>
+    <cellStyle name="_СЧДОГ_Февраль_РЕЧ" xfId="1144"/>
+    <cellStyle name="_СЧДОГ_Февраль_РЕЧ_БЕЛ" xfId="1145"/>
+    <cellStyle name="_СЧДОГ_Февраль_РЕЧ_РЕЧ" xfId="1146"/>
+    <cellStyle name="_СЧДОГ_Февраль_СИ" xfId="1147"/>
+    <cellStyle name="_СЧДОГ_Февраль_СИ_БЕЛ" xfId="1148"/>
+    <cellStyle name="_СЧДОГ_Февраль_СИ_РЕЧ" xfId="1149"/>
+    <cellStyle name="_СЧДОГ_Февраль_СР" xfId="1150"/>
+    <cellStyle name="_СЧДОГ_Февраль_СУБД" xfId="1151"/>
+    <cellStyle name="_СЧДОГ_Февраль_СУБД_БЕЛ" xfId="1152"/>
+    <cellStyle name="_СЧДОГ_Февраль_СУБД_РЕЧ" xfId="1153"/>
+    <cellStyle name="_СЧДОГ_ФШ" xfId="1154"/>
+    <cellStyle name="_СЧДОГ_ФШ_БЕЛ" xfId="1155"/>
+    <cellStyle name="_СЧДОГ_ФШ_РЕЧ" xfId="1156"/>
+    <cellStyle name="_ТЕК" xfId="1157"/>
+    <cellStyle name="_ТЕК_БЕЛ" xfId="1158"/>
+    <cellStyle name="_ТЕК_РЕЧ" xfId="1159"/>
+    <cellStyle name="_ТОР" xfId="1160"/>
+    <cellStyle name="_ТОР_БЕЛ" xfId="1161"/>
+    <cellStyle name="_ТОР_РЕЧ" xfId="1162"/>
+    <cellStyle name="_Февраль" xfId="1163"/>
+    <cellStyle name="_Февраль_Август" xfId="1164"/>
+    <cellStyle name="_Февраль_Август_Дистанц." xfId="1165"/>
+    <cellStyle name="_Февраль_Август_Индив." xfId="1166"/>
+    <cellStyle name="_Февраль_АКАД" xfId="1167"/>
+    <cellStyle name="_Февраль_АКАД_БЕЛ" xfId="1168"/>
+    <cellStyle name="_Февраль_АКАД_РЕЧ" xfId="1169"/>
+    <cellStyle name="_Февраль_Б9560" xfId="1170"/>
+    <cellStyle name="_Февраль_Б9560_БЕЛ" xfId="1171"/>
+    <cellStyle name="_Февраль_Б9560_РЕЧ" xfId="1172"/>
+    <cellStyle name="_Февраль_БЕЛ" xfId="1173"/>
+    <cellStyle name="_Февраль_БИНТ" xfId="1174"/>
+    <cellStyle name="_Февраль_БИНТ_БЕЛ" xfId="1175"/>
+    <cellStyle name="_Февраль_БИНТ_РЕЧ" xfId="1176"/>
+    <cellStyle name="_Февраль_БУХ" xfId="1177"/>
+    <cellStyle name="_Февраль_БУХ_БЕЛ" xfId="1178"/>
+    <cellStyle name="_Февраль_БУХ_РЕЧ" xfId="1179"/>
+    <cellStyle name="_Февраль_ВЕБДИЗ" xfId="1180"/>
+    <cellStyle name="_Февраль_ВЕБМАСТ" xfId="1181"/>
+    <cellStyle name="_Февраль_ВЕБМАСТ_БЕЛ" xfId="1182"/>
+    <cellStyle name="_Февраль_ВЕБМАСТ_РЕЧ" xfId="1183"/>
+    <cellStyle name="_Февраль_Дети" xfId="1184"/>
+    <cellStyle name="_Февраль_Дистанц." xfId="1185"/>
+    <cellStyle name="_Февраль_Индив." xfId="1186"/>
+    <cellStyle name="_Февраль_Индив._БЕЛ" xfId="1187"/>
+    <cellStyle name="_Февраль_Индив._РЕЧ" xfId="1188"/>
+    <cellStyle name="_Февраль_Июль" xfId="1189"/>
+    <cellStyle name="_Февраль_Июль_Август" xfId="1190"/>
+    <cellStyle name="_Февраль_Июль_Август_Дистанц." xfId="1191"/>
+    <cellStyle name="_Февраль_Июль_Август_Индив." xfId="1192"/>
+    <cellStyle name="_Февраль_Июль_БЕЛ" xfId="1193"/>
+    <cellStyle name="_Февраль_Июль_БИНТ" xfId="1194"/>
+    <cellStyle name="_Февраль_Июль_БИНТ_БЕЛ" xfId="1195"/>
+    <cellStyle name="_Февраль_Июль_БИНТ_РЕЧ" xfId="1196"/>
+    <cellStyle name="_Февраль_Июль_ВЕБДИЗ" xfId="1197"/>
+    <cellStyle name="_Февраль_Июль_ВЕБМАСТ" xfId="1198"/>
+    <cellStyle name="_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1199"/>
+    <cellStyle name="_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1200"/>
+    <cellStyle name="_Февраль_Июль_Дети" xfId="1201"/>
+    <cellStyle name="_Февраль_Июль_Дистанц." xfId="1202"/>
+    <cellStyle name="_Февраль_Июль_Индив." xfId="1203"/>
+    <cellStyle name="_Февраль_Июль_Индив._БЕЛ" xfId="1204"/>
+    <cellStyle name="_Февраль_Июль_Индив._РЕЧ" xfId="1205"/>
+    <cellStyle name="_Февраль_Июль_Июнь" xfId="1206"/>
+    <cellStyle name="_Февраль_Июль_Июнь_Август" xfId="1207"/>
+    <cellStyle name="_Февраль_Июль_Июнь_Дистанц." xfId="1208"/>
+    <cellStyle name="_Февраль_Июль_Июнь_Индив." xfId="1209"/>
+    <cellStyle name="_Февраль_Июль_Июнь_КБУ" xfId="1210"/>
+    <cellStyle name="_Февраль_Июль_КБУ" xfId="1211"/>
+    <cellStyle name="_Февраль_Июль_КРН" xfId="1212"/>
+    <cellStyle name="_Февраль_Июль_ОПШ" xfId="1213"/>
+    <cellStyle name="_Февраль_Июль_СР" xfId="1214"/>
+    <cellStyle name="_Февраль_Июнь" xfId="1215"/>
+    <cellStyle name="_Февраль_Июнь_1" xfId="1216"/>
+    <cellStyle name="_Февраль_Июнь_1_Август" xfId="1217"/>
+    <cellStyle name="_Февраль_Июнь_1_Дистанц." xfId="1218"/>
+    <cellStyle name="_Февраль_Июнь_1_Индив." xfId="1219"/>
+    <cellStyle name="_Февраль_Июнь_1_КБУ" xfId="1220"/>
+    <cellStyle name="_Февраль_Июнь_Август" xfId="1221"/>
+    <cellStyle name="_Февраль_Июнь_Август_Дистанц." xfId="1222"/>
+    <cellStyle name="_Февраль_Июнь_Август_Индив." xfId="1223"/>
+    <cellStyle name="_Февраль_Июнь_БЕЛ" xfId="1224"/>
+    <cellStyle name="_Февраль_Июнь_БИНТ" xfId="1225"/>
+    <cellStyle name="_Февраль_Июнь_БИНТ_БЕЛ" xfId="1226"/>
+    <cellStyle name="_Февраль_Июнь_БИНТ_РЕЧ" xfId="1227"/>
+    <cellStyle name="_Февраль_Июнь_БУХ" xfId="1228"/>
+    <cellStyle name="_Февраль_Июнь_БУХ_БЕЛ" xfId="1229"/>
+    <cellStyle name="_Февраль_Июнь_БУХ_РЕЧ" xfId="1230"/>
+    <cellStyle name="_Февраль_Июнь_ВЕБДИЗ" xfId="1231"/>
+    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ" xfId="1232"/>
+    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1233"/>
+    <cellStyle name="_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1234"/>
+    <cellStyle name="_Февраль_Июнь_Дети" xfId="1235"/>
+    <cellStyle name="_Февраль_Июнь_Дистанц." xfId="1236"/>
+    <cellStyle name="_Февраль_Июнь_Индив." xfId="1237"/>
+    <cellStyle name="_Февраль_Июнь_Индив._БЕЛ" xfId="1238"/>
+    <cellStyle name="_Февраль_Июнь_Индив._РЕЧ" xfId="1239"/>
+    <cellStyle name="_Февраль_Июнь_Июнь" xfId="1240"/>
+    <cellStyle name="_Февраль_Июнь_Июнь_Август" xfId="1241"/>
+    <cellStyle name="_Февраль_Июнь_Июнь_Дистанц." xfId="1242"/>
+    <cellStyle name="_Февраль_Июнь_Июнь_Индив." xfId="1243"/>
+    <cellStyle name="_Февраль_Июнь_Июнь_КБУ" xfId="1244"/>
+    <cellStyle name="_Февраль_Июнь_КБУ" xfId="1245"/>
+    <cellStyle name="_Февраль_Июнь_КРН" xfId="1246"/>
+    <cellStyle name="_Февраль_Июнь_ОПШ" xfId="1247"/>
+    <cellStyle name="_Февраль_Июнь_СР" xfId="1248"/>
+    <cellStyle name="_Февраль_КБУ" xfId="1249"/>
+    <cellStyle name="_Февраль_КРН" xfId="1250"/>
+    <cellStyle name="_Февраль_Май" xfId="1251"/>
+    <cellStyle name="_Февраль_Май_Август" xfId="1252"/>
+    <cellStyle name="_Февраль_Май_Август_Дистанц." xfId="1253"/>
+    <cellStyle name="_Февраль_Май_Август_Индив." xfId="1254"/>
+    <cellStyle name="_Февраль_Май_БЕЛ" xfId="1255"/>
+    <cellStyle name="_Февраль_Май_БИНТ" xfId="1256"/>
+    <cellStyle name="_Февраль_Май_БИНТ_БЕЛ" xfId="1257"/>
+    <cellStyle name="_Февраль_Май_БИНТ_РЕЧ" xfId="1258"/>
+    <cellStyle name="_Февраль_Май_ВЕБДИЗ" xfId="1259"/>
+    <cellStyle name="_Февраль_Май_ВЕБМАСТ" xfId="1260"/>
+    <cellStyle name="_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1261"/>
+    <cellStyle name="_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1262"/>
+    <cellStyle name="_Февраль_Май_Дети" xfId="1263"/>
+    <cellStyle name="_Февраль_Май_Дистанц." xfId="1264"/>
+    <cellStyle name="_Февраль_Май_Индив." xfId="1265"/>
+    <cellStyle name="_Февраль_Май_Индив._БЕЛ" xfId="1266"/>
+    <cellStyle name="_Февраль_Май_Индив._РЕЧ" xfId="1267"/>
+    <cellStyle name="_Февраль_Май_Июнь" xfId="1268"/>
+    <cellStyle name="_Февраль_Май_Июнь_Август" xfId="1269"/>
+    <cellStyle name="_Февраль_Май_Июнь_Дистанц." xfId="1270"/>
+    <cellStyle name="_Февраль_Май_Июнь_Индив." xfId="1271"/>
+    <cellStyle name="_Февраль_Май_Июнь_КБУ" xfId="1272"/>
+    <cellStyle name="_Февраль_Май_КБУ" xfId="1273"/>
+    <cellStyle name="_Февраль_Май_КРН" xfId="1274"/>
+    <cellStyle name="_Февраль_Май_ОПШ" xfId="1275"/>
+    <cellStyle name="_Февраль_Май_СР" xfId="1276"/>
+    <cellStyle name="_Февраль_ОПШ" xfId="1277"/>
+    <cellStyle name="_Февраль_РЕЧ" xfId="1278"/>
+    <cellStyle name="_Февраль_РЕЧ_БЕЛ" xfId="1279"/>
+    <cellStyle name="_Февраль_РЕЧ_РЕЧ" xfId="1280"/>
+    <cellStyle name="_Февраль_СИ" xfId="1281"/>
+    <cellStyle name="_Февраль_СИ_БЕЛ" xfId="1282"/>
+    <cellStyle name="_Февраль_СИ_РЕЧ" xfId="1283"/>
+    <cellStyle name="_Февраль_СР" xfId="1284"/>
+    <cellStyle name="_Февраль_СУБД" xfId="1285"/>
+    <cellStyle name="_Февраль_СУБД_БЕЛ" xfId="1286"/>
+    <cellStyle name="_Февраль_СУБД_РЕЧ" xfId="1287"/>
+    <cellStyle name="_ФШ" xfId="1288"/>
+    <cellStyle name="_ФШ_Апрель" xfId="1289"/>
+    <cellStyle name="_ФШ_Апрель_БЕЛ" xfId="1290"/>
+    <cellStyle name="_ФШ_Апрель_РЕЧ" xfId="1291"/>
+    <cellStyle name="_ФШ_БЕЛ" xfId="1292"/>
+    <cellStyle name="_ФШ_Июль" xfId="1293"/>
+    <cellStyle name="_ФШ_Июль_БЕЛ" xfId="1294"/>
+    <cellStyle name="_ФШ_Июль_РЕЧ" xfId="1295"/>
+    <cellStyle name="_ФШ_Июнь" xfId="1296"/>
+    <cellStyle name="_ФШ_Июнь_БЕЛ" xfId="1297"/>
+    <cellStyle name="_ФШ_Июнь_РЕЧ" xfId="1298"/>
+    <cellStyle name="_ФШ_Май" xfId="1299"/>
+    <cellStyle name="_ФШ_Май_БЕЛ" xfId="1300"/>
+    <cellStyle name="_ФШ_Май_РЕЧ" xfId="1301"/>
+    <cellStyle name="_ФШ_РЕЧ" xfId="1302"/>
+    <cellStyle name="_ФШ_Февраль" xfId="1303"/>
+    <cellStyle name="_ФШ_Февраль_БЕЛ" xfId="1304"/>
+    <cellStyle name="_ФШ_Февраль_РЕЧ" xfId="1305"/>
+    <cellStyle name="_ФШ_Январь" xfId="1306"/>
+    <cellStyle name="_ФШ_Январь_БЕЛ" xfId="1307"/>
+    <cellStyle name="_ФШ_Январь_РЕЧ" xfId="1308"/>
+    <cellStyle name="_Январь" xfId="1309"/>
+    <cellStyle name="_Январь_3ДМ" xfId="1310"/>
+    <cellStyle name="_Январь_3ДМ_БЕЛ" xfId="1311"/>
+    <cellStyle name="_Январь_3ДМ_РЕЧ" xfId="1312"/>
+    <cellStyle name="_Январь_Август" xfId="1313"/>
+    <cellStyle name="_Январь_Август_Дистанц." xfId="1314"/>
+    <cellStyle name="_Январь_Август_Индив." xfId="1315"/>
+    <cellStyle name="_Январь_АКАД" xfId="1316"/>
+    <cellStyle name="_Январь_АКАД_БЕЛ" xfId="1317"/>
+    <cellStyle name="_Январь_АКАД_РЕЧ" xfId="1318"/>
+    <cellStyle name="_Январь_Апрель" xfId="1319"/>
+    <cellStyle name="_Январь_Апрель_3ДМ" xfId="1320"/>
+    <cellStyle name="_Январь_Апрель_3ДМ_БЕЛ" xfId="1321"/>
+    <cellStyle name="_Январь_Апрель_3ДМ_РЕЧ" xfId="1322"/>
+    <cellStyle name="_Январь_Апрель_Август" xfId="1323"/>
+    <cellStyle name="_Январь_Апрель_Август_Дистанц." xfId="1324"/>
+    <cellStyle name="_Январь_Апрель_Август_Индив." xfId="1325"/>
+    <cellStyle name="_Январь_Апрель_АКАД" xfId="1326"/>
+    <cellStyle name="_Январь_Апрель_АКАД_БЕЛ" xfId="1327"/>
+    <cellStyle name="_Январь_Апрель_АКАД_РЕЧ" xfId="1328"/>
+    <cellStyle name="_Январь_Апрель_Б9560" xfId="1329"/>
+    <cellStyle name="_Январь_Апрель_Б9560_БЕЛ" xfId="1330"/>
+    <cellStyle name="_Январь_Апрель_Б9560_РЕЧ" xfId="1331"/>
+    <cellStyle name="_Январь_Апрель_БЕЛ" xfId="1332"/>
+    <cellStyle name="_Январь_Апрель_БИНТ" xfId="1333"/>
+    <cellStyle name="_Январь_Апрель_БИНТ_БЕЛ" xfId="1334"/>
+    <cellStyle name="_Январь_Апрель_БИНТ_РЕЧ" xfId="1335"/>
+    <cellStyle name="_Январь_Апрель_БУХ" xfId="1336"/>
+    <cellStyle name="_Январь_Апрель_БУХ_БЕЛ" xfId="1337"/>
+    <cellStyle name="_Январь_Апрель_БУХ_РЕЧ" xfId="1338"/>
+    <cellStyle name="_Январь_Апрель_ВЕБДИЗ" xfId="1339"/>
+    <cellStyle name="_Январь_Апрель_ВЕБДИЗ_БЕЛ" xfId="1340"/>
+    <cellStyle name="_Январь_Апрель_ВЕБДИЗ_РЕЧ" xfId="1341"/>
+    <cellStyle name="_Январь_Апрель_ВЕБМАСТ" xfId="1342"/>
+    <cellStyle name="_Январь_Апрель_ВЕБМАСТ_БЕЛ" xfId="1343"/>
+    <cellStyle name="_Январь_Апрель_ВЕБМАСТ_РЕЧ" xfId="1344"/>
+    <cellStyle name="_Январь_Апрель_ВУЕ" xfId="1345"/>
+    <cellStyle name="_Январь_Апрель_ВУЕ_БЕЛ" xfId="1346"/>
+    <cellStyle name="_Январь_Апрель_ВУЕ_РЕЧ" xfId="1347"/>
+    <cellStyle name="_Январь_Апрель_Дети" xfId="1348"/>
+    <cellStyle name="_Январь_Апрель_Дети_БЕЛ" xfId="1349"/>
+    <cellStyle name="_Январь_Апрель_Дети_РЕЧ" xfId="1350"/>
+    <cellStyle name="_Январь_Апрель_Дистанц." xfId="1351"/>
+    <cellStyle name="_Январь_Апрель_Индив." xfId="1352"/>
+    <cellStyle name="_Январь_Апрель_Индив._БЕЛ" xfId="1353"/>
+    <cellStyle name="_Январь_Апрель_Индив._РЕЧ" xfId="1354"/>
+    <cellStyle name="_Январь_Апрель_Июль" xfId="1355"/>
+    <cellStyle name="_Январь_Апрель_Июль_Август" xfId="1356"/>
+    <cellStyle name="_Январь_Апрель_Июль_Август_Дистанц." xfId="1357"/>
+    <cellStyle name="_Январь_Апрель_Июль_Август_Индив." xfId="1358"/>
+    <cellStyle name="_Январь_Апрель_Июль_БЕЛ" xfId="1359"/>
+    <cellStyle name="_Январь_Апрель_Июль_БИНТ" xfId="1360"/>
+    <cellStyle name="_Январь_Апрель_Июль_БИНТ_БЕЛ" xfId="1361"/>
+    <cellStyle name="_Январь_Апрель_Июль_БИНТ_РЕЧ" xfId="1362"/>
+    <cellStyle name="_Январь_Апрель_Июль_ВЕБДИЗ" xfId="1363"/>
+    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ" xfId="1364"/>
+    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ_БЕЛ" xfId="1365"/>
+    <cellStyle name="_Январь_Апрель_Июль_ВЕБМАСТ_РЕЧ" xfId="1366"/>
+    <cellStyle name="_Январь_Апрель_Июль_Дети" xfId="1367"/>
+    <cellStyle name="_Январь_Апрель_Июль_Дистанц." xfId="1368"/>
+    <cellStyle name="_Январь_Апрель_Июль_Индив." xfId="1369"/>
+    <cellStyle name="_Январь_Апрель_Июль_Индив._БЕЛ" xfId="1370"/>
+    <cellStyle name="_Январь_Апрель_Июль_Индив._РЕЧ" xfId="1371"/>
+    <cellStyle name="_Январь_Апрель_Июль_Июнь" xfId="1372"/>
+    <cellStyle name="_Январь_Апрель_Июль_Июнь_Август" xfId="1373"/>
+    <cellStyle name="_Январь_Апрель_Июль_Июнь_Дистанц." xfId="1374"/>
+    <cellStyle name="_Январь_Апрель_Июль_Июнь_Индив." xfId="1375"/>
+    <cellStyle name="_Январь_Апрель_Июль_Июнь_КБУ" xfId="1376"/>
+    <cellStyle name="_Январь_Апрель_Июль_КБУ" xfId="1377"/>
+    <cellStyle name="_Январь_Апрель_Июль_КРН" xfId="1378"/>
+    <cellStyle name="_Январь_Апрель_Июль_ОПШ" xfId="1379"/>
+    <cellStyle name="_Январь_Апрель_Июль_СР" xfId="1380"/>
+    <cellStyle name="_Январь_Апрель_Июнь" xfId="1381"/>
+    <cellStyle name="_Январь_Апрель_Июнь_1" xfId="1382"/>
+    <cellStyle name="_Январь_Апрель_Июнь_1_Август" xfId="1383"/>
+    <cellStyle name="_Январь_Апрель_Июнь_1_Дистанц." xfId="1384"/>
+    <cellStyle name="_Январь_Апрель_Июнь_1_Индив." xfId="1385"/>
+    <cellStyle name="_Январь_Апрель_Июнь_1_КБУ" xfId="1386"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Август" xfId="1387"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Август_Дистанц." xfId="1388"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Август_Индив." xfId="1389"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БЕЛ" xfId="1390"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БИНТ" xfId="1391"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БИНТ_БЕЛ" xfId="1392"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БИНТ_РЕЧ" xfId="1393"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БУХ" xfId="1394"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БУХ_БЕЛ" xfId="1395"/>
+    <cellStyle name="_Январь_Апрель_Июнь_БУХ_РЕЧ" xfId="1396"/>
+    <cellStyle name="_Январь_Апрель_Июнь_ВЕБДИЗ" xfId="1397"/>
+    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ" xfId="1398"/>
+    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ_БЕЛ" xfId="1399"/>
+    <cellStyle name="_Январь_Апрель_Июнь_ВЕБМАСТ_РЕЧ" xfId="1400"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Дети" xfId="1401"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Дистанц." xfId="1402"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Индив." xfId="1403"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Индив._БЕЛ" xfId="1404"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Индив._РЕЧ" xfId="1405"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Июнь" xfId="1406"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Август" xfId="1407"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Дистанц." xfId="1408"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Июнь_Индив." xfId="1409"/>
+    <cellStyle name="_Январь_Апрель_Июнь_Июнь_КБУ" xfId="1410"/>
+    <cellStyle name="_Январь_Апрель_Июнь_КБУ" xfId="1411"/>
+    <cellStyle name="_Январь_Апрель_Июнь_КРН" xfId="1412"/>
+    <cellStyle name="_Январь_Апрель_Июнь_ОПШ" xfId="1413"/>
+    <cellStyle name="_Январь_Апрель_Июнь_СР" xfId="1414"/>
+    <cellStyle name="_Январь_Апрель_КБУ" xfId="1415"/>
+    <cellStyle name="_Январь_Апрель_КБУ_БЕЛ" xfId="1416"/>
+    <cellStyle name="_Январь_Апрель_КБУ_РЕЧ" xfId="1417"/>
+    <cellStyle name="_Январь_Апрель_КРН" xfId="1418"/>
+    <cellStyle name="_Январь_Апрель_Май" xfId="1419"/>
+    <cellStyle name="_Январь_Апрель_Май_1" xfId="1420"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Август" xfId="1421"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Август_Дистанц." xfId="1422"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Август_Индив." xfId="1423"/>
+    <cellStyle name="_Январь_Апрель_Май_1_БЕЛ" xfId="1424"/>
+    <cellStyle name="_Январь_Апрель_Май_1_БИНТ" xfId="1425"/>
+    <cellStyle name="_Январь_Апрель_Май_1_БИНТ_БЕЛ" xfId="1426"/>
+    <cellStyle name="_Январь_Апрель_Май_1_БИНТ_РЕЧ" xfId="1427"/>
+    <cellStyle name="_Январь_Апрель_Май_1_ВЕБДИЗ" xfId="1428"/>
+    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ" xfId="1429"/>
+    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ_БЕЛ" xfId="1430"/>
+    <cellStyle name="_Январь_Апрель_Май_1_ВЕБМАСТ_РЕЧ" xfId="1431"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Дети" xfId="1432"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Дистанц." xfId="1433"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Индив." xfId="1434"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Индив._БЕЛ" xfId="1435"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Индив._РЕЧ" xfId="1436"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Июнь" xfId="1437"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Август" xfId="1438"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Дистанц." xfId="1439"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Июнь_Индив." xfId="1440"/>
+    <cellStyle name="_Январь_Апрель_Май_1_Июнь_КБУ" xfId="1441"/>
+    <cellStyle name="_Январь_Апрель_Май_1_КБУ" xfId="1442"/>
+    <cellStyle name="_Январь_Апрель_Май_1_КРН" xfId="1443"/>
+    <cellStyle name="_Январь_Апрель_Май_1_ОПШ" xfId="1444"/>
+    <cellStyle name="_Январь_Апрель_Май_1_СР" xfId="1445"/>
+    <cellStyle name="_Январь_Апрель_Май_Август" xfId="1446"/>
+    <cellStyle name="_Январь_Апрель_Май_Август_Дистанц." xfId="1447"/>
+    <cellStyle name="_Январь_Апрель_Май_Август_Индив." xfId="1448"/>
+    <cellStyle name="_Январь_Апрель_Май_АКАД" xfId="1449"/>
+    <cellStyle name="_Январь_Апрель_Май_АКАД_БЕЛ" xfId="1450"/>
+    <cellStyle name="_Январь_Апрель_Май_АКАД_РЕЧ" xfId="1451"/>
+    <cellStyle name="_Январь_Апрель_Май_Б9560" xfId="1452"/>
+    <cellStyle name="_Январь_Апрель_Май_Б9560_БЕЛ" xfId="1453"/>
+    <cellStyle name="_Январь_Апрель_Май_Б9560_РЕЧ" xfId="1454"/>
+    <cellStyle name="_Январь_Апрель_Май_БЕЛ" xfId="1455"/>
+    <cellStyle name="_Январь_Апрель_Май_БИНТ" xfId="1456"/>
+    <cellStyle name="_Январь_Апрель_Май_БИНТ_БЕЛ" xfId="1457"/>
+    <cellStyle name="_Январь_Апрель_Май_БИНТ_РЕЧ" xfId="1458"/>
+    <cellStyle name="_Январь_Апрель_Май_БУХ" xfId="1459"/>
+    <cellStyle name="_Январь_Апрель_Май_БУХ_БЕЛ" xfId="1460"/>
+    <cellStyle name="_Январь_Апрель_Май_БУХ_РЕЧ" xfId="1461"/>
+    <cellStyle name="_Январь_Апрель_Май_ВЕБДИЗ" xfId="1462"/>
+    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ" xfId="1463"/>
+    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ_БЕЛ" xfId="1464"/>
+    <cellStyle name="_Январь_Апрель_Май_ВЕБМАСТ_РЕЧ" xfId="1465"/>
+    <cellStyle name="_Январь_Апрель_Май_Дети" xfId="1466"/>
+    <cellStyle name="_Январь_Апрель_Май_Дистанц." xfId="1467"/>
+    <cellStyle name="_Январь_Апрель_Май_Индив." xfId="1468"/>
+    <cellStyle name="_Январь_Апрель_Май_Индив._БЕЛ" xfId="1469"/>
+    <cellStyle name="_Январь_Апрель_Май_Индив._РЕЧ" xfId="1470"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль" xfId="1471"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Август" xfId="1472"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Август_Дистанц." xfId="1473"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Август_Индив." xfId="1474"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_БЕЛ" xfId="1475"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ" xfId="1476"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ_БЕЛ" xfId="1477"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_БИНТ_РЕЧ" xfId="1478"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБДИЗ" xfId="1479"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ" xfId="1480"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="1481"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="1482"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Дети" xfId="1483"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Дистанц." xfId="1484"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Индив." xfId="1485"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Индив._БЕЛ" xfId="1486"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Индив._РЕЧ" xfId="1487"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь" xfId="1488"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Август" xfId="1489"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Дистанц." xfId="1490"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_Индив." xfId="1491"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_Июнь_КБУ" xfId="1492"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_КБУ" xfId="1493"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_КРН" xfId="1494"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_ОПШ" xfId="1495"/>
+    <cellStyle name="_Январь_Апрель_Май_Июль_СР" xfId="1496"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь" xfId="1497"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_1" xfId="1498"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Август" xfId="1499"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Дистанц." xfId="1500"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_1_Индив." xfId="1501"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_1_КБУ" xfId="1502"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Август" xfId="1503"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Август_Дистанц." xfId="1504"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Август_Индив." xfId="1505"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БЕЛ" xfId="1506"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ" xfId="1507"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ_БЕЛ" xfId="1508"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БИНТ_РЕЧ" xfId="1509"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ" xfId="1510"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ_БЕЛ" xfId="1511"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_БУХ_РЕЧ" xfId="1512"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБДИЗ" xfId="1513"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ" xfId="1514"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="1515"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="1516"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Дети" xfId="1517"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Дистанц." xfId="1518"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив." xfId="1519"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив._БЕЛ" xfId="1520"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Индив._РЕЧ" xfId="1521"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь" xfId="1522"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Август" xfId="1523"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Дистанц." xfId="1524"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_Индив." xfId="1525"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_Июнь_КБУ" xfId="1526"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_КБУ" xfId="1527"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_КРН" xfId="1528"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_ОПШ" xfId="1529"/>
+    <cellStyle name="_Январь_Апрель_Май_Июнь_СР" xfId="1530"/>
+    <cellStyle name="_Январь_Апрель_Май_КБУ" xfId="1531"/>
+    <cellStyle name="_Январь_Апрель_Май_КРН" xfId="1532"/>
+    <cellStyle name="_Январь_Апрель_Май_Май" xfId="1533"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Август" xfId="1534"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Август_Дистанц." xfId="1535"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Август_Индив." xfId="1536"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_БЕЛ" xfId="1537"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ" xfId="1538"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ_БЕЛ" xfId="1539"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_БИНТ_РЕЧ" xfId="1540"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБДИЗ" xfId="1541"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ" xfId="1542"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ_БЕЛ" xfId="1543"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_ВЕБМАСТ_РЕЧ" xfId="1544"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Дети" xfId="1545"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Дистанц." xfId="1546"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Индив." xfId="1547"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Индив._БЕЛ" xfId="1548"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Индив._РЕЧ" xfId="1549"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Июнь" xfId="1550"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Август" xfId="1551"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Дистанц." xfId="1552"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_Индив." xfId="1553"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_Июнь_КБУ" xfId="1554"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_КБУ" xfId="1555"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_КРН" xfId="1556"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_ОПШ" xfId="1557"/>
+    <cellStyle name="_Январь_Апрель_Май_Май_СР" xfId="1558"/>
+    <cellStyle name="_Январь_Апрель_Май_ОПШ" xfId="1559"/>
+    <cellStyle name="_Январь_Апрель_Май_РЕЧ" xfId="1560"/>
+    <cellStyle name="_Январь_Апрель_Май_РЕЧ_БЕЛ" xfId="1561"/>
+    <cellStyle name="_Январь_Апрель_Май_РЕЧ_РЕЧ" xfId="1562"/>
+    <cellStyle name="_Январь_Апрель_Май_СИ" xfId="1563"/>
+    <cellStyle name="_Январь_Апрель_Май_СИ_БЕЛ" xfId="1564"/>
+    <cellStyle name="_Январь_Апрель_Май_СИ_РЕЧ" xfId="1565"/>
+    <cellStyle name="_Январь_Апрель_Май_СР" xfId="1566"/>
+    <cellStyle name="_Январь_Апрель_Май_СУБД" xfId="1567"/>
+    <cellStyle name="_Январь_Апрель_Май_СУБД_БЕЛ" xfId="1568"/>
+    <cellStyle name="_Январь_Апрель_Май_СУБД_РЕЧ" xfId="1569"/>
+    <cellStyle name="_Январь_Апрель_НТ" xfId="1570"/>
+    <cellStyle name="_Январь_Апрель_НТ_БЕЛ" xfId="1571"/>
+    <cellStyle name="_Январь_Апрель_НТ_РЕЧ" xfId="1572"/>
+    <cellStyle name="_Январь_Апрель_ОПШ" xfId="1573"/>
+    <cellStyle name="_Январь_Апрель_Офис" xfId="1574"/>
+    <cellStyle name="_Январь_Апрель_Офис_БЕЛ" xfId="1575"/>
+    <cellStyle name="_Январь_Апрель_Офис_РЕЧ" xfId="1576"/>
+    <cellStyle name="_Январь_Апрель_РЕЧ" xfId="1577"/>
+    <cellStyle name="_Январь_Апрель_РЕЧ_БЕЛ" xfId="1578"/>
+    <cellStyle name="_Январь_Апрель_РЕЧ_РЕЧ" xfId="1579"/>
+    <cellStyle name="_Январь_Апрель_СИ" xfId="1580"/>
+    <cellStyle name="_Январь_Апрель_СИ_БЕЛ" xfId="1581"/>
+    <cellStyle name="_Январь_Апрель_СИ_РЕЧ" xfId="1582"/>
+    <cellStyle name="_Январь_Апрель_СИС" xfId="1583"/>
+    <cellStyle name="_Январь_Апрель_СИС_БЕЛ" xfId="1584"/>
+    <cellStyle name="_Январь_Апрель_СИС_РЕЧ" xfId="1585"/>
+    <cellStyle name="_Январь_Апрель_СР" xfId="1586"/>
+    <cellStyle name="_Январь_Апрель_СУБД" xfId="1587"/>
+    <cellStyle name="_Январь_Апрель_СУБД_БЕЛ" xfId="1588"/>
+    <cellStyle name="_Январь_Апрель_СУБД_РЕЧ" xfId="1589"/>
+    <cellStyle name="_Январь_Апрель_ТЕК" xfId="1590"/>
+    <cellStyle name="_Январь_Апрель_ТЕК_БЕЛ" xfId="1591"/>
+    <cellStyle name="_Январь_Апрель_ТЕК_РЕЧ" xfId="1592"/>
+    <cellStyle name="_Январь_Апрель_Февраль" xfId="1593"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Август" xfId="1594"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Август_Дистанц." xfId="1595"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Август_Индив." xfId="1596"/>
+    <cellStyle name="_Январь_Апрель_Февраль_АКАД" xfId="1597"/>
+    <cellStyle name="_Январь_Апрель_Февраль_АКАД_БЕЛ" xfId="1598"/>
+    <cellStyle name="_Январь_Апрель_Февраль_АКАД_РЕЧ" xfId="1599"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Б9560" xfId="1600"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Б9560_БЕЛ" xfId="1601"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Б9560_РЕЧ" xfId="1602"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БЕЛ" xfId="1603"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БИНТ" xfId="1604"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БИНТ_БЕЛ" xfId="1605"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БИНТ_РЕЧ" xfId="1606"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БУХ" xfId="1607"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БУХ_БЕЛ" xfId="1608"/>
+    <cellStyle name="_Январь_Апрель_Февраль_БУХ_РЕЧ" xfId="1609"/>
+    <cellStyle name="_Январь_Апрель_Февраль_ВЕБДИЗ" xfId="1610"/>
+    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ" xfId="1611"/>
+    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ_БЕЛ" xfId="1612"/>
+    <cellStyle name="_Январь_Апрель_Февраль_ВЕБМАСТ_РЕЧ" xfId="1613"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Дети" xfId="1614"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Дистанц." xfId="1615"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Индив." xfId="1616"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Индив._БЕЛ" xfId="1617"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Индив._РЕЧ" xfId="1618"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль" xfId="1619"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август" xfId="1620"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август_Дистанц." xfId="1621"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Август_Индив." xfId="1622"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_БЕЛ" xfId="1623"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ" xfId="1624"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ_БЕЛ" xfId="1625"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_БИНТ_РЕЧ" xfId="1626"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБДИЗ" xfId="1627"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ" xfId="1628"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ_БЕЛ" xfId="1629"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_ВЕБМАСТ_РЕЧ" xfId="1630"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Дети" xfId="1631"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Дистанц." xfId="1632"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив." xfId="1633"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив._БЕЛ" xfId="1634"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Индив._РЕЧ" xfId="1635"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь" xfId="1636"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Август" xfId="1637"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Дистанц." xfId="1638"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_Индив." xfId="1639"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_Июнь_КБУ" xfId="1640"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_КБУ" xfId="1641"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_КРН" xfId="1642"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_ОПШ" xfId="1643"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июль_СР" xfId="1644"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь" xfId="1645"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1" xfId="1646"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Август" xfId="1647"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Дистанц." xfId="1648"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_Индив." xfId="1649"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_1_КБУ" xfId="1650"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август" xfId="1651"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август_Дистанц." xfId="1652"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Август_Индив." xfId="1653"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БЕЛ" xfId="1654"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ" xfId="1655"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ_БЕЛ" xfId="1656"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БИНТ_РЕЧ" xfId="1657"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ" xfId="1658"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ_БЕЛ" xfId="1659"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_БУХ_РЕЧ" xfId="1660"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБДИЗ" xfId="1661"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ" xfId="1662"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ_БЕЛ" xfId="1663"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ВЕБМАСТ_РЕЧ" xfId="1664"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Дети" xfId="1665"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Дистанц." xfId="1666"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив." xfId="1667"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив._БЕЛ" xfId="1668"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Индив._РЕЧ" xfId="1669"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь" xfId="1670"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Август" xfId="1671"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Дистанц." xfId="1672"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_Индив." xfId="1673"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_Июнь_КБУ" xfId="1674"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_КБУ" xfId="1675"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_КРН" xfId="1676"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_ОПШ" xfId="1677"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Июнь_СР" xfId="1678"/>
+    <cellStyle name="_Январь_Апрель_Февраль_КБУ" xfId="1679"/>
+    <cellStyle name="_Январь_Апрель_Февраль_КРН" xfId="1680"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май" xfId="1681"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Август" xfId="1682"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Август_Дистанц." xfId="1683"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Август_Индив." xfId="1684"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_БЕЛ" xfId="1685"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ" xfId="1686"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ_БЕЛ" xfId="1687"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_БИНТ_РЕЧ" xfId="1688"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБДИЗ" xfId="1689"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ" xfId="1690"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ_БЕЛ" xfId="1691"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_ВЕБМАСТ_РЕЧ" xfId="1692"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Дети" xfId="1693"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Дистанц." xfId="1694"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив." xfId="1695"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив._БЕЛ" xfId="1696"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Индив._РЕЧ" xfId="1697"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь" xfId="1698"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Август" xfId="1699"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Дистанц." xfId="1700"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_Индив." xfId="1701"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_Июнь_КБУ" xfId="1702"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_КБУ" xfId="1703"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_КРН" xfId="1704"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_ОПШ" xfId="1705"/>
+    <cellStyle name="_Январь_Апрель_Февраль_Май_СР" xfId="1706"/>
+    <cellStyle name="_Январь_Апрель_Февраль_ОПШ" xfId="1707"/>
+    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ" xfId="1708"/>
+    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ_БЕЛ" xfId="1709"/>
+    <cellStyle name="_Январь_Апрель_Февраль_РЕЧ_РЕЧ" xfId="1710"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СИ" xfId="1711"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СИ_БЕЛ" xfId="1712"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СИ_РЕЧ" xfId="1713"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СР" xfId="1714"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СУБД" xfId="1715"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СУБД_БЕЛ" xfId="1716"/>
+    <cellStyle name="_Январь_Апрель_Февраль_СУБД_РЕЧ" xfId="1717"/>
+    <cellStyle name="_Январь_Апрель_ФШ" xfId="1718"/>
+    <cellStyle name="_Январь_Апрель_ФШ_БЕЛ" xfId="1719"/>
+    <cellStyle name="_Январь_Апрель_ФШ_РЕЧ" xfId="1720"/>
+    <cellStyle name="_Январь_Б9560" xfId="1721"/>
+    <cellStyle name="_Январь_Б9560_БЕЛ" xfId="1722"/>
+    <cellStyle name="_Январь_Б9560_РЕЧ" xfId="1723"/>
+    <cellStyle name="_Январь_БЕЛ" xfId="1724"/>
+    <cellStyle name="_Январь_БЕЛ_БЕЛ" xfId="1725"/>
+    <cellStyle name="_Январь_БЕЛ_РЕЧ" xfId="1726"/>
+    <cellStyle name="_Январь_БИНТ" xfId="1727"/>
+    <cellStyle name="_Январь_БИНТ_БЕЛ" xfId="1728"/>
+    <cellStyle name="_Январь_БИНТ_РЕЧ" xfId="1729"/>
+    <cellStyle name="_Январь_БУХ" xfId="1730"/>
+    <cellStyle name="_Январь_БУХ_БЕЛ" xfId="1731"/>
+    <cellStyle name="_Январь_БУХ_РЕЧ" xfId="1732"/>
+    <cellStyle name="_Январь_ВЕБДИЗ" xfId="1733"/>
+    <cellStyle name="_Январь_ВЕБДИЗ_БЕЛ" xfId="1734"/>
+    <cellStyle name="_Январь_ВЕБДИЗ_РЕЧ" xfId="1735"/>
+    <cellStyle name="_Январь_ВЕБМАСТ" xfId="1736"/>
+    <cellStyle name="_Январь_ВЕБМАСТ_БЕЛ" xfId="1737"/>
+    <cellStyle name="_Январь_ВЕБМАСТ_РЕЧ" xfId="1738"/>
+    <cellStyle name="_Январь_ВУЕ" xfId="1739"/>
+    <cellStyle name="_Январь_ВУЕ_БЕЛ" xfId="1740"/>
+    <cellStyle name="_Январь_ВУЕ_РЕЧ" xfId="1741"/>
+    <cellStyle name="_Январь_Дети" xfId="1742"/>
+    <cellStyle name="_Январь_Дети_БЕЛ" xfId="1743"/>
+    <cellStyle name="_Январь_Дети_РЕЧ" xfId="1744"/>
+    <cellStyle name="_Январь_Дистанц." xfId="1745"/>
+    <cellStyle name="_Январь_Заявление" xfId="1746"/>
+    <cellStyle name="_Январь_Заявление_БЕЛ" xfId="1747"/>
+    <cellStyle name="_Январь_Заявление_РЕЧ" xfId="1748"/>
+    <cellStyle name="_Январь_Индив." xfId="1749"/>
+    <cellStyle name="_Январь_Индив._БЕЛ" xfId="1750"/>
+    <cellStyle name="_Январь_Индив._РЕЧ" xfId="1751"/>
+    <cellStyle name="_Январь_ИНТ" xfId="1752"/>
+    <cellStyle name="_Январь_ИНТ_БЕЛ" xfId="1753"/>
+    <cellStyle name="_Январь_ИНТ_РЕЧ" xfId="1754"/>
+    <cellStyle name="_Январь_Июль" xfId="1755"/>
+    <cellStyle name="_Январь_Июль_Август" xfId="1756"/>
+    <cellStyle name="_Январь_Июль_Август_Дистанц." xfId="1757"/>
+    <cellStyle name="_Январь_Июль_Август_Индив." xfId="1758"/>
+    <cellStyle name="_Январь_Июль_БЕЛ" xfId="1759"/>
+    <cellStyle name="_Январь_Июль_БИНТ" xfId="1760"/>
+    <cellStyle name="_Январь_Июль_БИНТ_БЕЛ" xfId="1761"/>
+    <cellStyle name="_Январь_Июль_БИНТ_РЕЧ" xfId="1762"/>
+    <cellStyle name="_Январь_Июль_ВЕБДИЗ" xfId="1763"/>
+    <cellStyle name="_Январь_Июль_ВЕБМАСТ" xfId="1764"/>
+    <cellStyle name="_Январь_Июль_ВЕБМАСТ_БЕЛ" xfId="1765"/>
+    <cellStyle name="_Январь_Июль_ВЕБМАСТ_РЕЧ" xfId="1766"/>
+    <cellStyle name="_Январь_Июль_Дети" xfId="1767"/>
+    <cellStyle name="_Январь_Июль_Дистанц." xfId="1768"/>
+    <cellStyle name="_Январь_Июль_Индив." xfId="1769"/>
+    <cellStyle name="_Январь_Июль_Индив._БЕЛ" xfId="1770"/>
+    <cellStyle name="_Январь_Июль_Индив._РЕЧ" xfId="1771"/>
+    <cellStyle name="_Январь_Июль_Июнь" xfId="1772"/>
+    <cellStyle name="_Январь_Июль_Июнь_Август" xfId="1773"/>
+    <cellStyle name="_Январь_Июль_Июнь_Дистанц." xfId="1774"/>
+    <cellStyle name="_Январь_Июль_Июнь_Индив." xfId="1775"/>
+    <cellStyle name="_Январь_Июль_Июнь_КБУ" xfId="1776"/>
+    <cellStyle name="_Январь_Июль_КБУ" xfId="1777"/>
+    <cellStyle name="_Январь_Июль_КРН" xfId="1778"/>
+    <cellStyle name="_Январь_Июль_ОПШ" xfId="1779"/>
+    <cellStyle name="_Январь_Июль_СР" xfId="1780"/>
+    <cellStyle name="_Январь_Июнь" xfId="1781"/>
+    <cellStyle name="_Январь_Июнь_1" xfId="1782"/>
+    <cellStyle name="_Январь_Июнь_1_Август" xfId="1783"/>
+    <cellStyle name="_Январь_Июнь_1_Дистанц." xfId="1784"/>
+    <cellStyle name="_Январь_Июнь_1_Индив." xfId="1785"/>
+    <cellStyle name="_Январь_Июнь_1_КБУ" xfId="1786"/>
+    <cellStyle name="_Январь_Июнь_Август" xfId="1787"/>
+    <cellStyle name="_Январь_Июнь_Август_Дистанц." xfId="1788"/>
+    <cellStyle name="_Январь_Июнь_Август_Индив." xfId="1789"/>
+    <cellStyle name="_Январь_Июнь_БЕЛ" xfId="1790"/>
+    <cellStyle name="_Январь_Июнь_БИНТ" xfId="1791"/>
+    <cellStyle name="_Январь_Июнь_БИНТ_БЕЛ" xfId="1792"/>
+    <cellStyle name="_Январь_Июнь_БИНТ_РЕЧ" xfId="1793"/>
+    <cellStyle name="_Январь_Июнь_БУХ" xfId="1794"/>
+    <cellStyle name="_Январь_Июнь_БУХ_БЕЛ" xfId="1795"/>
+    <cellStyle name="_Январь_Июнь_БУХ_РЕЧ" xfId="1796"/>
+    <cellStyle name="_Январь_Июнь_ВЕБДИЗ" xfId="1797"/>
+    <cellStyle name="_Январь_Июнь_ВЕБМАСТ" xfId="1798"/>
+    <cellStyle name="_Январь_Июнь_ВЕБМАСТ_БЕЛ" xfId="1799"/>
+    <cellStyle name="_Январь_Июнь_ВЕБМАСТ_РЕЧ" xfId="1800"/>
+    <cellStyle name="_Январь_Июнь_Дети" xfId="1801"/>
+    <cellStyle name="_Январь_Июнь_Дистанц." xfId="1802"/>
+    <cellStyle name="_Январь_Июнь_Индив." xfId="1803"/>
+    <cellStyle name="_Январь_Июнь_Индив._БЕЛ" xfId="1804"/>
+    <cellStyle name="_Январь_Июнь_Индив._РЕЧ" xfId="1805"/>
+    <cellStyle name="_Январь_Июнь_Июнь" xfId="1806"/>
+    <cellStyle name="_Январь_Июнь_Июнь_Август" xfId="1807"/>
+    <cellStyle name="_Январь_Июнь_Июнь_Дистанц." xfId="1808"/>
+    <cellStyle name="_Январь_Июнь_Июнь_Индив." xfId="1809"/>
+    <cellStyle name="_Январь_Июнь_Июнь_КБУ" xfId="1810"/>
+    <cellStyle name="_Январь_Июнь_КБУ" xfId="1811"/>
+    <cellStyle name="_Январь_Июнь_КРН" xfId="1812"/>
+    <cellStyle name="_Январь_Июнь_ОПШ" xfId="1813"/>
+    <cellStyle name="_Январь_Июнь_СР" xfId="1814"/>
+    <cellStyle name="_Январь_КБУ" xfId="1815"/>
+    <cellStyle name="_Январь_КБУ_БЕЛ" xfId="1816"/>
+    <cellStyle name="_Январь_КБУ_РЕЧ" xfId="1817"/>
+    <cellStyle name="_Январь_Консультация" xfId="1818"/>
+    <cellStyle name="_Январь_Консультация_БЕЛ" xfId="1819"/>
+    <cellStyle name="_Январь_Консультация_РЕЧ" xfId="1820"/>
+    <cellStyle name="_Январь_КРН" xfId="1821"/>
+    <cellStyle name="_Январь_КРН_БЕЛ" xfId="1822"/>
+    <cellStyle name="_Январь_КРН_РЕЧ" xfId="1823"/>
+    <cellStyle name="_Январь_ЛСХ" xfId="1824"/>
+    <cellStyle name="_Январь_ЛСХ_БЕЛ" xfId="1825"/>
+    <cellStyle name="_Январь_ЛСХ_РЕЧ" xfId="1826"/>
+    <cellStyle name="_Январь_Май" xfId="1827"/>
+    <cellStyle name="_Январь_Май_1" xfId="1828"/>
+    <cellStyle name="_Январь_Май_1_Август" xfId="1829"/>
+    <cellStyle name="_Январь_Май_1_Август_Дистанц." xfId="1830"/>
+    <cellStyle name="_Январь_Май_1_Август_Индив." xfId="1831"/>
+    <cellStyle name="_Январь_Май_1_БЕЛ" xfId="1832"/>
+    <cellStyle name="_Январь_Май_1_БИНТ" xfId="1833"/>
+    <cellStyle name="_Январь_Май_1_БИНТ_БЕЛ" xfId="1834"/>
+    <cellStyle name="_Январь_Май_1_БИНТ_РЕЧ" xfId="1835"/>
+    <cellStyle name="_Январь_Май_1_ВЕБДИЗ" xfId="1836"/>
+    <cellStyle name="_Январь_Май_1_ВЕБМАСТ" xfId="1837"/>
+    <cellStyle name="_Январь_Май_1_ВЕБМАСТ_БЕЛ" xfId="1838"/>
+    <cellStyle name="_Январь_Май_1_ВЕБМАСТ_РЕЧ" xfId="1839"/>
+    <cellStyle name="_Январь_Май_1_Дети" xfId="1840"/>
+    <cellStyle name="_Январь_Май_1_Дистанц." xfId="1841"/>
+    <cellStyle name="_Январь_Май_1_Индив." xfId="1842"/>
+    <cellStyle name="_Январь_Май_1_Индив._БЕЛ" xfId="1843"/>
+    <cellStyle name="_Январь_Май_1_Индив._РЕЧ" xfId="1844"/>
+    <cellStyle name="_Январь_Май_1_Июнь" xfId="1845"/>
+    <cellStyle name="_Январь_Май_1_Июнь_Август" xfId="1846"/>
+    <cellStyle name="_Январь_Май_1_Июнь_Дистанц." xfId="1847"/>
+    <cellStyle name="_Январь_Май_1_Июнь_Индив." xfId="1848"/>
+    <cellStyle name="_Январь_Май_1_Июнь_КБУ" xfId="1849"/>
+    <cellStyle name="_Январь_Май_1_КБУ" xfId="1850"/>
+    <cellStyle name="_Январь_Май_1_КРН" xfId="1851"/>
+    <cellStyle name="_Январь_Май_1_ОПШ" xfId="1852"/>
+    <cellStyle name="_Январь_Май_1_СР" xfId="1853"/>
+    <cellStyle name="_Январь_Май_Август" xfId="1854"/>
+    <cellStyle name="_Январь_Май_Август_Дистанц." xfId="1855"/>
+    <cellStyle name="_Январь_Май_Август_Индив." xfId="1856"/>
+    <cellStyle name="_Январь_Май_АКАД" xfId="1857"/>
+    <cellStyle name="_Январь_Май_АКАД_БЕЛ" xfId="1858"/>
+    <cellStyle name="_Январь_Май_АКАД_РЕЧ" xfId="1859"/>
+    <cellStyle name="_Январь_Май_Б9560" xfId="1860"/>
+    <cellStyle name="_Январь_Май_Б9560_БЕЛ" xfId="1861"/>
+    <cellStyle name="_Январь_Май_Б9560_РЕЧ" xfId="1862"/>
+    <cellStyle name="_Январь_Май_БЕЛ" xfId="1863"/>
+    <cellStyle name="_Январь_Май_БИНТ" xfId="1864"/>
+    <cellStyle name="_Январь_Май_БИНТ_БЕЛ" xfId="1865"/>
+    <cellStyle name="_Январь_Май_БИНТ_РЕЧ" xfId="1866"/>
+    <cellStyle name="_Январь_Май_БУХ" xfId="1867"/>
+    <cellStyle name="_Январь_Май_БУХ_БЕЛ" xfId="1868"/>
+    <cellStyle name="_Январь_Май_БУХ_РЕЧ" xfId="1869"/>
+    <cellStyle name="_Январь_Май_ВЕБДИЗ" xfId="1870"/>
+    <cellStyle name="_Январь_Май_ВЕБМАСТ" xfId="1871"/>
+    <cellStyle name="_Январь_Май_ВЕБМАСТ_БЕЛ" xfId="1872"/>
+    <cellStyle name="_Январь_Май_ВЕБМАСТ_РЕЧ" xfId="1873"/>
+    <cellStyle name="_Январь_Май_Дети" xfId="1874"/>
+    <cellStyle name="_Январь_Май_Дистанц." xfId="1875"/>
+    <cellStyle name="_Январь_Май_Индив." xfId="1876"/>
+    <cellStyle name="_Январь_Май_Индив._БЕЛ" xfId="1877"/>
+    <cellStyle name="_Январь_Май_Индив._РЕЧ" xfId="1878"/>
+    <cellStyle name="_Январь_Май_Июль" xfId="1879"/>
+    <cellStyle name="_Январь_Май_Июль_Август" xfId="1880"/>
+    <cellStyle name="_Январь_Май_Июль_Август_Дистанц." xfId="1881"/>
+    <cellStyle name="_Январь_Май_Июль_Август_Индив." xfId="1882"/>
+    <cellStyle name="_Январь_Май_Июль_БЕЛ" xfId="1883"/>
+    <cellStyle name="_Январь_Май_Июль_БИНТ" xfId="1884"/>
+    <cellStyle name="_Январь_Май_Июль_БИНТ_БЕЛ" xfId="1885"/>
+    <cellStyle name="_Январь_Май_Июль_БИНТ_РЕЧ" xfId="1886"/>
+    <cellStyle name="_Январь_Май_Июль_ВЕБДИЗ" xfId="1887"/>
+    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ" xfId="1888"/>
+    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ_БЕЛ" xfId="1889"/>
+    <cellStyle name="_Январь_Май_Июль_ВЕБМАСТ_РЕЧ" xfId="1890"/>
+    <cellStyle name="_Январь_Май_Июль_Дети" xfId="1891"/>
+    <cellStyle name="_Январь_Май_Июль_Дистанц." xfId="1892"/>
+    <cellStyle name="_Январь_Май_Июль_Индив." xfId="1893"/>
+    <cellStyle name="_Январь_Май_Июль_Индив._БЕЛ" xfId="1894"/>
+    <cellStyle name="_Январь_Май_Июль_Индив._РЕЧ" xfId="1895"/>
+    <cellStyle name="_Январь_Май_Июль_Июнь" xfId="1896"/>
+    <cellStyle name="_Январь_Май_Июль_Июнь_Август" xfId="1897"/>
+    <cellStyle name="_Январь_Май_Июль_Июнь_Дистанц." xfId="1898"/>
+    <cellStyle name="_Январь_Май_Июль_Июнь_Индив." xfId="1899"/>
+    <cellStyle name="_Январь_Май_Июль_Июнь_КБУ" xfId="1900"/>
+    <cellStyle name="_Январь_Май_Июль_КБУ" xfId="1901"/>
+    <cellStyle name="_Январь_Май_Июль_КРН" xfId="1902"/>
+    <cellStyle name="_Январь_Май_Июль_ОПШ" xfId="1903"/>
+    <cellStyle name="_Январь_Май_Июль_СР" xfId="1904"/>
+    <cellStyle name="_Январь_Май_Июнь" xfId="1905"/>
+    <cellStyle name="_Январь_Май_Июнь_1" xfId="1906"/>
+    <cellStyle name="_Январь_Май_Июнь_1_Август" xfId="1907"/>
+    <cellStyle name="_Январь_Май_Июнь_1_Дистанц." xfId="1908"/>
+    <cellStyle name="_Январь_Май_Июнь_1_Индив." xfId="1909"/>
+    <cellStyle name="_Январь_Май_Июнь_1_КБУ" xfId="1910"/>
+    <cellStyle name="_Январь_Май_Июнь_Август" xfId="1911"/>
+    <cellStyle name="_Январь_Май_Июнь_Август_Дистанц." xfId="1912"/>
+    <cellStyle name="_Январь_Май_Июнь_Август_Индив." xfId="1913"/>
+    <cellStyle name="_Январь_Май_Июнь_БЕЛ" xfId="1914"/>
+    <cellStyle name="_Январь_Май_Июнь_БИНТ" xfId="1915"/>
+    <cellStyle name="_Январь_Май_Июнь_БИНТ_БЕЛ" xfId="1916"/>
+    <cellStyle name="_Январь_Май_Июнь_БИНТ_РЕЧ" xfId="1917"/>
+    <cellStyle name="_Январь_Май_Июнь_БУХ" xfId="1918"/>
+    <cellStyle name="_Январь_Май_Июнь_БУХ_БЕЛ" xfId="1919"/>
+    <cellStyle name="_Январь_Май_Июнь_БУХ_РЕЧ" xfId="1920"/>
+    <cellStyle name="_Январь_Май_Июнь_ВЕБДИЗ" xfId="1921"/>
+    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ" xfId="1922"/>
+    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ_БЕЛ" xfId="1923"/>
+    <cellStyle name="_Январь_Май_Июнь_ВЕБМАСТ_РЕЧ" xfId="1924"/>
+    <cellStyle name="_Январь_Май_Июнь_Дети" xfId="1925"/>
+    <cellStyle name="_Январь_Май_Июнь_Дистанц." xfId="1926"/>
+    <cellStyle name="_Январь_Май_Июнь_Индив." xfId="1927"/>
+    <cellStyle name="_Январь_Май_Июнь_Индив._БЕЛ" xfId="1928"/>
+    <cellStyle name="_Январь_Май_Июнь_Индив._РЕЧ" xfId="1929"/>
+    <cellStyle name="_Январь_Май_Июнь_Июнь" xfId="1930"/>
+    <cellStyle name="_Январь_Май_Июнь_Июнь_Август" xfId="1931"/>
+    <cellStyle name="_Январь_Май_Июнь_Июнь_Дистанц." xfId="1932"/>
+    <cellStyle name="_Январь_Май_Июнь_Июнь_Индив." xfId="1933"/>
+    <cellStyle name="_Январь_Май_Июнь_Июнь_КБУ" xfId="1934"/>
+    <cellStyle name="_Январь_Май_Июнь_КБУ" xfId="1935"/>
+    <cellStyle name="_Январь_Май_Июнь_КРН" xfId="1936"/>
+    <cellStyle name="_Январь_Май_Июнь_ОПШ" xfId="1937"/>
+    <cellStyle name="_Январь_Май_Июнь_СР" xfId="1938"/>
+    <cellStyle name="_Январь_Май_КБУ" xfId="1939"/>
+    <cellStyle name="_Январь_Май_КРН" xfId="1940"/>
+    <cellStyle name="_Январь_Май_Май" xfId="1941"/>
+    <cellStyle name="_Январь_Май_Май_Август" xfId="1942"/>
+    <cellStyle name="_Январь_Май_Май_Август_Дистанц." xfId="1943"/>
+    <cellStyle name="_Январь_Май_Май_Август_Индив." xfId="1944"/>
+    <cellStyle name="_Январь_Май_Май_БЕЛ" xfId="1945"/>
+    <cellStyle name="_Январь_Май_Май_БИНТ" xfId="1946"/>
+    <cellStyle name="_Январь_Май_Май_БИНТ_БЕЛ" xfId="1947"/>
+    <cellStyle name="_Январь_Май_Май_БИНТ_РЕЧ" xfId="1948"/>
+    <cellStyle name="_Январь_Май_Май_ВЕБДИЗ" xfId="1949"/>
+    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ" xfId="1950"/>
+    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ_БЕЛ" xfId="1951"/>
+    <cellStyle name="_Январь_Май_Май_ВЕБМАСТ_РЕЧ" xfId="1952"/>
+    <cellStyle name="_Январь_Май_Май_Дети" xfId="1953"/>
+    <cellStyle name="_Январь_Май_Май_Дистанц." xfId="1954"/>
+    <cellStyle name="_Январь_Май_Май_Индив." xfId="1955"/>
+    <cellStyle name="_Январь_Май_Май_Индив._БЕЛ" xfId="1956"/>
+    <cellStyle name="_Январь_Май_Май_Индив._РЕЧ" xfId="1957"/>
+    <cellStyle name="_Январь_Май_Май_Июнь" xfId="1958"/>
+    <cellStyle name="_Январь_Май_Май_Июнь_Август" xfId="1959"/>
+    <cellStyle name="_Январь_Май_Май_Июнь_Дистанц." xfId="1960"/>
+    <cellStyle name="_Январь_Май_Май_Июнь_Индив." xfId="1961"/>
+    <cellStyle name="_Январь_Май_Май_Июнь_КБУ" xfId="1962"/>
+    <cellStyle name="_Январь_Май_Май_КБУ" xfId="1963"/>
+    <cellStyle name="_Январь_Май_Май_КРН" xfId="1964"/>
+    <cellStyle name="_Январь_Май_Май_ОПШ" xfId="1965"/>
+    <cellStyle name="_Январь_Май_Май_СР" xfId="1966"/>
+    <cellStyle name="_Январь_Май_ОПШ" xfId="1967"/>
+    <cellStyle name="_Январь_Май_РЕЧ" xfId="1968"/>
+    <cellStyle name="_Январь_Май_РЕЧ_БЕЛ" xfId="1969"/>
+    <cellStyle name="_Январь_Май_РЕЧ_РЕЧ" xfId="1970"/>
+    <cellStyle name="_Январь_Май_СИ" xfId="1971"/>
+    <cellStyle name="_Январь_Май_СИ_БЕЛ" xfId="1972"/>
+    <cellStyle name="_Январь_Май_СИ_РЕЧ" xfId="1973"/>
+    <cellStyle name="_Январь_Май_СР" xfId="1974"/>
+    <cellStyle name="_Январь_Май_СУБД" xfId="1975"/>
+    <cellStyle name="_Январь_Май_СУБД_БЕЛ" xfId="1976"/>
+    <cellStyle name="_Январь_Май_СУБД_РЕЧ" xfId="1977"/>
+    <cellStyle name="_Январь_МП" xfId="1978"/>
+    <cellStyle name="_Январь_МП_БЕЛ" xfId="1979"/>
+    <cellStyle name="_Январь_МП_РЕЧ" xfId="1980"/>
+    <cellStyle name="_Январь_НТ" xfId="1981"/>
+    <cellStyle name="_Январь_НТ_БЕЛ" xfId="1982"/>
+    <cellStyle name="_Январь_НТ_РЕЧ" xfId="1983"/>
+    <cellStyle name="_Январь_ОПШ" xfId="1984"/>
+    <cellStyle name="_Январь_ОПШ_БЕЛ" xfId="1985"/>
+    <cellStyle name="_Январь_ОПШ_РЕЧ" xfId="1986"/>
+    <cellStyle name="_Январь_Офис" xfId="1987"/>
+    <cellStyle name="_Январь_Офис_БЕЛ" xfId="1988"/>
+    <cellStyle name="_Январь_Офис_РЕЧ" xfId="1989"/>
+    <cellStyle name="_Январь_ПРШ" xfId="1990"/>
+    <cellStyle name="_Январь_ПРШ_БЕЛ" xfId="1991"/>
+    <cellStyle name="_Январь_ПРШ_РЕЧ" xfId="1992"/>
+    <cellStyle name="_Январь_РЕЧ" xfId="1993"/>
+    <cellStyle name="_Январь_РЕЧ_БЕЛ" xfId="1994"/>
+    <cellStyle name="_Январь_РЕЧ_РЕЧ" xfId="1995"/>
+    <cellStyle name="_Январь_СВБ" xfId="1996"/>
+    <cellStyle name="_Январь_СВБ_БЕЛ" xfId="1997"/>
+    <cellStyle name="_Январь_СВБ_РЕЧ" xfId="1998"/>
+    <cellStyle name="_Январь_СИ" xfId="1999"/>
+    <cellStyle name="_Январь_СИ_БЕЛ" xfId="2000"/>
+    <cellStyle name="_Январь_СИ_РЕЧ" xfId="2001"/>
+    <cellStyle name="_Январь_СИС" xfId="2002"/>
+    <cellStyle name="_Январь_СИС_БЕЛ" xfId="2003"/>
+    <cellStyle name="_Январь_СИС_РЕЧ" xfId="2004"/>
+    <cellStyle name="_Январь_СР" xfId="2005"/>
+    <cellStyle name="_Январь_СУБД" xfId="2006"/>
+    <cellStyle name="_Январь_СУБД_БЕЛ" xfId="2007"/>
+    <cellStyle name="_Январь_СУБД_РЕЧ" xfId="2008"/>
+    <cellStyle name="_Январь_ТЕК" xfId="2009"/>
+    <cellStyle name="_Январь_ТЕК_БЕЛ" xfId="2010"/>
+    <cellStyle name="_Январь_ТЕК_РЕЧ" xfId="2011"/>
+    <cellStyle name="_Январь_ТОР" xfId="2012"/>
+    <cellStyle name="_Январь_ТОР_БЕЛ" xfId="2013"/>
+    <cellStyle name="_Январь_ТОР_РЕЧ" xfId="2014"/>
+    <cellStyle name="_Январь_Февраль" xfId="2015"/>
+    <cellStyle name="_Январь_Февраль_1" xfId="2016"/>
+    <cellStyle name="_Январь_Февраль_1_Август" xfId="2017"/>
+    <cellStyle name="_Январь_Февраль_1_Август_Дистанц." xfId="2018"/>
+    <cellStyle name="_Январь_Февраль_1_Август_Индив." xfId="2019"/>
+    <cellStyle name="_Январь_Февраль_1_АКАД" xfId="2020"/>
+    <cellStyle name="_Январь_Февраль_1_АКАД_БЕЛ" xfId="2021"/>
+    <cellStyle name="_Январь_Февраль_1_АКАД_РЕЧ" xfId="2022"/>
+    <cellStyle name="_Январь_Февраль_1_Б9560" xfId="2023"/>
+    <cellStyle name="_Январь_Февраль_1_Б9560_БЕЛ" xfId="2024"/>
+    <cellStyle name="_Январь_Февраль_1_Б9560_РЕЧ" xfId="2025"/>
+    <cellStyle name="_Январь_Февраль_1_БЕЛ" xfId="2026"/>
+    <cellStyle name="_Январь_Февраль_1_БИНТ" xfId="2027"/>
+    <cellStyle name="_Январь_Февраль_1_БИНТ_БЕЛ" xfId="2028"/>
+    <cellStyle name="_Январь_Февраль_1_БИНТ_РЕЧ" xfId="2029"/>
+    <cellStyle name="_Январь_Февраль_1_БУХ" xfId="2030"/>
+    <cellStyle name="_Январь_Февраль_1_БУХ_БЕЛ" xfId="2031"/>
+    <cellStyle name="_Январь_Февраль_1_БУХ_РЕЧ" xfId="2032"/>
+    <cellStyle name="_Январь_Февраль_1_ВЕБДИЗ" xfId="2033"/>
+    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ" xfId="2034"/>
+    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ_БЕЛ" xfId="2035"/>
+    <cellStyle name="_Январь_Февраль_1_ВЕБМАСТ_РЕЧ" xfId="2036"/>
+    <cellStyle name="_Январь_Февраль_1_Дети" xfId="2037"/>
+    <cellStyle name="_Январь_Февраль_1_Дистанц." xfId="2038"/>
+    <cellStyle name="_Январь_Февраль_1_Индив." xfId="2039"/>
+    <cellStyle name="_Январь_Февраль_1_Индив._БЕЛ" xfId="2040"/>
+    <cellStyle name="_Январь_Февраль_1_Индив._РЕЧ" xfId="2041"/>
+    <cellStyle name="_Январь_Февраль_1_Июль" xfId="2042"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Август" xfId="2043"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Август_Дистанц." xfId="2044"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Август_Индив." xfId="2045"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_БЕЛ" xfId="2046"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ" xfId="2047"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ_БЕЛ" xfId="2048"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_БИНТ_РЕЧ" xfId="2049"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБДИЗ" xfId="2050"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ" xfId="2051"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ_БЕЛ" xfId="2052"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_ВЕБМАСТ_РЕЧ" xfId="2053"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Дети" xfId="2054"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Дистанц." xfId="2055"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Индив." xfId="2056"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Индив._БЕЛ" xfId="2057"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Индив._РЕЧ" xfId="2058"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Июнь" xfId="2059"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Август" xfId="2060"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Дистанц." xfId="2061"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_Индив." xfId="2062"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_Июнь_КБУ" xfId="2063"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_КБУ" xfId="2064"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_КРН" xfId="2065"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_ОПШ" xfId="2066"/>
+    <cellStyle name="_Январь_Февраль_1_Июль_СР" xfId="2067"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь" xfId="2068"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_1" xfId="2069"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_1_Август" xfId="2070"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_1_Дистанц." xfId="2071"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_1_Индив." xfId="2072"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_1_КБУ" xfId="2073"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Август" xfId="2074"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Август_Дистанц." xfId="2075"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Август_Индив." xfId="2076"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БЕЛ" xfId="2077"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ" xfId="2078"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ_БЕЛ" xfId="2079"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БИНТ_РЕЧ" xfId="2080"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ" xfId="2081"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ_БЕЛ" xfId="2082"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_БУХ_РЕЧ" xfId="2083"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБДИЗ" xfId="2084"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ" xfId="2085"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ_БЕЛ" xfId="2086"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_ВЕБМАСТ_РЕЧ" xfId="2087"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Дети" xfId="2088"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Дистанц." xfId="2089"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Индив." xfId="2090"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Индив._БЕЛ" xfId="2091"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Индив._РЕЧ" xfId="2092"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь" xfId="2093"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Август" xfId="2094"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Дистанц." xfId="2095"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_Индив." xfId="2096"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_Июнь_КБУ" xfId="2097"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_КБУ" xfId="2098"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_КРН" xfId="2099"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_ОПШ" xfId="2100"/>
+    <cellStyle name="_Январь_Февраль_1_Июнь_СР" xfId="2101"/>
+    <cellStyle name="_Январь_Февраль_1_КБУ" xfId="2102"/>
+    <cellStyle name="_Январь_Февраль_1_КРН" xfId="2103"/>
+    <cellStyle name="_Январь_Февраль_1_Май" xfId="2104"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Август" xfId="2105"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Август_Дистанц." xfId="2106"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Август_Индив." xfId="2107"/>
+    <cellStyle name="_Январь_Февраль_1_Май_БЕЛ" xfId="2108"/>
+    <cellStyle name="_Январь_Февраль_1_Май_БИНТ" xfId="2109"/>
+    <cellStyle name="_Январь_Февраль_1_Май_БИНТ_БЕЛ" xfId="2110"/>
+    <cellStyle name="_Январь_Февраль_1_Май_БИНТ_РЕЧ" xfId="2111"/>
+    <cellStyle name="_Январь_Февраль_1_Май_ВЕБДИЗ" xfId="2112"/>
+    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ" xfId="2113"/>
+    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ_БЕЛ" xfId="2114"/>
+    <cellStyle name="_Январь_Февраль_1_Май_ВЕБМАСТ_РЕЧ" xfId="2115"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Дети" xfId="2116"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Дистанц." xfId="2117"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Индив." xfId="2118"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Индив._БЕЛ" xfId="2119"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Индив._РЕЧ" xfId="2120"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Июнь" xfId="2121"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Август" xfId="2122"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Дистанц." xfId="2123"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Июнь_Индив." xfId="2124"/>
+    <cellStyle name="_Январь_Февраль_1_Май_Июнь_КБУ" xfId="2125"/>
+    <cellStyle name="_Январь_Февраль_1_Май_КБУ" xfId="2126"/>
+    <cellStyle name="_Январь_Февраль_1_Май_КРН" xfId="2127"/>
+    <cellStyle name="_Январь_Февраль_1_Май_ОПШ" xfId="2128"/>
+    <cellStyle name="_Январь_Февраль_1_Май_СР" xfId="2129"/>
+    <cellStyle name="_Январь_Февраль_1_ОПШ" xfId="2130"/>
+    <cellStyle name="_Январь_Февраль_1_РЕЧ" xfId="2131"/>
+    <cellStyle name="_Январь_Февраль_1_РЕЧ_БЕЛ" xfId="2132"/>
+    <cellStyle name="_Январь_Февраль_1_РЕЧ_РЕЧ" xfId="2133"/>
+    <cellStyle name="_Январь_Февраль_1_СИ" xfId="2134"/>
+    <cellStyle name="_Январь_Февраль_1_СИ_БЕЛ" xfId="2135"/>
+    <cellStyle name="_Январь_Февраль_1_СИ_РЕЧ" xfId="2136"/>
+    <cellStyle name="_Январь_Февраль_1_СР" xfId="2137"/>
+    <cellStyle name="_Январь_Февраль_1_СУБД" xfId="2138"/>
+    <cellStyle name="_Январь_Февраль_1_СУБД_БЕЛ" xfId="2139"/>
+    <cellStyle name="_Январь_Февраль_1_СУБД_РЕЧ" xfId="2140"/>
+    <cellStyle name="_Январь_Февраль_БЕЛ" xfId="2141"/>
+    <cellStyle name="_Январь_Февраль_РЕЧ" xfId="2142"/>
+    <cellStyle name="_Январь_ФШ" xfId="2143"/>
+    <cellStyle name="_Январь_ФШ_БЕЛ" xfId="2144"/>
+    <cellStyle name="_Январь_ФШ_РЕЧ" xfId="2145"/>
+    <cellStyle name="Currency0" xfId="2146"/>
+    <cellStyle name="Euro" xfId="2147"/>
+    <cellStyle name="Normal1" xfId="2148"/>
+    <cellStyle name="Акцент1 2" xfId="2161"/>
+    <cellStyle name="Денежный [0] 2" xfId="2153"/>
+    <cellStyle name="Денежный 2" xfId="2154"/>
+    <cellStyle name="Денежный 2 2" xfId="2167"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="2156" xr:uid="{00000000-0005-0000-0000-000069080000}"/>
-    <cellStyle name="Обычный 2 2" xfId="2169" xr:uid="{00000000-0005-0000-0000-00006A080000}"/>
-    <cellStyle name="Обычный 3" xfId="2158" xr:uid="{00000000-0005-0000-0000-00006B080000}"/>
-    <cellStyle name="Обычный 3 2" xfId="2168" xr:uid="{00000000-0005-0000-0000-00006C080000}"/>
-    <cellStyle name="Обычный 4" xfId="2160" xr:uid="{00000000-0005-0000-0000-00006D080000}"/>
-    <cellStyle name="Обычный 5" xfId="2163" xr:uid="{00000000-0005-0000-0000-00006E080000}"/>
-    <cellStyle name="Обычный 6" xfId="2164" xr:uid="{00000000-0005-0000-0000-00006F080000}"/>
-    <cellStyle name="Обычный 7" xfId="2171" xr:uid="{00000000-0005-0000-0000-000070080000}"/>
-    <cellStyle name="Обычный_DHL" xfId="2155" xr:uid="{00000000-0005-0000-0000-000071080000}"/>
-    <cellStyle name="Обычный_Excel 2000" xfId="2162" xr:uid="{00000000-0005-0000-0000-000072080000}"/>
+    <cellStyle name="Обычный 2" xfId="2156"/>
+    <cellStyle name="Обычный 2 2" xfId="2169"/>
+    <cellStyle name="Обычный 3" xfId="2158"/>
+    <cellStyle name="Обычный 3 2" xfId="2168"/>
+    <cellStyle name="Обычный 4" xfId="2160"/>
+    <cellStyle name="Обычный 5" xfId="2163"/>
+    <cellStyle name="Обычный 6" xfId="2164"/>
+    <cellStyle name="Обычный 7" xfId="2171"/>
+    <cellStyle name="Обычный_DHL" xfId="2155"/>
+    <cellStyle name="Обычный_Excel 2000" xfId="2162"/>
     <cellStyle name="Процентный" xfId="2170" builtinId="5"/>
-    <cellStyle name="Процентный 2" xfId="2157" xr:uid="{00000000-0005-0000-0000-000074080000}"/>
-    <cellStyle name="Процентный 3" xfId="2165" xr:uid="{00000000-0005-0000-0000-000075080000}"/>
-    <cellStyle name="Процентный 4" xfId="2172" xr:uid="{00000000-0005-0000-0000-000076080000}"/>
-    <cellStyle name="Стиль 1" xfId="2149" xr:uid="{00000000-0005-0000-0000-000077080000}"/>
-    <cellStyle name="Стиль_названий" xfId="2152" xr:uid="{00000000-0005-0000-0000-000078080000}"/>
-    <cellStyle name="Тысячи [0]_Лист1" xfId="2150" xr:uid="{00000000-0005-0000-0000-000079080000}"/>
-    <cellStyle name="Тысячи_Лист1" xfId="2151" xr:uid="{00000000-0005-0000-0000-00007A080000}"/>
+    <cellStyle name="Процентный 2" xfId="2157"/>
+    <cellStyle name="Процентный 3" xfId="2165"/>
+    <cellStyle name="Процентный 4" xfId="2172"/>
+    <cellStyle name="Стиль 1" xfId="2149"/>
+    <cellStyle name="Стиль_названий" xfId="2152"/>
+    <cellStyle name="Тысячи [0]_Лист1" xfId="2150"/>
+    <cellStyle name="Тысячи_Лист1" xfId="2151"/>
     <cellStyle name="Финансовый" xfId="2159" builtinId="3"/>
-    <cellStyle name="Финансовый 2" xfId="2166" xr:uid="{00000000-0005-0000-0000-00007C080000}"/>
-    <cellStyle name="Финансовый 3" xfId="2173" xr:uid="{00000000-0005-0000-0000-00007D080000}"/>
+    <cellStyle name="Финансовый 2" xfId="2166"/>
+    <cellStyle name="Финансовый 3" xfId="2173"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -55857,16 +55856,24 @@
           </cell>
         </row>
         <row r="14">
-          <cell r="B14"/>
+          <cell r="B14">
+            <v>0</v>
+          </cell>
         </row>
         <row r="15">
-          <cell r="B15"/>
+          <cell r="B15">
+            <v>0</v>
+          </cell>
         </row>
         <row r="16">
-          <cell r="B16"/>
+          <cell r="B16">
+            <v>0</v>
+          </cell>
         </row>
         <row r="17">
-          <cell r="B17"/>
+          <cell r="B17">
+            <v>0</v>
+          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="30"/>
@@ -55971,23 +55978,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -56023,23 +56013,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -56215,14 +56188,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист3">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -56814,7 +56787,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="19"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5">
+        <f>SUMPRODUCT(C3:C11,D3:D11)</f>
+        <v>280000</v>
+      </c>
       <c r="G13" s="3"/>
     </row>
   </sheetData>
@@ -56833,14 +56809,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78960C4-5B50-4062-A570-81A7173DAE01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -57357,7 +57333,10 @@
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="12">
+        <f>SUMPRODUCT((E2:E14/D2:D14&gt;$H$2)*1)</f>
+        <v>5</v>
+      </c>
       <c r="J3" s="15" t="s">
         <v>39</v>
       </c>
@@ -57383,7 +57362,10 @@
       <c r="H4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="12">
+        <f>SUMPRODUCT((E2:E14/D2:D14&gt;$H$2)*(C2:C14="МСК")*1)</f>
+        <v>1</v>
+      </c>
       <c r="L4" s="15" t="s">
         <v>40</v>
       </c>
@@ -57409,7 +57391,10 @@
       <c r="H5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12">
+        <f>SUMPRODUCT((E2:E14/D2:D14&gt;$H$2)*(C2:C14="МСК")*E2:E14)</f>
+        <v>66000</v>
+      </c>
       <c r="J5" s="18" t="s">
         <v>41</v>
       </c>

</xml_diff>